<commit_message>
Update SQL-Templates + Schema_Rights_Definition Excel
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EBF57C-386B-4CA5-BBE3-3629AF528448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE46E3E-A72B-4BAE-9B57-BB6F441368C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="111">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -377,9 +377,6 @@
     <t>42_cre_table_frontend_log.sql</t>
   </si>
   <si>
-    <t>(ähnlich template_cre_table.sql) Tabelle_id muss int und nicht primary key sein</t>
-  </si>
-  <si>
     <t>44_cre_table_frontend_in.sql</t>
   </si>
   <si>
@@ -398,9 +395,6 @@
     <t>52_cre_view_fe_out.sql</t>
   </si>
   <si>
-    <t>(neu ungetestet ) template_cre_view3.sql</t>
-  </si>
-  <si>
     <t>db2frontend_out</t>
   </si>
   <si>
@@ -534,6 +528,12 @@
   </si>
   <si>
     <t>./R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx[frontend_table_description]</t>
+  </si>
+  <si>
+    <t>INT_ID</t>
+  </si>
+  <si>
+    <t>template_cre_view3.sql</t>
   </si>
 </sst>
 </file>
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +964,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -981,10 +981,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1087,7 +1087,7 @@
     </row>
     <row r="23" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>9</v>
@@ -1102,7 +1102,7 @@
         <v>35</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>18</v>
@@ -1117,10 +1117,10 @@
         <v>33</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>12</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -1155,7 +1155,7 @@
         <v>21</v>
       </c>
       <c r="F24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H24" t="s">
         <v>1</v>
@@ -1189,7 +1189,7 @@
         <v>24</v>
       </c>
       <c r="F26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H26" t="s">
         <v>1</v>
@@ -1204,7 +1204,7 @@
         <v>7</v>
       </c>
       <c r="L26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M26" t="s">
         <v>14</v>
@@ -1238,7 +1238,7 @@
         <v>21</v>
       </c>
       <c r="F28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I28" t="s">
         <v>2</v>
@@ -1269,7 +1269,7 @@
         <v>24</v>
       </c>
       <c r="F30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I30" t="s">
         <v>2</v>
@@ -1281,7 +1281,7 @@
         <v>13</v>
       </c>
       <c r="L30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M30" t="s">
         <v>15</v>
@@ -1398,19 +1398,22 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B37" t="s">
         <v>57</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>58</v>
+      <c r="C37" t="s">
+        <v>44</v>
       </c>
       <c r="D37" t="s">
         <v>23</v>
       </c>
       <c r="E37" t="s">
         <v>24</v>
+      </c>
+      <c r="F37" t="s">
+        <v>109</v>
       </c>
       <c r="H37" t="s">
         <v>54</v>
@@ -1432,7 +1435,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C39" t="s">
         <v>44</v>
@@ -1480,16 +1483,19 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D42" t="s">
-        <v>61</v>
-      </c>
-      <c r="E42" t="s">
-        <v>60</v>
+      <c r="F42" t="s">
+        <v>109</v>
       </c>
       <c r="H42" t="s">
         <v>54</v>
@@ -1501,10 +1507,10 @@
         <v>42</v>
       </c>
       <c r="K42" t="s">
+        <v>61</v>
+      </c>
+      <c r="M42" t="s">
         <v>62</v>
-      </c>
-      <c r="M42" t="s">
-        <v>63</v>
       </c>
       <c r="N42" t="s">
         <v>24</v>
@@ -1528,16 +1534,16 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" t="s">
         <v>64</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" t="s">
-        <v>61</v>
-      </c>
-      <c r="E45" t="s">
-        <v>66</v>
       </c>
       <c r="G45" t="s">
         <v>6</v>
@@ -1546,7 +1552,7 @@
         <v>4</v>
       </c>
       <c r="J45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N45" t="s">
         <v>24</v>
@@ -1573,8 +1579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F89407-B4C6-4C58-A69A-9922A85B5EFC}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,7 +1594,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1604,39 +1610,39 @@
         <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1646,122 +1652,122 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change right for frontend_user and cds2db_user #348
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE46E3E-A72B-4BAE-9B57-BB6F441368C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
     <sheet name="table_description_convert_def" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="D23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="H23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="I33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="P33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="K38" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -148,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K39" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="K40" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -172,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K42" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="K43" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -201,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="111">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -539,7 +538,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -935,11 +934,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:C33"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,209 +1373,218 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="I36" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>49</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>50</v>
-      </c>
-      <c r="E36" t="s">
-        <v>24</v>
-      </c>
-      <c r="H36" t="s">
-        <v>1</v>
-      </c>
-      <c r="K36" t="s">
-        <v>50</v>
-      </c>
-      <c r="M36" t="s">
-        <v>51</v>
-      </c>
-      <c r="N36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>108</v>
-      </c>
-      <c r="B37" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" t="s">
-        <v>23</v>
       </c>
       <c r="E37" t="s">
         <v>24</v>
       </c>
-      <c r="F37" t="s">
+      <c r="H37" t="s">
+        <v>1</v>
+      </c>
+      <c r="K37" t="s">
+        <v>50</v>
+      </c>
+      <c r="M37" t="s">
+        <v>51</v>
+      </c>
+      <c r="N37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" t="s">
         <v>109</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H38" t="s">
         <v>54</v>
       </c>
-      <c r="I37" t="s">
-        <v>2</v>
-      </c>
-      <c r="J37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I38" t="s">
         <v>2</v>
       </c>
       <c r="J38" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>107</v>
-      </c>
-      <c r="C39" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" t="s">
-        <v>53</v>
-      </c>
-      <c r="H39" t="s">
-        <v>54</v>
-      </c>
       <c r="I39" t="s">
         <v>2</v>
       </c>
       <c r="J39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" t="s">
         <v>42</v>
       </c>
-      <c r="K39" t="s">
-        <v>55</v>
-      </c>
-      <c r="M39" t="s">
-        <v>56</v>
-      </c>
-      <c r="N39" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>53</v>
+      </c>
+      <c r="H40" t="s">
+        <v>54</v>
+      </c>
       <c r="I40" t="s">
         <v>2</v>
       </c>
       <c r="J40" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="K40" t="s">
+        <v>55</v>
+      </c>
+      <c r="M40" t="s">
+        <v>56</v>
+      </c>
+      <c r="N40" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
+        <v>2</v>
+      </c>
+      <c r="J41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
         <v>4</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J42" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>58</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>44</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>60</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E43" t="s">
         <v>59</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F43" t="s">
         <v>109</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H43" t="s">
         <v>54</v>
       </c>
-      <c r="I42" t="s">
-        <v>2</v>
-      </c>
-      <c r="J42" t="s">
-        <v>42</v>
-      </c>
-      <c r="K42" t="s">
-        <v>61</v>
-      </c>
-      <c r="M42" t="s">
-        <v>62</v>
-      </c>
-      <c r="N42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I43" t="s">
         <v>2</v>
       </c>
       <c r="J43" t="s">
-        <v>22</v>
+        <v>60</v>
+      </c>
+      <c r="K43" t="s">
+        <v>61</v>
+      </c>
+      <c r="M43" t="s">
+        <v>62</v>
+      </c>
+      <c r="N43" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D45" t="s">
-        <v>60</v>
-      </c>
-      <c r="E45" t="s">
-        <v>64</v>
-      </c>
-      <c r="G45" t="s">
-        <v>6</v>
-      </c>
       <c r="I45" t="s">
         <v>4</v>
       </c>
       <c r="J45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" t="s">
         <v>60</v>
       </c>
-      <c r="N45" t="s">
-        <v>24</v>
-      </c>
-      <c r="O45" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>64</v>
+      </c>
+      <c r="G46" t="s">
+        <v>6</v>
+      </c>
       <c r="I46" t="s">
         <v>4</v>
       </c>
       <c r="J46" t="s">
+        <v>60</v>
+      </c>
+      <c r="N46" t="s">
+        <v>24</v>
+      </c>
+      <c r="O46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>4</v>
+      </c>
+      <c r="J47" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F89407-B4C6-4C58-A69A-9922A85B5EFC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">

</xml_diff>

<commit_message>
Add data views for cds2db-modul with rights
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="112">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -533,13 +533,16 @@
   </si>
   <si>
     <t>template_cre_view3.sql</t>
+  </si>
+  <si>
+    <t>21_cre_view_typ_cds2db_all.sql</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,6 +598,12 @@
       <name val="Segoe UI"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -641,7 +650,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -652,6 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Erklärender Text" xfId="1" builtinId="53"/>
@@ -938,7 +948,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,10 +1331,10 @@
       <c r="G33" t="s">
         <v>6</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="I33" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J33" s="6" t="s">
+      <c r="J33" s="8" t="s">
         <v>20</v>
       </c>
       <c r="N33" t="s">
@@ -1336,10 +1346,10 @@
       <c r="P33" s="6"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J34" s="6" t="s">
+      <c r="J34" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1373,31 +1383,52 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I36" t="s">
-        <v>4</v>
-      </c>
-      <c r="J36" t="s">
-        <v>20</v>
+      <c r="B36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" t="s">
+        <v>50</v>
+      </c>
+      <c r="M36" t="s">
+        <v>51</v>
+      </c>
+      <c r="N36" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="G37" t="s">
+        <v>6</v>
       </c>
       <c r="H37" t="s">
-        <v>1</v>
-      </c>
-      <c r="K37" t="s">
-        <v>50</v>
-      </c>
-      <c r="M37" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="I37" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="N37" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Bring structures and functionalities for front-end tables up to date through current definitions and generated scripts
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -123,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K38" authorId="0" shapeId="0">
+    <comment ref="K44" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K40" authorId="0" shapeId="0">
+    <comment ref="K45" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -171,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K43" authorId="0" shapeId="0">
+    <comment ref="K50" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="113">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -536,6 +536,9 @@
   </si>
   <si>
     <t>21_cre_view_typ_cds2db_all.sql</t>
+  </si>
+  <si>
+    <t>43_cre_table_frontend_log.sql</t>
   </si>
 </sst>
 </file>
@@ -945,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,19 +1442,16 @@
         <v>108</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="C38" t="s">
         <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E38" t="s">
-        <v>24</v>
-      </c>
-      <c r="F38" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="H38" t="s">
         <v>54</v>
@@ -1460,7 +1460,7 @@
         <v>2</v>
       </c>
       <c r="J38" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -1472,138 +1472,213 @@
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="I40" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" t="s">
         <v>44</v>
       </c>
-      <c r="D40" t="s">
-        <v>42</v>
-      </c>
-      <c r="E40" t="s">
-        <v>53</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="D41" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" t="s">
+        <v>59</v>
+      </c>
+      <c r="F41" t="s">
+        <v>109</v>
+      </c>
+      <c r="H41" t="s">
         <v>54</v>
       </c>
-      <c r="I40" t="s">
-        <v>2</v>
-      </c>
-      <c r="J40" t="s">
-        <v>42</v>
-      </c>
-      <c r="K40" t="s">
-        <v>55</v>
-      </c>
-      <c r="M40" t="s">
-        <v>56</v>
-      </c>
-      <c r="N40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
         <v>2</v>
       </c>
       <c r="J41" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I42" t="s">
+        <v>2</v>
+      </c>
+      <c r="J42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
         <v>4</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J43" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" t="s">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" t="s">
         <v>44</v>
       </c>
-      <c r="D43" t="s">
-        <v>60</v>
-      </c>
-      <c r="E43" t="s">
-        <v>59</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="D44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" t="s">
         <v>109</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H44" t="s">
         <v>54</v>
       </c>
-      <c r="I43" t="s">
-        <v>2</v>
-      </c>
-      <c r="J43" t="s">
-        <v>60</v>
-      </c>
-      <c r="K43" t="s">
-        <v>61</v>
-      </c>
-      <c r="M43" t="s">
-        <v>62</v>
-      </c>
-      <c r="N43" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
         <v>2</v>
       </c>
       <c r="J44" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="K44" t="s">
+        <v>55</v>
+      </c>
+      <c r="L44" t="s">
+        <v>102</v>
+      </c>
+      <c r="M44" t="s">
+        <v>56</v>
+      </c>
+      <c r="N44" t="s">
+        <v>53</v>
+      </c>
+      <c r="O44" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" t="s">
+        <v>109</v>
+      </c>
+      <c r="H45" t="s">
+        <v>54</v>
+      </c>
       <c r="I45" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J45" t="s">
         <v>23</v>
       </c>
+      <c r="K45" t="s">
+        <v>61</v>
+      </c>
+      <c r="L45" t="s">
+        <v>102</v>
+      </c>
+      <c r="M45" t="s">
+        <v>62</v>
+      </c>
+      <c r="N45" t="s">
+        <v>59</v>
+      </c>
+      <c r="O45" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="I46" t="s">
+        <v>2</v>
+      </c>
+      <c r="J46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C47" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>60</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
         <v>64</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G47" t="s">
         <v>6</v>
       </c>
-      <c r="I46" t="s">
-        <v>4</v>
-      </c>
-      <c r="J46" t="s">
-        <v>60</v>
-      </c>
-      <c r="N46" t="s">
-        <v>24</v>
-      </c>
-      <c r="O46" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I47" t="s">
         <v>4</v>
       </c>
       <c r="J47" t="s">
+        <v>60</v>
+      </c>
+      <c r="N47" t="s">
+        <v>24</v>
+      </c>
+      <c r="O47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>4</v>
+      </c>
+      <c r="J48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" t="s">
+        <v>109</v>
+      </c>
+      <c r="H50" t="s">
+        <v>54</v>
+      </c>
+      <c r="I50" t="s">
+        <v>2</v>
+      </c>
+      <c r="J50" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
+        <v>2</v>
+      </c>
+      <c r="J51" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DB - New view of last raw data to optimize FHIR import
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -123,30 +123,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="K44" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Wie 30 und 31</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="K45" authorId="0" shapeId="0">
       <text>
         <r>
@@ -171,7 +147,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="K50" authorId="0" shapeId="0">
+    <comment ref="K46" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Wie 30 und 31</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="116">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -539,6 +539,15 @@
   </si>
   <si>
     <t>43_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t>22_cre_view_raw_cds2db_last.sql</t>
+  </si>
+  <si>
+    <t>_lraw</t>
+  </si>
+  <si>
+    <t>template_cre_view4.sql</t>
   </si>
 </sst>
 </file>
@@ -948,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,133 +1447,124 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" t="s">
+        <v>115</v>
+      </c>
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" t="s">
+        <v>114</v>
+      </c>
+      <c r="I38" t="s">
+        <v>4</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N38" t="s">
+        <v>24</v>
+      </c>
+      <c r="O38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>108</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>107</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>44</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>42</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>53</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H39" t="s">
         <v>54</v>
       </c>
-      <c r="I38" t="s">
-        <v>2</v>
-      </c>
-      <c r="J38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I39" t="s">
         <v>2</v>
       </c>
       <c r="J39" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I40" t="s">
+        <v>2</v>
+      </c>
+      <c r="J40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
         <v>4</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J41" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>58</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>44</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>60</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>59</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F42" t="s">
         <v>109</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H42" t="s">
         <v>54</v>
       </c>
-      <c r="I41" t="s">
-        <v>2</v>
-      </c>
-      <c r="J41" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I42" t="s">
         <v>2</v>
       </c>
       <c r="J42" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I43" t="s">
+        <v>2</v>
+      </c>
+      <c r="J43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
         <v>4</v>
-      </c>
-      <c r="J43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" t="s">
-        <v>44</v>
-      </c>
-      <c r="D44" t="s">
-        <v>23</v>
-      </c>
-      <c r="E44" t="s">
-        <v>24</v>
-      </c>
-      <c r="F44" t="s">
-        <v>109</v>
-      </c>
-      <c r="H44" t="s">
-        <v>54</v>
-      </c>
-      <c r="I44" t="s">
-        <v>2</v>
       </c>
       <c r="J44" t="s">
         <v>23</v>
       </c>
-      <c r="K44" t="s">
-        <v>55</v>
-      </c>
-      <c r="L44" t="s">
-        <v>102</v>
-      </c>
-      <c r="M44" t="s">
-        <v>56</v>
-      </c>
-      <c r="N44" t="s">
-        <v>53</v>
-      </c>
-      <c r="O44" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>112</v>
+        <v>57</v>
       </c>
       <c r="C45" t="s">
         <v>44</v>
@@ -1588,97 +1588,138 @@
         <v>23</v>
       </c>
       <c r="K45" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="L45" t="s">
         <v>102</v>
       </c>
       <c r="M45" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="N45" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="O45" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" t="s">
+        <v>109</v>
+      </c>
+      <c r="H46" t="s">
+        <v>54</v>
+      </c>
       <c r="I46" t="s">
         <v>2</v>
       </c>
       <c r="J46" t="s">
+        <v>23</v>
+      </c>
+      <c r="K46" t="s">
+        <v>61</v>
+      </c>
+      <c r="L46" t="s">
+        <v>102</v>
+      </c>
+      <c r="M46" t="s">
+        <v>62</v>
+      </c>
+      <c r="N46" t="s">
+        <v>59</v>
+      </c>
+      <c r="O46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>2</v>
+      </c>
+      <c r="J47" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>60</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>64</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G48" t="s">
         <v>6</v>
       </c>
-      <c r="I47" t="s">
-        <v>4</v>
-      </c>
-      <c r="J47" t="s">
-        <v>60</v>
-      </c>
-      <c r="N47" t="s">
-        <v>24</v>
-      </c>
-      <c r="O47" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I48" t="s">
         <v>4</v>
       </c>
       <c r="J48" t="s">
+        <v>60</v>
+      </c>
+      <c r="N48" t="s">
+        <v>24</v>
+      </c>
+      <c r="O48" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>4</v>
+      </c>
+      <c r="J49" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>57</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>44</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>23</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E51" t="s">
         <v>24</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F51" t="s">
         <v>109</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H51" t="s">
         <v>54</v>
       </c>
-      <c r="I50" t="s">
-        <v>2</v>
-      </c>
-      <c r="J50" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I51" t="s">
         <v>2</v>
       </c>
       <c r="J51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I52" t="s">
+        <v>2</v>
+      </c>
+      <c r="J52" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DB - Standardize the naming of views to represent data types and restrictions
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="116">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -346,9 +346,6 @@
     <t>19_cre_view_typ_dataproc_all.sql</t>
   </si>
   <si>
-    <t>_all</t>
-  </si>
-  <si>
     <t>20_take_over_check_date.sql</t>
   </si>
   <si>
@@ -544,10 +541,13 @@
     <t>22_cre_view_raw_cds2db_last.sql</t>
   </si>
   <si>
-    <t>_lraw</t>
-  </si>
-  <si>
     <t>template_cre_view4.sql</t>
+  </si>
+  <si>
+    <t>_raw_last</t>
+  </si>
+  <si>
+    <t>_raw_diff</t>
   </si>
 </sst>
 </file>
@@ -985,7 +985,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1002,10 +1002,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
     </row>
     <row r="23" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>9</v>
@@ -1123,7 +1123,7 @@
         <v>35</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>18</v>
@@ -1138,10 +1138,10 @@
         <v>33</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>12</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B24" t="s">
         <v>0</v>
@@ -1176,7 +1176,7 @@
         <v>21</v>
       </c>
       <c r="F24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H24" t="s">
         <v>1</v>
@@ -1210,7 +1210,7 @@
         <v>24</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H26" t="s">
         <v>1</v>
@@ -1225,7 +1225,7 @@
         <v>7</v>
       </c>
       <c r="L26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M26" t="s">
         <v>14</v>
@@ -1259,7 +1259,7 @@
         <v>21</v>
       </c>
       <c r="F28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I28" t="s">
         <v>2</v>
@@ -1290,7 +1290,7 @@
         <v>24</v>
       </c>
       <c r="F30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I30" t="s">
         <v>2</v>
@@ -1302,7 +1302,7 @@
         <v>13</v>
       </c>
       <c r="L30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M30" t="s">
         <v>15</v>
@@ -1343,6 +1343,9 @@
       <c r="G33" t="s">
         <v>6</v>
       </c>
+      <c r="H33" t="s">
+        <v>115</v>
+      </c>
       <c r="I33" s="8" t="s">
         <v>4</v>
       </c>
@@ -1381,9 +1384,6 @@
       <c r="G35" t="s">
         <v>6</v>
       </c>
-      <c r="H35" t="s">
-        <v>48</v>
-      </c>
       <c r="I35" t="s">
         <v>4</v>
       </c>
@@ -1396,10 +1396,10 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" t="s">
         <v>49</v>
-      </c>
-      <c r="C36" t="s">
-        <v>50</v>
       </c>
       <c r="E36" t="s">
         <v>24</v>
@@ -1408,10 +1408,10 @@
         <v>1</v>
       </c>
       <c r="K36" t="s">
+        <v>49</v>
+      </c>
+      <c r="M36" t="s">
         <v>50</v>
-      </c>
-      <c r="M36" t="s">
-        <v>51</v>
       </c>
       <c r="N36" t="s">
         <v>24</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C37" t="s">
         <v>46</v>
@@ -1433,9 +1433,6 @@
       <c r="G37" t="s">
         <v>6</v>
       </c>
-      <c r="H37" t="s">
-        <v>48</v>
-      </c>
       <c r="I37" t="s">
         <v>4</v>
       </c>
@@ -1448,10 +1445,10 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" t="s">
         <v>113</v>
-      </c>
-      <c r="C38" t="s">
-        <v>115</v>
       </c>
       <c r="D38" t="s">
         <v>20</v>
@@ -1480,10 +1477,10 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C39" t="s">
         <v>44</v>
@@ -1492,10 +1489,10 @@
         <v>42</v>
       </c>
       <c r="E39" t="s">
+        <v>52</v>
+      </c>
+      <c r="H39" t="s">
         <v>53</v>
-      </c>
-      <c r="H39" t="s">
-        <v>54</v>
       </c>
       <c r="I39" t="s">
         <v>2</v>
@@ -1522,28 +1519,28 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
         <v>44</v>
       </c>
       <c r="D42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I42" t="s">
         <v>2</v>
       </c>
       <c r="J42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -1564,7 +1561,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" t="s">
         <v>44</v>
@@ -1576,10 +1573,10 @@
         <v>24</v>
       </c>
       <c r="F45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I45" t="s">
         <v>2</v>
@@ -1588,24 +1585,24 @@
         <v>23</v>
       </c>
       <c r="K45" t="s">
+        <v>54</v>
+      </c>
+      <c r="L45" t="s">
+        <v>101</v>
+      </c>
+      <c r="M45" t="s">
         <v>55</v>
       </c>
-      <c r="L45" t="s">
-        <v>102</v>
-      </c>
-      <c r="M45" t="s">
-        <v>56</v>
-      </c>
       <c r="N45" t="s">
+        <v>52</v>
+      </c>
+      <c r="O45" t="s">
         <v>53</v>
-      </c>
-      <c r="O45" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C46" t="s">
         <v>44</v>
@@ -1617,10 +1614,10 @@
         <v>24</v>
       </c>
       <c r="F46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I46" t="s">
         <v>2</v>
@@ -1629,19 +1626,19 @@
         <v>23</v>
       </c>
       <c r="K46" t="s">
+        <v>60</v>
+      </c>
+      <c r="L46" t="s">
+        <v>101</v>
+      </c>
+      <c r="M46" t="s">
         <v>61</v>
       </c>
-      <c r="L46" t="s">
-        <v>102</v>
-      </c>
-      <c r="M46" t="s">
-        <v>62</v>
-      </c>
       <c r="N46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -1654,16 +1651,16 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" t="s">
+        <v>59</v>
+      </c>
+      <c r="E48" t="s">
         <v>63</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D48" t="s">
-        <v>60</v>
-      </c>
-      <c r="E48" t="s">
-        <v>64</v>
       </c>
       <c r="G48" t="s">
         <v>6</v>
@@ -1672,13 +1669,13 @@
         <v>4</v>
       </c>
       <c r="J48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N48" t="s">
         <v>24</v>
       </c>
       <c r="O48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
@@ -1691,7 +1688,7 @@
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
         <v>44</v>
@@ -1703,10 +1700,10 @@
         <v>24</v>
       </c>
       <c r="F51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I51" t="s">
         <v>2</v>
@@ -1749,7 +1746,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1762,42 +1759,42 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1807,122 +1804,122 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DB - Creating the views for data processor to access all and last study data (46_cre_view_fe_dataproc_last, 47_cre_view_fe_dataproc_all)
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="12420"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autor:</t>
         </r>
@@ -92,7 +92,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Bei diesen Views funktioniert die Rechtevergabe im gegensatz zu den diff und view3 Views noch statisch</t>
@@ -107,7 +107,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autor:</t>
         </r>
@@ -116,7 +116,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 12.7. haben wir in der view geändert - cds2db nicht mehr notwendig</t>
@@ -131,7 +131,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autor:</t>
         </r>
@@ -140,14 +140,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="K46" authorId="0" shapeId="0">
+    <comment ref="K47" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +155,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Autor:</t>
         </r>
@@ -164,31 +164,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Wie 30 und 31</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K51" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Wie 30 und 31</t>
@@ -200,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="122">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -557,13 +533,22 @@
   </si>
   <si>
     <t>get_last_processing_nr_typed</t>
+  </si>
+  <si>
+    <t>46_cre_view_fe_dataproc_last.sql</t>
+  </si>
+  <si>
+    <t>47_cre_view_fe_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t>_fe_last</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -605,19 +590,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -671,18 +643,20 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Erklärender Text" xfId="1" builtinId="53"/>
@@ -966,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,7 +1105,7 @@
       <c r="E23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="6" t="s">
         <v>64</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -1367,10 +1341,10 @@
       <c r="H33" t="s">
         <v>115</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J33" s="8" t="s">
+      <c r="J33" s="7" t="s">
         <v>20</v>
       </c>
       <c r="N33" t="s">
@@ -1379,13 +1353,13 @@
       <c r="O33" t="s">
         <v>1</v>
       </c>
-      <c r="P33" s="6"/>
+      <c r="P33" s="5"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I34" s="8" t="s">
+      <c r="I34" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J34" s="8" t="s">
+      <c r="J34" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1457,7 +1431,7 @@
       <c r="I37" t="s">
         <v>4</v>
       </c>
-      <c r="J37" s="8" t="s">
+      <c r="J37" s="7" t="s">
         <v>20</v>
       </c>
       <c r="N37" t="s">
@@ -1486,7 +1460,7 @@
       <c r="I38" t="s">
         <v>4</v>
       </c>
-      <c r="J38" s="8" t="s">
+      <c r="J38" s="7" t="s">
         <v>20</v>
       </c>
       <c r="N38" t="s">
@@ -1573,6 +1547,7 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C44" s="8"/>
       <c r="I44" t="s">
         <v>4</v>
       </c>
@@ -1584,7 +1559,7 @@
       <c r="B45" t="s">
         <v>56</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="9" t="s">
         <v>44</v>
       </c>
       <c r="D45" t="s">
@@ -1622,124 +1597,168 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="C46" s="9"/>
+      <c r="J46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>111</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>23</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
         <v>24</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F47" t="s">
         <v>108</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H47" t="s">
         <v>53</v>
       </c>
-      <c r="I46" t="s">
-        <v>2</v>
-      </c>
-      <c r="J46" t="s">
-        <v>23</v>
-      </c>
-      <c r="K46" t="s">
-        <v>60</v>
-      </c>
-      <c r="L46" t="s">
-        <v>101</v>
-      </c>
-      <c r="M46" t="s">
-        <v>61</v>
-      </c>
-      <c r="N46" t="s">
-        <v>58</v>
-      </c>
-      <c r="O46" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I47" t="s">
         <v>2</v>
       </c>
       <c r="J47" t="s">
+        <v>23</v>
+      </c>
+      <c r="K47" t="s">
+        <v>60</v>
+      </c>
+      <c r="L47" t="s">
+        <v>101</v>
+      </c>
+      <c r="M47" t="s">
+        <v>61</v>
+      </c>
+      <c r="N47" t="s">
+        <v>58</v>
+      </c>
+      <c r="O47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C48" s="9"/>
+      <c r="I48" t="s">
+        <v>2</v>
+      </c>
+      <c r="J48" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C49" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>59</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>63</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G49" t="s">
         <v>6</v>
       </c>
-      <c r="I48" t="s">
-        <v>4</v>
-      </c>
-      <c r="J48" t="s">
-        <v>59</v>
-      </c>
-      <c r="N48" t="s">
-        <v>24</v>
-      </c>
-      <c r="O48" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I49" t="s">
         <v>4</v>
       </c>
       <c r="J49" t="s">
+        <v>59</v>
+      </c>
+      <c r="N49" t="s">
+        <v>24</v>
+      </c>
+      <c r="O49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C50" s="9"/>
+      <c r="I50" t="s">
+        <v>4</v>
+      </c>
+      <c r="J50" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>56</v>
-      </c>
-      <c r="C51" t="s">
-        <v>44</v>
+        <v>119</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="D51" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E51" t="s">
+        <v>43</v>
+      </c>
+      <c r="G51" t="s">
+        <v>6</v>
+      </c>
+      <c r="H51" t="s">
+        <v>121</v>
+      </c>
+      <c r="I51" t="s">
+        <v>4</v>
+      </c>
+      <c r="J51" t="s">
+        <v>42</v>
+      </c>
+      <c r="N51" t="s">
         <v>24</v>
       </c>
-      <c r="F51" t="s">
-        <v>108</v>
-      </c>
-      <c r="H51" t="s">
+      <c r="O51" t="s">
         <v>53</v>
       </c>
-      <c r="I51" t="s">
-        <v>2</v>
-      </c>
-      <c r="J51" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>120</v>
+      </c>
+      <c r="C52" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" t="s">
+        <v>43</v>
+      </c>
+      <c r="G52" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" t="s">
+        <v>53</v>
+      </c>
       <c r="I52" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J52" t="s">
-        <v>22</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="N52" t="s">
+        <v>24</v>
+      </c>
+      <c r="O52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C53" s="9"/>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C54" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DB - Creating views for the data processor that only contain the latest data
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -123,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K45" authorId="0" shapeId="0">
+    <comment ref="K46" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K47" authorId="0" shapeId="0">
+    <comment ref="K48" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="124">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -542,6 +542,12 @@
   </si>
   <si>
     <t>_fe_last</t>
+  </si>
+  <si>
+    <t>19_cre_view_typ_dataproc_last.sql</t>
+  </si>
+  <si>
+    <t>_last</t>
   </si>
 </sst>
 </file>
@@ -940,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q54"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1391,22 +1397,28 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" t="s">
-        <v>49</v>
+        <v>122</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
       </c>
       <c r="E36" t="s">
-        <v>24</v>
+        <v>43</v>
+      </c>
+      <c r="G36" t="s">
+        <v>6</v>
       </c>
       <c r="H36" t="s">
-        <v>1</v>
-      </c>
-      <c r="K36" t="s">
-        <v>49</v>
-      </c>
-      <c r="M36" t="s">
-        <v>50</v>
+        <v>123</v>
+      </c>
+      <c r="I36" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36" t="s">
+        <v>42</v>
       </c>
       <c r="N36" t="s">
         <v>24</v>
@@ -1414,25 +1426,22 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="E37" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" t="s">
-        <v>6</v>
-      </c>
-      <c r="I37" t="s">
-        <v>4</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="H37" t="s">
+        <v>1</v>
+      </c>
+      <c r="K37" t="s">
+        <v>49</v>
+      </c>
+      <c r="M37" t="s">
+        <v>50</v>
       </c>
       <c r="N37" t="s">
         <v>24</v>
@@ -1440,10 +1449,10 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C38" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="D38" t="s">
         <v>20</v>
@@ -1454,9 +1463,6 @@
       <c r="G38" t="s">
         <v>6</v>
       </c>
-      <c r="H38" t="s">
-        <v>114</v>
-      </c>
       <c r="I38" t="s">
         <v>4</v>
       </c>
@@ -1466,268 +1472,265 @@
       <c r="N38" t="s">
         <v>24</v>
       </c>
-      <c r="O38" t="s">
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" t="s">
+        <v>114</v>
+      </c>
+      <c r="I39" t="s">
+        <v>4</v>
+      </c>
+      <c r="J39" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N39" t="s">
+        <v>24</v>
+      </c>
+      <c r="O39" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>107</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>106</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>44</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>42</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>52</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H40" t="s">
         <v>53</v>
       </c>
-      <c r="I39" t="s">
-        <v>2</v>
-      </c>
-      <c r="J39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I40" t="s">
         <v>2</v>
       </c>
       <c r="J40" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
+        <v>2</v>
+      </c>
+      <c r="J41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
         <v>4</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J42" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>57</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>44</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>59</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E43" t="s">
         <v>58</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F43" t="s">
         <v>108</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H43" t="s">
         <v>53</v>
       </c>
-      <c r="I42" t="s">
-        <v>2</v>
-      </c>
-      <c r="J42" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I43" t="s">
         <v>2</v>
       </c>
       <c r="J43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>2</v>
+      </c>
+      <c r="J44" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C44" s="8"/>
-      <c r="I44" t="s">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C45" s="8"/>
+      <c r="I45" t="s">
         <v>4</v>
-      </c>
-      <c r="J44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D45" t="s">
-        <v>23</v>
-      </c>
-      <c r="E45" t="s">
-        <v>24</v>
-      </c>
-      <c r="F45" t="s">
-        <v>108</v>
-      </c>
-      <c r="H45" t="s">
-        <v>53</v>
-      </c>
-      <c r="I45" t="s">
-        <v>2</v>
       </c>
       <c r="J45" t="s">
         <v>23</v>
       </c>
-      <c r="K45" t="s">
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" t="s">
+        <v>108</v>
+      </c>
+      <c r="H46" t="s">
+        <v>53</v>
+      </c>
+      <c r="I46" t="s">
+        <v>2</v>
+      </c>
+      <c r="J46" t="s">
+        <v>23</v>
+      </c>
+      <c r="K46" t="s">
         <v>54</v>
       </c>
-      <c r="L45" t="s">
+      <c r="L46" t="s">
         <v>101</v>
       </c>
-      <c r="M45" t="s">
+      <c r="M46" t="s">
         <v>55</v>
       </c>
-      <c r="N45" t="s">
+      <c r="N46" t="s">
         <v>52</v>
       </c>
-      <c r="O45" t="s">
+      <c r="O46" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C46" s="9"/>
-      <c r="J46" t="s">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C47" s="9"/>
+      <c r="J47" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C48" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>23</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>24</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F48" t="s">
         <v>108</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H48" t="s">
         <v>53</v>
       </c>
-      <c r="I47" t="s">
-        <v>2</v>
-      </c>
-      <c r="J47" t="s">
-        <v>23</v>
-      </c>
-      <c r="K47" t="s">
-        <v>60</v>
-      </c>
-      <c r="L47" t="s">
-        <v>101</v>
-      </c>
-      <c r="M47" t="s">
-        <v>61</v>
-      </c>
-      <c r="N47" t="s">
-        <v>58</v>
-      </c>
-      <c r="O47" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C48" s="9"/>
       <c r="I48" t="s">
         <v>2</v>
       </c>
       <c r="J48" t="s">
+        <v>23</v>
+      </c>
+      <c r="K48" t="s">
+        <v>60</v>
+      </c>
+      <c r="L48" t="s">
+        <v>101</v>
+      </c>
+      <c r="M48" t="s">
+        <v>61</v>
+      </c>
+      <c r="N48" t="s">
+        <v>58</v>
+      </c>
+      <c r="O48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C49" s="9"/>
+      <c r="I49" t="s">
+        <v>2</v>
+      </c>
+      <c r="J49" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C50" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>59</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>63</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G50" t="s">
         <v>6</v>
       </c>
-      <c r="I49" t="s">
-        <v>4</v>
-      </c>
-      <c r="J49" t="s">
-        <v>59</v>
-      </c>
-      <c r="N49" t="s">
-        <v>24</v>
-      </c>
-      <c r="O49" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C50" s="9"/>
       <c r="I50" t="s">
         <v>4</v>
       </c>
       <c r="J50" t="s">
-        <v>22</v>
+        <v>59</v>
+      </c>
+      <c r="N50" t="s">
+        <v>24</v>
+      </c>
+      <c r="O50" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D51" t="s">
-        <v>42</v>
-      </c>
-      <c r="E51" t="s">
-        <v>43</v>
-      </c>
-      <c r="G51" t="s">
-        <v>6</v>
-      </c>
-      <c r="H51" t="s">
-        <v>121</v>
-      </c>
+      <c r="C51" s="9"/>
       <c r="I51" t="s">
         <v>4</v>
       </c>
       <c r="J51" t="s">
-        <v>42</v>
-      </c>
-      <c r="N51" t="s">
-        <v>24</v>
-      </c>
-      <c r="O51" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>120</v>
-      </c>
-      <c r="C52" t="s">
-        <v>46</v>
+        <v>119</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="D52" t="s">
         <v>42</v>
@@ -1739,7 +1742,7 @@
         <v>6</v>
       </c>
       <c r="H52" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="I52" t="s">
         <v>4</v>
@@ -1755,10 +1758,42 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C53" s="9"/>
+      <c r="B53" t="s">
+        <v>120</v>
+      </c>
+      <c r="C53" t="s">
+        <v>46</v>
+      </c>
+      <c r="D53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" t="s">
+        <v>43</v>
+      </c>
+      <c r="G53" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" t="s">
+        <v>53</v>
+      </c>
+      <c r="I53" t="s">
+        <v>4</v>
+      </c>
+      <c r="J53" t="s">
+        <v>42</v>
+      </c>
+      <c r="N53" t="s">
+        <v>24</v>
+      </c>
+      <c r="O53" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C54" s="9"/>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C55" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DB - Creating views to display the latest version of the FHIR resources
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="12420"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21330" windowHeight="6345"/>
   </bookViews>
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
     <sheet name="table_description_convert_def" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -123,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K46" authorId="0" shapeId="0">
+    <comment ref="K50" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K48" authorId="0" shapeId="0">
+    <comment ref="K52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="131">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -548,6 +548,27 @@
   </si>
   <si>
     <t>_last</t>
+  </si>
+  <si>
+    <t>template_cre_view5.sql</t>
+  </si>
+  <si>
+    <t>_raw_last_version</t>
+  </si>
+  <si>
+    <t>_last_version</t>
+  </si>
+  <si>
+    <t>23_cre_view_typ_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t>23_cre_view_raw_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t>23_cre_view_typ_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t>23_cre_view_raw_dataproc_last_version.sql</t>
   </si>
 </sst>
 </file>
@@ -946,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q55"/>
+  <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,211 +1527,248 @@
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>107</v>
-      </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="C40" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="D40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40" t="s">
+        <v>126</v>
+      </c>
+      <c r="I40" t="s">
+        <v>4</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" t="s">
+        <v>124</v>
+      </c>
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" t="s">
+        <v>125</v>
+      </c>
+      <c r="I41" t="s">
+        <v>4</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N41" t="s">
+        <v>24</v>
+      </c>
+      <c r="O41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" t="s">
         <v>42</v>
       </c>
-      <c r="E40" t="s">
-        <v>52</v>
-      </c>
-      <c r="H40" t="s">
-        <v>53</v>
-      </c>
-      <c r="I40" t="s">
-        <v>2</v>
-      </c>
-      <c r="J40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I41" t="s">
-        <v>2</v>
-      </c>
-      <c r="J41" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>43</v>
+      </c>
+      <c r="G42" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" t="s">
+        <v>126</v>
+      </c>
       <c r="I42" t="s">
         <v>4</v>
       </c>
       <c r="J42" t="s">
-        <v>23</v>
+        <v>42</v>
+      </c>
+      <c r="N42" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>57</v>
+        <v>130</v>
       </c>
       <c r="C43" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" t="s">
+        <v>43</v>
+      </c>
+      <c r="G43" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" t="s">
+        <v>125</v>
+      </c>
+      <c r="I43" t="s">
+        <v>4</v>
+      </c>
+      <c r="J43" t="s">
+        <v>42</v>
+      </c>
+      <c r="N43" t="s">
+        <v>24</v>
+      </c>
+      <c r="O43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>107</v>
+      </c>
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" t="s">
         <v>44</v>
       </c>
-      <c r="D43" t="s">
-        <v>59</v>
-      </c>
-      <c r="E43" t="s">
-        <v>58</v>
-      </c>
-      <c r="F43" t="s">
-        <v>108</v>
-      </c>
-      <c r="H43" t="s">
+      <c r="D44" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" t="s">
+        <v>52</v>
+      </c>
+      <c r="H44" t="s">
         <v>53</v>
       </c>
-      <c r="I43" t="s">
-        <v>2</v>
-      </c>
-      <c r="J43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
         <v>2</v>
       </c>
       <c r="J44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>2</v>
+      </c>
+      <c r="J45" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C45" s="8"/>
-      <c r="I45" t="s">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
         <v>4</v>
-      </c>
-      <c r="J45" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D46" t="s">
-        <v>23</v>
-      </c>
-      <c r="E46" t="s">
-        <v>24</v>
-      </c>
-      <c r="F46" t="s">
-        <v>108</v>
-      </c>
-      <c r="H46" t="s">
-        <v>53</v>
-      </c>
-      <c r="I46" t="s">
-        <v>2</v>
       </c>
       <c r="J46" t="s">
         <v>23</v>
       </c>
-      <c r="K46" t="s">
-        <v>54</v>
-      </c>
-      <c r="L46" t="s">
-        <v>101</v>
-      </c>
-      <c r="M46" t="s">
-        <v>55</v>
-      </c>
-      <c r="N46" t="s">
-        <v>52</v>
-      </c>
-      <c r="O46" t="s">
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" t="s">
+        <v>59</v>
+      </c>
+      <c r="E47" t="s">
+        <v>58</v>
+      </c>
+      <c r="F47" t="s">
+        <v>108</v>
+      </c>
+      <c r="H47" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C47" s="9"/>
+      <c r="I47" t="s">
+        <v>2</v>
+      </c>
       <c r="J47" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>111</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" t="s">
-        <v>23</v>
-      </c>
-      <c r="E48" t="s">
-        <v>24</v>
-      </c>
-      <c r="F48" t="s">
-        <v>108</v>
-      </c>
-      <c r="H48" t="s">
-        <v>53</v>
-      </c>
       <c r="I48" t="s">
         <v>2</v>
       </c>
       <c r="J48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C49" s="8"/>
+      <c r="I49" t="s">
+        <v>4</v>
+      </c>
+      <c r="J49" t="s">
         <v>23</v>
-      </c>
-      <c r="K48" t="s">
-        <v>60</v>
-      </c>
-      <c r="L48" t="s">
-        <v>101</v>
-      </c>
-      <c r="M48" t="s">
-        <v>61</v>
-      </c>
-      <c r="N48" t="s">
-        <v>58</v>
-      </c>
-      <c r="O48" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C49" s="9"/>
-      <c r="I49" t="s">
-        <v>2</v>
-      </c>
-      <c r="J49" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>62</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>109</v>
+        <v>56</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="D50" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="E50" t="s">
-        <v>63</v>
-      </c>
-      <c r="G50" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="F50" t="s">
+        <v>108</v>
+      </c>
+      <c r="H50" t="s">
+        <v>53</v>
       </c>
       <c r="I50" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J50" t="s">
-        <v>59</v>
+        <v>23</v>
+      </c>
+      <c r="K50" t="s">
+        <v>54</v>
+      </c>
+      <c r="L50" t="s">
+        <v>101</v>
+      </c>
+      <c r="M50" t="s">
+        <v>55</v>
       </c>
       <c r="N50" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="O50" t="s">
         <v>53</v>
@@ -1718,82 +1776,167 @@
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C51" s="9"/>
-      <c r="I51" t="s">
-        <v>4</v>
-      </c>
       <c r="J51" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>119</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="D52" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E52" t="s">
-        <v>43</v>
-      </c>
-      <c r="G52" t="s">
-        <v>6</v>
+        <v>24</v>
+      </c>
+      <c r="F52" t="s">
+        <v>108</v>
       </c>
       <c r="H52" t="s">
-        <v>121</v>
+        <v>53</v>
       </c>
       <c r="I52" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J52" t="s">
-        <v>42</v>
+        <v>23</v>
+      </c>
+      <c r="K52" t="s">
+        <v>60</v>
+      </c>
+      <c r="L52" t="s">
+        <v>101</v>
+      </c>
+      <c r="M52" t="s">
+        <v>61</v>
       </c>
       <c r="N52" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="O52" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>120</v>
-      </c>
-      <c r="C53" t="s">
-        <v>46</v>
-      </c>
-      <c r="D53" t="s">
-        <v>42</v>
-      </c>
-      <c r="E53" t="s">
-        <v>43</v>
-      </c>
-      <c r="G53" t="s">
+      <c r="C53" s="9"/>
+      <c r="I53" t="s">
+        <v>2</v>
+      </c>
+      <c r="J53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" t="s">
+        <v>59</v>
+      </c>
+      <c r="E54" t="s">
+        <v>63</v>
+      </c>
+      <c r="G54" t="s">
         <v>6</v>
       </c>
-      <c r="H53" t="s">
+      <c r="I54" t="s">
+        <v>4</v>
+      </c>
+      <c r="J54" t="s">
+        <v>59</v>
+      </c>
+      <c r="N54" t="s">
+        <v>24</v>
+      </c>
+      <c r="O54" t="s">
         <v>53</v>
       </c>
-      <c r="I53" t="s">
-        <v>4</v>
-      </c>
-      <c r="J53" t="s">
-        <v>42</v>
-      </c>
-      <c r="N53" t="s">
-        <v>24</v>
-      </c>
-      <c r="O53" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C54" s="9"/>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C55" s="9"/>
+      <c r="I55" t="s">
+        <v>4</v>
+      </c>
+      <c r="J55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>119</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" t="s">
+        <v>42</v>
+      </c>
+      <c r="E56" t="s">
+        <v>43</v>
+      </c>
+      <c r="G56" t="s">
+        <v>6</v>
+      </c>
+      <c r="H56" t="s">
+        <v>121</v>
+      </c>
+      <c r="I56" t="s">
+        <v>4</v>
+      </c>
+      <c r="J56" t="s">
+        <v>42</v>
+      </c>
+      <c r="N56" t="s">
+        <v>24</v>
+      </c>
+      <c r="O56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>120</v>
+      </c>
+      <c r="C57" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" t="s">
+        <v>42</v>
+      </c>
+      <c r="E57" t="s">
+        <v>43</v>
+      </c>
+      <c r="G57" t="s">
+        <v>6</v>
+      </c>
+      <c r="H57" t="s">
+        <v>53</v>
+      </c>
+      <c r="I57" t="s">
+        <v>4</v>
+      </c>
+      <c r="J57" t="s">
+        <v>42</v>
+      </c>
+      <c r="N57" t="s">
+        <v>24</v>
+      </c>
+      <c r="O57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C58" s="9"/>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C59" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DB - Draft of the templates for the function for reloading historical data during FHIT import
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -123,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K50" authorId="0" shapeId="0">
+    <comment ref="K51" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K52" authorId="0" shapeId="0">
+    <comment ref="K53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="133">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -569,6 +569,12 @@
   </si>
   <si>
     <t>23_cre_view_raw_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t>25_adding_historical_raw_records.sql</t>
+  </si>
+  <si>
+    <t>template_adding_historical_records.sql</t>
   </si>
 </sst>
 </file>
@@ -967,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q59"/>
+  <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="G20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,263 +1655,260 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" t="s">
+        <v>125</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N44" t="s">
+        <v>21</v>
+      </c>
+      <c r="O44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>107</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>106</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>44</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>42</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>52</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H45" t="s">
         <v>53</v>
       </c>
-      <c r="I44" t="s">
-        <v>2</v>
-      </c>
-      <c r="J44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I45" t="s">
         <v>2</v>
       </c>
       <c r="J45" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I46" t="s">
+        <v>2</v>
+      </c>
+      <c r="J46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
         <v>4</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J47" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>57</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>44</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>59</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>58</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F48" t="s">
         <v>108</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H48" t="s">
         <v>53</v>
       </c>
-      <c r="I47" t="s">
-        <v>2</v>
-      </c>
-      <c r="J47" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I48" t="s">
         <v>2</v>
       </c>
       <c r="J48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>2</v>
+      </c>
+      <c r="J49" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C49" s="8"/>
-      <c r="I49" t="s">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C50" s="8"/>
+      <c r="I50" t="s">
         <v>4</v>
-      </c>
-      <c r="J49" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>56</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D50" t="s">
-        <v>23</v>
-      </c>
-      <c r="E50" t="s">
-        <v>24</v>
-      </c>
-      <c r="F50" t="s">
-        <v>108</v>
-      </c>
-      <c r="H50" t="s">
-        <v>53</v>
-      </c>
-      <c r="I50" t="s">
-        <v>2</v>
       </c>
       <c r="J50" t="s">
         <v>23</v>
       </c>
-      <c r="K50" t="s">
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D51" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" t="s">
+        <v>108</v>
+      </c>
+      <c r="H51" t="s">
+        <v>53</v>
+      </c>
+      <c r="I51" t="s">
+        <v>2</v>
+      </c>
+      <c r="J51" t="s">
+        <v>23</v>
+      </c>
+      <c r="K51" t="s">
         <v>54</v>
       </c>
-      <c r="L50" t="s">
+      <c r="L51" t="s">
         <v>101</v>
       </c>
-      <c r="M50" t="s">
+      <c r="M51" t="s">
         <v>55</v>
       </c>
-      <c r="N50" t="s">
+      <c r="N51" t="s">
         <v>52</v>
       </c>
-      <c r="O50" t="s">
+      <c r="O51" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C51" s="9"/>
-      <c r="J51" t="s">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C52" s="9"/>
+      <c r="J52" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>111</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C53" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>23</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E53" t="s">
         <v>24</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F53" t="s">
         <v>108</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H53" t="s">
         <v>53</v>
       </c>
-      <c r="I52" t="s">
-        <v>2</v>
-      </c>
-      <c r="J52" t="s">
-        <v>23</v>
-      </c>
-      <c r="K52" t="s">
-        <v>60</v>
-      </c>
-      <c r="L52" t="s">
-        <v>101</v>
-      </c>
-      <c r="M52" t="s">
-        <v>61</v>
-      </c>
-      <c r="N52" t="s">
-        <v>58</v>
-      </c>
-      <c r="O52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C53" s="9"/>
       <c r="I53" t="s">
         <v>2</v>
       </c>
       <c r="J53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K53" t="s">
+        <v>60</v>
+      </c>
+      <c r="L53" t="s">
+        <v>101</v>
+      </c>
+      <c r="M53" t="s">
+        <v>61</v>
+      </c>
+      <c r="N53" t="s">
+        <v>58</v>
+      </c>
+      <c r="O53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C54" s="9"/>
+      <c r="I54" t="s">
+        <v>2</v>
+      </c>
+      <c r="J54" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C55" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>59</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E55" t="s">
         <v>63</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G55" t="s">
         <v>6</v>
       </c>
-      <c r="I54" t="s">
-        <v>4</v>
-      </c>
-      <c r="J54" t="s">
-        <v>59</v>
-      </c>
-      <c r="N54" t="s">
-        <v>24</v>
-      </c>
-      <c r="O54" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C55" s="9"/>
       <c r="I55" t="s">
         <v>4</v>
       </c>
       <c r="J55" t="s">
-        <v>22</v>
+        <v>59</v>
+      </c>
+      <c r="N55" t="s">
+        <v>24</v>
+      </c>
+      <c r="O55" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>119</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D56" t="s">
-        <v>42</v>
-      </c>
-      <c r="E56" t="s">
-        <v>43</v>
-      </c>
-      <c r="G56" t="s">
-        <v>6</v>
-      </c>
-      <c r="H56" t="s">
-        <v>121</v>
-      </c>
+      <c r="C56" s="9"/>
       <c r="I56" t="s">
         <v>4</v>
       </c>
       <c r="J56" t="s">
-        <v>42</v>
-      </c>
-      <c r="N56" t="s">
-        <v>24</v>
-      </c>
-      <c r="O56" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>120</v>
-      </c>
-      <c r="C57" t="s">
-        <v>46</v>
+        <v>119</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="D57" t="s">
         <v>42</v>
@@ -1917,7 +1920,7 @@
         <v>6</v>
       </c>
       <c r="H57" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="I57" t="s">
         <v>4</v>
@@ -1933,10 +1936,42 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C58" s="9"/>
+      <c r="B58" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58" t="s">
+        <v>42</v>
+      </c>
+      <c r="E58" t="s">
+        <v>43</v>
+      </c>
+      <c r="G58" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" t="s">
+        <v>53</v>
+      </c>
+      <c r="I58" t="s">
+        <v>4</v>
+      </c>
+      <c r="J58" t="s">
+        <v>42</v>
+      </c>
+      <c r="N58" t="s">
+        <v>24</v>
+      </c>
+      <c r="O58" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C59" s="9"/>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C60" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DB - Distinction between raw and typed implemented due to different representation of the time
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="133">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -976,7 +976,7 @@
   <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1545,6 +1545,9 @@
       <c r="E40" t="s">
         <v>25</v>
       </c>
+      <c r="F40" t="s">
+        <v>66</v>
+      </c>
       <c r="G40" t="s">
         <v>6</v>
       </c>
@@ -1574,6 +1577,9 @@
       <c r="E41" t="s">
         <v>25</v>
       </c>
+      <c r="F41" t="s">
+        <v>65</v>
+      </c>
       <c r="G41" t="s">
         <v>6</v>
       </c>
@@ -1606,6 +1612,9 @@
       <c r="E42" t="s">
         <v>43</v>
       </c>
+      <c r="F42" t="s">
+        <v>66</v>
+      </c>
       <c r="G42" t="s">
         <v>6</v>
       </c>
@@ -1634,6 +1643,9 @@
       </c>
       <c r="E43" t="s">
         <v>43</v>
+      </c>
+      <c r="F43" t="s">
+        <v>65</v>
       </c>
       <c r="G43" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
DB - LAST FHIR VIEWs Unterscheiden zwischen raw and typed views als extra skript (unterschiedliche darstellung Datumsangabe)
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="134">
   <si>
     <t>10_cre_table_raw_cds2db_in.sql</t>
   </si>
@@ -575,6 +575,9 @@
   </si>
   <si>
     <t>template_adding_historical_records.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view6.sql</t>
   </si>
 </sst>
 </file>
@@ -976,7 +979,7 @@
   <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,7 +1572,7 @@
         <v>128</v>
       </c>
       <c r="C41" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D41" t="s">
         <v>20</v>
@@ -1636,7 +1639,7 @@
         <v>130</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D43" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
DB - Rename the init scripts to maintain proper naming in the future
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -178,30 +178,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="136">
   <si>
-    <t>10_cre_table_raw_cds2db_in.sql</t>
-  </si>
-  <si>
     <t>_raw</t>
   </si>
   <si>
     <t>INSERT, DELETE, UPDATE, SELECT</t>
   </si>
   <si>
-    <t>12_cre_table_raw_db_log.sql</t>
-  </si>
-  <si>
     <t>SELECT</t>
   </si>
   <si>
-    <t>18_cre_view_raw_type_diff_log.sql</t>
-  </si>
-  <si>
     <t>v_</t>
   </si>
   <si>
-    <t>30_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
     <t>SEQ_NAME</t>
   </si>
   <si>
@@ -217,21 +205,12 @@
     <t>COPY_FUNC_NAME</t>
   </si>
   <si>
-    <t>31_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
     <t>copy_raw_cds_in_to_db_log</t>
   </si>
   <si>
     <t>copy_type_cds_in_to_db_log</t>
   </si>
   <si>
-    <t>14_cre_table_typ_cds2db_in.sql</t>
-  </si>
-  <si>
-    <t>16_cre_table_typ_log.sql</t>
-  </si>
-  <si>
     <t>TABLE_PREFIX</t>
   </si>
   <si>
@@ -319,12 +298,6 @@
     <t>template_cre_view2.sql</t>
   </si>
   <si>
-    <t>19_cre_view_typ_dataproc_all.sql</t>
-  </si>
-  <si>
-    <t>20_take_over_check_date.sql</t>
-  </si>
-  <si>
     <t>template_take_over_check_date_function.sql</t>
   </si>
   <si>
@@ -340,33 +313,18 @@
     <t>_fe</t>
   </si>
   <si>
-    <t>60_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
     <t>copy_fe_dp_in_to_db_log</t>
   </si>
   <si>
-    <t>42_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t>44_cre_table_frontend_in.sql</t>
-  </si>
-  <si>
     <t>db2frontend_in</t>
   </si>
   <si>
     <t>db2frontend_user</t>
   </si>
   <si>
-    <t>62_fe_in_to_db_log.sql</t>
-  </si>
-  <si>
     <t>copy_fe_fe_in_to_db_log</t>
   </si>
   <si>
-    <t>52_cre_view_fe_out.sql</t>
-  </si>
-  <si>
     <t>db2frontend_out</t>
   </si>
   <si>
@@ -496,9 +454,6 @@
     <t>Pfad zur Excel-Datei gefolgt vom Namen des Tabellenblattes in eckigen Klammern mit den Tabellenbeschreibungen</t>
   </si>
   <si>
-    <t>40_cre_table_typ_dataproc_in.sql</t>
-  </si>
-  <si>
     <t>./R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx[frontend_table_description]</t>
   </si>
   <si>
@@ -508,15 +463,6 @@
     <t>template_cre_view3.sql</t>
   </si>
   <si>
-    <t>21_cre_view_typ_cds2db_all.sql</t>
-  </si>
-  <si>
-    <t>43_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t>22_cre_view_raw_cds2db_last.sql</t>
-  </si>
-  <si>
     <t>template_cre_view4.sql</t>
   </si>
   <si>
@@ -526,27 +472,15 @@
     <t>_raw_diff</t>
   </si>
   <si>
-    <t>15_get_last_processing_nr_typed.sql</t>
-  </si>
-  <si>
     <t>template_get_last_pnr_typed.sql</t>
   </si>
   <si>
     <t>get_last_processing_nr_typed</t>
   </si>
   <si>
-    <t>46_cre_view_fe_dataproc_last.sql</t>
-  </si>
-  <si>
-    <t>47_cre_view_fe_dataproc_all.sql</t>
-  </si>
-  <si>
     <t>_fe_last</t>
   </si>
   <si>
-    <t>19_cre_view_typ_dataproc_last.sql</t>
-  </si>
-  <si>
     <t>_last</t>
   </si>
   <si>
@@ -559,31 +493,97 @@
     <t>_last_version</t>
   </si>
   <si>
-    <t>23_cre_view_typ_cds2db_last_version.sql</t>
-  </si>
-  <si>
-    <t>23_cre_view_raw_cds2db_last_version.sql</t>
-  </si>
-  <si>
-    <t>23_cre_view_typ_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t>23_cre_view_raw_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t>25_adding_historical_raw_records.sql</t>
-  </si>
-  <si>
     <t>template_adding_historical_records.sql</t>
   </si>
   <si>
     <t>template_cre_view6.sql</t>
   </si>
   <si>
-    <t>45_cre_table_frontend_in_trig.sql</t>
-  </si>
-  <si>
     <t>template_cre_trigger_set_id.sql</t>
+  </si>
+  <si>
+    <t>100_cre_table_raw_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t>120_cre_table_raw_db_log.sql</t>
+  </si>
+  <si>
+    <t>140_cre_table_typ_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t>160_cre_table_typ_log.sql</t>
+  </si>
+  <si>
+    <t>180_cre_view_raw_type_diff_log.sql</t>
+  </si>
+  <si>
+    <t>190_cre_view_typ_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t>190_cre_view_typ_dataproc_last.sql</t>
+  </si>
+  <si>
+    <t>200_take_over_check_date.sql</t>
+  </si>
+  <si>
+    <t>210_cre_view_typ_cds2db_all.sql</t>
+  </si>
+  <si>
+    <t>220_cre_view_raw_cds2db_last.sql</t>
+  </si>
+  <si>
+    <t>230_cre_view_typ_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t>230_cre_view_raw_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t>230_cre_view_typ_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t>230_cre_view_raw_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t>250_adding_historical_raw_records.sql</t>
+  </si>
+  <si>
+    <t>400_cre_table_typ_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t>440_cre_table_frontend_in.sql</t>
+  </si>
+  <si>
+    <t>420_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t>430_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t>520_cre_view_fe_out.sql</t>
+  </si>
+  <si>
+    <t>450_cre_table_frontend_in_trig.sql</t>
+  </si>
+  <si>
+    <t>460_cre_view_fe_dataproc_last.sql</t>
+  </si>
+  <si>
+    <t>470_cre_view_fe_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t>300_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>150_get_last_processing_nr_typed.sql</t>
+  </si>
+  <si>
+    <t>310_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>600_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>620_fe_in_to_db_log.sql</t>
   </si>
 </sst>
 </file>
@@ -984,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,15 +1010,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1027,99 +1027,99 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B18" s="2"/>
     </row>
@@ -1128,881 +1128,881 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q23" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" t="s">
         <v>0</v>
       </c>
-      <c r="C24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>1</v>
       </c>
-      <c r="I24" t="s">
-        <v>2</v>
-      </c>
       <c r="J24" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F26" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="H26" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
         <v>1</v>
       </c>
-      <c r="I26" t="s">
-        <v>2</v>
-      </c>
       <c r="J26" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K26" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="L26" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="M26" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26" t="s">
         <v>14</v>
       </c>
-      <c r="N26" t="s">
-        <v>21</v>
-      </c>
       <c r="O26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="I28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="K28" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="L28" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="M28" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="N28" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
         <v>17</v>
       </c>
-      <c r="C30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" t="s">
-        <v>24</v>
-      </c>
       <c r="F30" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="I30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K30" t="s">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="L30" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="M30" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N30" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I32" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J32" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E33" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G33" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H33" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="N33" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="O33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P33" s="5"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I34" s="7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D35" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E35" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G35" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I35" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J35" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N35" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D36" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G36" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="I36" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J36" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N36" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E37" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="M37" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="N37" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D38" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G38" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="N38" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="D39" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E39" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G39" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H39" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="I39" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="N39" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="O39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E40" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F40" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="G40" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H40" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="I40" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="N40" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C41" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E41" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F41" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="G41" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H41" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="I41" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="N41" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="O41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C42" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="D42" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E42" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F42" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="G42" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H42" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="I42" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J42" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N42" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E43" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F43" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="G43" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H43" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="I43" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J43" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N43" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="O43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C44" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="D44" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E44" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G44" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H44" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="N44" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="O44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="C45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" t="s">
+        <v>43</v>
+      </c>
+      <c r="H45" t="s">
         <v>44</v>
       </c>
-      <c r="D45" t="s">
-        <v>42</v>
-      </c>
-      <c r="E45" t="s">
-        <v>52</v>
-      </c>
-      <c r="H45" t="s">
-        <v>53</v>
-      </c>
       <c r="I45" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I46" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I47" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J47" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="C48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" t="s">
+        <v>46</v>
+      </c>
+      <c r="F48" t="s">
+        <v>93</v>
+      </c>
+      <c r="H48" t="s">
         <v>44</v>
       </c>
-      <c r="D48" t="s">
-        <v>59</v>
-      </c>
-      <c r="E48" t="s">
-        <v>58</v>
-      </c>
-      <c r="F48" t="s">
-        <v>108</v>
-      </c>
-      <c r="H48" t="s">
-        <v>53</v>
-      </c>
       <c r="I48" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I49" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C50" s="8"/>
       <c r="I50" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J50" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="C51" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" t="s">
+        <v>93</v>
+      </c>
+      <c r="H51" t="s">
         <v>44</v>
       </c>
-      <c r="D51" t="s">
-        <v>23</v>
-      </c>
-      <c r="E51" t="s">
-        <v>24</v>
-      </c>
-      <c r="F51" t="s">
-        <v>108</v>
-      </c>
-      <c r="H51" t="s">
-        <v>53</v>
-      </c>
       <c r="I51" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K51" t="s">
-        <v>54</v>
+        <v>134</v>
       </c>
       <c r="L51" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="M51" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="N51" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="O51" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C52" s="9"/>
       <c r="J52" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="C53" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" t="s">
+        <v>17</v>
+      </c>
+      <c r="F53" t="s">
+        <v>93</v>
+      </c>
+      <c r="H53" t="s">
         <v>44</v>
       </c>
-      <c r="D53" t="s">
-        <v>23</v>
-      </c>
-      <c r="E53" t="s">
-        <v>24</v>
-      </c>
-      <c r="F53" t="s">
-        <v>108</v>
-      </c>
-      <c r="H53" t="s">
-        <v>53</v>
-      </c>
       <c r="I53" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K53" t="s">
-        <v>60</v>
+        <v>135</v>
       </c>
       <c r="L53" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="M53" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="N53" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="O53" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C54" s="9"/>
       <c r="I54" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D55" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E55" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="G55" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I55" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J55" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="N55" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="O55" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C56" s="9"/>
       <c r="I56" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J56" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="D57" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E57" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="H57" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D58" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E58" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G58" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H58" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="I58" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J58" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N58" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="O58" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="C59" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D59" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E59" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G59" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H59" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="I59" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J59" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N59" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="O59" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
@@ -2037,180 +2037,180 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DB - rename views to _last_import
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -10,7 +10,7 @@
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
     <sheet name="table_description_convert_def" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -481,9 +481,6 @@
     <t>_fe_last</t>
   </si>
   <si>
-    <t>_last</t>
-  </si>
-  <si>
     <t>template_cre_view5.sql</t>
   </si>
   <si>
@@ -584,6 +581,9 @@
   </si>
   <si>
     <t>620_fe_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>_last_import</t>
   </si>
 </sst>
 </file>
@@ -985,7 +985,7 @@
   <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1189,7 @@
         <v>90</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s">
         <v>37</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
@@ -1247,7 +1247,7 @@
         <v>16</v>
       </c>
       <c r="K26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L26" t="s">
         <v>87</v>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
         <v>37</v>
@@ -1293,7 +1293,7 @@
         <v>13</v>
       </c>
       <c r="K28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L28" t="s">
         <v>98</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
         <v>37</v>
@@ -1336,7 +1336,7 @@
         <v>16</v>
       </c>
       <c r="K30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L30" t="s">
         <v>87</v>
@@ -1366,7 +1366,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33" t="s">
         <v>38</v>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
         <v>39</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>94</v>
@@ -1448,7 +1448,7 @@
         <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="I36" t="s">
         <v>2</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C37" t="s">
         <v>40</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C38" t="s">
         <v>39</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C39" t="s">
         <v>95</v>
@@ -1543,10 +1543,10 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
@@ -1561,7 +1561,7 @@
         <v>3</v>
       </c>
       <c r="H40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I40" t="s">
         <v>2</v>
@@ -1575,10 +1575,10 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D41" t="s">
         <v>13</v>
@@ -1593,7 +1593,7 @@
         <v>3</v>
       </c>
       <c r="H41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I41" t="s">
         <v>2</v>
@@ -1610,10 +1610,10 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D42" t="s">
         <v>35</v>
@@ -1628,7 +1628,7 @@
         <v>3</v>
       </c>
       <c r="H42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I42" t="s">
         <v>2</v>
@@ -1642,10 +1642,10 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D43" t="s">
         <v>35</v>
@@ -1660,7 +1660,7 @@
         <v>3</v>
       </c>
       <c r="H43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I43" t="s">
         <v>2</v>
@@ -1677,10 +1677,10 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D44" t="s">
         <v>13</v>
@@ -1692,7 +1692,7 @@
         <v>3</v>
       </c>
       <c r="H44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J44" s="7" t="s">
         <v>13</v>
@@ -1709,7 +1709,7 @@
         <v>92</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C45" t="s">
         <v>37</v>
@@ -1748,7 +1748,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C48" t="s">
         <v>37</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>37</v>
@@ -1815,7 +1815,7 @@
         <v>16</v>
       </c>
       <c r="K51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L51" t="s">
         <v>87</v>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>37</v>
@@ -1862,7 +1862,7 @@
         <v>16</v>
       </c>
       <c r="K53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L53" t="s">
         <v>87</v>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C55" s="10" t="s">
         <v>94</v>
@@ -1926,10 +1926,10 @@
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D57" t="s">
         <v>47</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>94</v>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C59" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
DB - Transferring the metadata even if nothing has changed in the actual FHIR data (raw) Refs #667
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -517,9 +517,6 @@
     <t>190_cre_view_typ_dataproc_all.sql</t>
   </si>
   <si>
-    <t>190_cre_view_typ_dataproc_last.sql</t>
-  </si>
-  <si>
     <t>200_take_over_check_date.sql</t>
   </si>
   <si>
@@ -584,6 +581,9 @@
   </si>
   <si>
     <t>_last_import</t>
+  </si>
+  <si>
+    <t>190_cre_view_typ_dataproc_last_import.sql</t>
   </si>
 </sst>
 </file>
@@ -985,7 +985,7 @@
   <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1247,7 @@
         <v>16</v>
       </c>
       <c r="K26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L26" t="s">
         <v>87</v>
@@ -1293,7 +1293,7 @@
         <v>13</v>
       </c>
       <c r="K28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L28" t="s">
         <v>98</v>
@@ -1336,7 +1336,7 @@
         <v>16</v>
       </c>
       <c r="K30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L30" t="s">
         <v>87</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>94</v>
@@ -1448,7 +1448,7 @@
         <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I36" t="s">
         <v>2</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C37" t="s">
         <v>40</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C38" t="s">
         <v>39</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C39" t="s">
         <v>95</v>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C40" t="s">
         <v>101</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C41" t="s">
         <v>105</v>
@@ -1610,7 +1610,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C42" t="s">
         <v>101</v>
@@ -1642,7 +1642,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C43" t="s">
         <v>105</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C44" t="s">
         <v>104</v>
@@ -1709,7 +1709,7 @@
         <v>92</v>
       </c>
       <c r="B45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C45" t="s">
         <v>37</v>
@@ -1748,7 +1748,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C48" t="s">
         <v>37</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>37</v>
@@ -1815,7 +1815,7 @@
         <v>16</v>
       </c>
       <c r="K51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L51" t="s">
         <v>87</v>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>37</v>
@@ -1862,7 +1862,7 @@
         <v>16</v>
       </c>
       <c r="K53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L53" t="s">
         <v>87</v>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C55" s="10" t="s">
         <v>94</v>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>106</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>94</v>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C59" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
DB - Restructuring the SQL templates for the views - renaming the templates
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="134">
   <si>
     <t>_raw</t>
   </si>
@@ -292,12 +292,6 @@
     <t>template_cre_table.sql</t>
   </si>
   <si>
-    <t>template_cre_view.sql</t>
-  </si>
-  <si>
-    <t>template_cre_view2.sql</t>
-  </si>
-  <si>
     <t>template_take_over_check_date_function.sql</t>
   </si>
   <si>
@@ -460,15 +454,6 @@
     <t>INT_ID</t>
   </si>
   <si>
-    <t>template_cre_view3.sql</t>
-  </si>
-  <si>
-    <t>template_cre_view4.sql</t>
-  </si>
-  <si>
-    <t>_raw_last</t>
-  </si>
-  <si>
     <t>_raw_diff</t>
   </si>
   <si>
@@ -481,9 +466,6 @@
     <t>_fe_last</t>
   </si>
   <si>
-    <t>template_cre_view5.sql</t>
-  </si>
-  <si>
     <t>_raw_last_version</t>
   </si>
   <si>
@@ -493,9 +475,6 @@
     <t>template_adding_historical_records.sql</t>
   </si>
   <si>
-    <t>template_cre_view6.sql</t>
-  </si>
-  <si>
     <t>template_cre_trigger_set_id.sql</t>
   </si>
   <si>
@@ -523,9 +502,6 @@
     <t>210_cre_view_typ_cds2db_all.sql</t>
   </si>
   <si>
-    <t>220_cre_view_raw_cds2db_last.sql</t>
-  </si>
-  <si>
     <t>230_cre_view_typ_cds2db_last_version.sql</t>
   </si>
   <si>
@@ -584,6 +560,24 @@
   </si>
   <si>
     <t>190_cre_view_typ_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t>220_cre_view_raw_cds2db_last_import.sql</t>
+  </si>
+  <si>
+    <t>_raw_last_import</t>
+  </si>
+  <si>
+    <t>template_cre_view_diff.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_all.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_last_import.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_last_version.sql</t>
   </si>
 </sst>
 </file>
@@ -685,7 +679,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -699,6 +693,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Erklärender Text" xfId="1" builtinId="53"/>
@@ -984,19 +979,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="B38" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B61" sqref="B52:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="41" customWidth="1"/>
     <col min="3" max="3" width="43.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
-    <col min="7" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
     <col min="9" max="9" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40.5703125" customWidth="1"/>
@@ -1010,7 +1006,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1027,10 +1023,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1133,7 +1129,7 @@
     </row>
     <row r="23" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>5</v>
@@ -1148,7 +1144,7 @@
         <v>28</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>11</v>
@@ -1163,10 +1159,10 @@
         <v>26</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>8</v>
@@ -1186,10 +1182,10 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
         <v>37</v>
@@ -1201,7 +1197,7 @@
         <v>14</v>
       </c>
       <c r="F24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H24" t="s">
         <v>0</v>
@@ -1223,7 +1219,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
@@ -1235,7 +1231,7 @@
         <v>17</v>
       </c>
       <c r="F26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H26" t="s">
         <v>0</v>
@@ -1247,10 +1243,10 @@
         <v>16</v>
       </c>
       <c r="K26" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="L26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M26" t="s">
         <v>9</v>
@@ -1272,7 +1268,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s">
         <v>37</v>
@@ -1284,7 +1280,7 @@
         <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I28" t="s">
         <v>1</v>
@@ -1293,13 +1289,13 @@
         <v>13</v>
       </c>
       <c r="K28" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="L28" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="M28" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="N28" t="s">
         <v>17</v>
@@ -1314,8 +1310,8 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>110</v>
+      <c r="B30" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="C30" t="s">
         <v>37</v>
@@ -1327,7 +1323,7 @@
         <v>17</v>
       </c>
       <c r="F30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I30" t="s">
         <v>1</v>
@@ -1336,10 +1332,10 @@
         <v>16</v>
       </c>
       <c r="K30" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="L30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M30" t="s">
         <v>10</v>
@@ -1349,6 +1345,7 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B31" s="11"/>
       <c r="I31" t="s">
         <v>1</v>
       </c>
@@ -1357,6 +1354,7 @@
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="11"/>
       <c r="I32" t="s">
         <v>2</v>
       </c>
@@ -1365,11 +1363,11 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>111</v>
+      <c r="B33" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
       <c r="D33" t="s">
         <v>13</v>
@@ -1381,7 +1379,7 @@
         <v>3</v>
       </c>
       <c r="H33" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I33" s="7" t="s">
         <v>2</v>
@@ -1398,6 +1396,7 @@
       <c r="P33" s="5"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="11"/>
       <c r="I34" s="7" t="s">
         <v>2</v>
       </c>
@@ -1406,11 +1405,11 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>112</v>
+      <c r="B35" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="D35" t="s">
         <v>35</v>
@@ -1432,11 +1431,11 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>135</v>
+      <c r="B36" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="D36" t="s">
         <v>35</v>
@@ -1448,7 +1447,7 @@
         <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="I36" t="s">
         <v>2</v>
@@ -1461,11 +1460,11 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>113</v>
+      <c r="B37" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E37" t="s">
         <v>17</v>
@@ -1474,21 +1473,21 @@
         <v>0</v>
       </c>
       <c r="K37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N37" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>114</v>
+      <c r="B38" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="D38" t="s">
         <v>13</v>
@@ -1510,11 +1509,11 @@
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>115</v>
-      </c>
-      <c r="C39" t="s">
-        <v>95</v>
+      <c r="B39" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>132</v>
       </c>
       <c r="D39" t="s">
         <v>13</v>
@@ -1526,7 +1525,7 @@
         <v>3</v>
       </c>
       <c r="H39" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
       <c r="I39" t="s">
         <v>2</v>
@@ -1542,11 +1541,11 @@
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>116</v>
+      <c r="B40" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C40" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
@@ -1555,13 +1554,13 @@
         <v>18</v>
       </c>
       <c r="F40" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G40" t="s">
         <v>3</v>
       </c>
       <c r="H40" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I40" t="s">
         <v>2</v>
@@ -1574,11 +1573,11 @@
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>117</v>
+      <c r="B41" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="D41" t="s">
         <v>13</v>
@@ -1587,13 +1586,13 @@
         <v>18</v>
       </c>
       <c r="F41" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G41" t="s">
         <v>3</v>
       </c>
       <c r="H41" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="I41" t="s">
         <v>2</v>
@@ -1609,11 +1608,11 @@
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>118</v>
+      <c r="B42" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="D42" t="s">
         <v>35</v>
@@ -1622,13 +1621,13 @@
         <v>36</v>
       </c>
       <c r="F42" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G42" t="s">
         <v>3</v>
       </c>
       <c r="H42" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I42" t="s">
         <v>2</v>
@@ -1641,11 +1640,11 @@
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>119</v>
+      <c r="B43" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="D43" t="s">
         <v>35</v>
@@ -1654,13 +1653,13 @@
         <v>36</v>
       </c>
       <c r="F43" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G43" t="s">
         <v>3</v>
       </c>
       <c r="H43" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="I43" t="s">
         <v>2</v>
@@ -1676,11 +1675,11 @@
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>120</v>
+      <c r="B44" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D44" t="s">
         <v>13</v>
@@ -1692,7 +1691,7 @@
         <v>3</v>
       </c>
       <c r="H44" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="J44" s="7" t="s">
         <v>13</v>
@@ -1706,10 +1705,10 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B45" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C45" t="s">
         <v>37</v>
@@ -1718,10 +1717,10 @@
         <v>35</v>
       </c>
       <c r="E45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H45" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I45" t="s">
         <v>1</v>
@@ -1748,28 +1747,28 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C48" t="s">
         <v>37</v>
       </c>
       <c r="D48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E48" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F48" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H48" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I48" t="s">
         <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
@@ -1791,7 +1790,7 @@
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>37</v>
@@ -1803,10 +1802,10 @@
         <v>17</v>
       </c>
       <c r="F51" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I51" t="s">
         <v>1</v>
@@ -1815,30 +1814,31 @@
         <v>16</v>
       </c>
       <c r="K51" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="L51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M51" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N51" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" s="11"/>
       <c r="C52" s="9"/>
       <c r="J52" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>124</v>
+      <c r="B53" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>37</v>
@@ -1850,10 +1850,10 @@
         <v>17</v>
       </c>
       <c r="F53" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H53" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I53" t="s">
         <v>1</v>
@@ -1862,22 +1862,23 @@
         <v>16</v>
       </c>
       <c r="K53" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="L53" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M53" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N53" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O53" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" s="11"/>
       <c r="C54" s="9"/>
       <c r="I54" t="s">
         <v>1</v>
@@ -1887,17 +1888,17 @@
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>125</v>
+      <c r="B55" s="11" t="s">
+        <v>117</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="D55" t="s">
+        <v>45</v>
+      </c>
+      <c r="E55" t="s">
         <v>47</v>
-      </c>
-      <c r="E55" t="s">
-        <v>49</v>
       </c>
       <c r="G55" t="s">
         <v>3</v>
@@ -1906,16 +1907,17 @@
         <v>2</v>
       </c>
       <c r="J55" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N55" t="s">
         <v>17</v>
       </c>
       <c r="O55" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56" s="11"/>
       <c r="C56" s="9"/>
       <c r="I56" t="s">
         <v>2</v>
@@ -1925,28 +1927,28 @@
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>126</v>
+      <c r="B57" s="11" t="s">
+        <v>118</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D57" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E57" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H57" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>127</v>
+      <c r="B58" s="11" t="s">
+        <v>119</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="D58" t="s">
         <v>35</v>
@@ -1958,7 +1960,7 @@
         <v>3</v>
       </c>
       <c r="H58" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I58" t="s">
         <v>2</v>
@@ -1970,15 +1972,15 @@
         <v>17</v>
       </c>
       <c r="O58" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>128</v>
+      <c r="B59" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="D59" t="s">
         <v>35</v>
@@ -1990,7 +1992,7 @@
         <v>3</v>
       </c>
       <c r="H59" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I59" t="s">
         <v>2</v>
@@ -2002,13 +2004,15 @@
         <v>17</v>
       </c>
       <c r="O59" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B60" s="11"/>
       <c r="C60" s="9"/>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61" s="11"/>
       <c r="C61" s="9"/>
     </row>
   </sheetData>
@@ -2037,7 +2041,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2050,42 +2054,42 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2095,122 +2099,122 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DB - renaming the fe last import view to match the general naming scheme
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -10,7 +10,7 @@
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
     <sheet name="table_description_convert_def" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -463,9 +463,6 @@
     <t>get_last_processing_nr_typed</t>
   </si>
   <si>
-    <t>_fe_last</t>
-  </si>
-  <si>
     <t>_raw_last_version</t>
   </si>
   <si>
@@ -535,9 +532,6 @@
     <t>450_cre_table_frontend_in_trig.sql</t>
   </si>
   <si>
-    <t>460_cre_view_fe_dataproc_last.sql</t>
-  </si>
-  <si>
     <t>470_cre_view_fe_dataproc_all.sql</t>
   </si>
   <si>
@@ -578,6 +572,12 @@
   </si>
   <si>
     <t>template_cre_view_last_version.sql</t>
+  </si>
+  <si>
+    <t>460_cre_view_fe_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t>_fe_last_import</t>
   </si>
 </sst>
 </file>
@@ -979,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B61" sqref="B52:B61"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1185,7 @@
         <v>88</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
         <v>37</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
@@ -1243,7 +1243,7 @@
         <v>16</v>
       </c>
       <c r="K26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L26" t="s">
         <v>85</v>
@@ -1268,7 +1268,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
         <v>37</v>
@@ -1289,7 +1289,7 @@
         <v>13</v>
       </c>
       <c r="K28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L28" t="s">
         <v>93</v>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
         <v>37</v>
@@ -1332,7 +1332,7 @@
         <v>16</v>
       </c>
       <c r="K30" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L30" t="s">
         <v>85</v>
@@ -1364,10 +1364,10 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D33" t="s">
         <v>13</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D35" t="s">
         <v>35</v>
@@ -1432,10 +1432,10 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D36" t="s">
         <v>35</v>
@@ -1447,7 +1447,7 @@
         <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I36" t="s">
         <v>2</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
@@ -1484,10 +1484,10 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D38" t="s">
         <v>13</v>
@@ -1510,10 +1510,10 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D39" t="s">
         <v>13</v>
@@ -1525,7 +1525,7 @@
         <v>3</v>
       </c>
       <c r="H39" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I39" t="s">
         <v>2</v>
@@ -1542,10 +1542,10 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C40" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
@@ -1560,7 +1560,7 @@
         <v>3</v>
       </c>
       <c r="H40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I40" t="s">
         <v>2</v>
@@ -1574,10 +1574,10 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C41" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D41" t="s">
         <v>13</v>
@@ -1592,7 +1592,7 @@
         <v>3</v>
       </c>
       <c r="H41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I41" t="s">
         <v>2</v>
@@ -1609,10 +1609,10 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C42" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D42" t="s">
         <v>35</v>
@@ -1627,7 +1627,7 @@
         <v>3</v>
       </c>
       <c r="H42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I42" t="s">
         <v>2</v>
@@ -1641,10 +1641,10 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D43" t="s">
         <v>35</v>
@@ -1659,7 +1659,7 @@
         <v>3</v>
       </c>
       <c r="H43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I43" t="s">
         <v>2</v>
@@ -1676,10 +1676,10 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D44" t="s">
         <v>13</v>
@@ -1691,7 +1691,7 @@
         <v>3</v>
       </c>
       <c r="H44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J44" s="7" t="s">
         <v>13</v>
@@ -1708,7 +1708,7 @@
         <v>90</v>
       </c>
       <c r="B45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
         <v>37</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C48" t="s">
         <v>37</v>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>37</v>
@@ -1814,7 +1814,7 @@
         <v>16</v>
       </c>
       <c r="K51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L51" t="s">
         <v>85</v>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>37</v>
@@ -1862,7 +1862,7 @@
         <v>16</v>
       </c>
       <c r="K53" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L53" t="s">
         <v>85</v>
@@ -1889,10 +1889,10 @@
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D55" t="s">
         <v>45</v>
@@ -1928,10 +1928,10 @@
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D57" t="s">
         <v>45</v>
@@ -1945,10 +1945,10 @@
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" s="11" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D58" t="s">
         <v>35</v>
@@ -1960,7 +1960,7 @@
         <v>3</v>
       </c>
       <c r="H58" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="I58" t="s">
         <v>2</v>
@@ -1977,10 +1977,10 @@
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C59" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D59" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
DB - generalize the migration script in the definition to always be up to date Refs #685
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -123,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K51" authorId="0" shapeId="0">
+    <comment ref="K52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K53" authorId="0" shapeId="0">
+    <comment ref="K54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -176,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="135">
   <si>
     <t>_raw</t>
   </si>
@@ -578,6 +578,9 @@
   </si>
   <si>
     <t>_fe_last_import</t>
+  </si>
+  <si>
+    <t>template_micration.sql</t>
   </si>
 </sst>
 </file>
@@ -679,7 +682,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -694,6 +697,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Erklärender Text" xfId="1" builtinId="53"/>
@@ -977,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,283 +1708,262 @@
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B45" s="11" t="str">
+        <f ca="1">"micration_x_to_"&amp;TEXT(TODAY(),"jjjj")&amp;"_"&amp;TEXT(TODAY(),"MM")&amp;"_"&amp;TEXT(TODAY(),"TT")&amp;".sql"</f>
+        <v>micration_x_to_2025_04_18.sql</v>
+      </c>
+      <c r="C45" t="s">
+        <v>134</v>
+      </c>
+      <c r="J45" s="7"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>90</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>112</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>37</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>35</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
         <v>41</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H46" t="s">
         <v>42</v>
       </c>
-      <c r="I45" t="s">
-        <v>1</v>
-      </c>
-      <c r="J45" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I46" t="s">
         <v>1</v>
       </c>
       <c r="J46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B47" s="12"/>
+      <c r="I47" t="s">
+        <v>1</v>
+      </c>
+      <c r="J47" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I47" t="s">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
         <v>2</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J48" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>113</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>37</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>45</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>44</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F49" t="s">
         <v>91</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H49" t="s">
         <v>42</v>
       </c>
-      <c r="I48" t="s">
-        <v>1</v>
-      </c>
-      <c r="J48" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I49" t="s">
         <v>1</v>
       </c>
       <c r="J49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
+        <v>1</v>
+      </c>
+      <c r="J50" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C50" s="8"/>
-      <c r="I50" t="s">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C51" s="8"/>
+      <c r="I51" t="s">
         <v>2</v>
-      </c>
-      <c r="J50" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>114</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D51" t="s">
-        <v>16</v>
-      </c>
-      <c r="E51" t="s">
-        <v>17</v>
-      </c>
-      <c r="F51" t="s">
-        <v>91</v>
-      </c>
-      <c r="H51" t="s">
-        <v>42</v>
-      </c>
-      <c r="I51" t="s">
-        <v>1</v>
       </c>
       <c r="J51" t="s">
         <v>16</v>
       </c>
-      <c r="K51" t="s">
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" t="s">
+        <v>91</v>
+      </c>
+      <c r="H52" t="s">
+        <v>42</v>
+      </c>
+      <c r="I52" t="s">
+        <v>1</v>
+      </c>
+      <c r="J52" t="s">
+        <v>16</v>
+      </c>
+      <c r="K52" t="s">
         <v>122</v>
       </c>
-      <c r="L51" t="s">
+      <c r="L52" t="s">
         <v>85</v>
       </c>
-      <c r="M51" t="s">
+      <c r="M52" t="s">
         <v>43</v>
       </c>
-      <c r="N51" t="s">
+      <c r="N52" t="s">
         <v>41</v>
       </c>
-      <c r="O51" t="s">
+      <c r="O52" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="11"/>
-      <c r="C52" s="9"/>
-      <c r="J52" t="s">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53" s="11"/>
+      <c r="C53" s="9"/>
+      <c r="J53" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="11" t="s">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C54" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>16</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E54" t="s">
         <v>17</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F54" t="s">
         <v>91</v>
       </c>
-      <c r="H53" t="s">
+      <c r="H54" t="s">
         <v>42</v>
       </c>
-      <c r="I53" t="s">
-        <v>1</v>
-      </c>
-      <c r="J53" t="s">
-        <v>16</v>
-      </c>
-      <c r="K53" t="s">
-        <v>123</v>
-      </c>
-      <c r="L53" t="s">
-        <v>85</v>
-      </c>
-      <c r="M53" t="s">
-        <v>46</v>
-      </c>
-      <c r="N53" t="s">
-        <v>44</v>
-      </c>
-      <c r="O53" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="11"/>
-      <c r="C54" s="9"/>
       <c r="I54" t="s">
         <v>1</v>
       </c>
       <c r="J54" t="s">
+        <v>16</v>
+      </c>
+      <c r="K54" t="s">
+        <v>123</v>
+      </c>
+      <c r="L54" t="s">
+        <v>85</v>
+      </c>
+      <c r="M54" t="s">
+        <v>46</v>
+      </c>
+      <c r="N54" t="s">
+        <v>44</v>
+      </c>
+      <c r="O54" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B55" s="11"/>
+      <c r="C55" s="9"/>
+      <c r="I55" t="s">
+        <v>1</v>
+      </c>
+      <c r="J55" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="11" t="s">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C56" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>45</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E56" t="s">
         <v>47</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G56" t="s">
         <v>3</v>
       </c>
-      <c r="I55" t="s">
-        <v>2</v>
-      </c>
-      <c r="J55" t="s">
-        <v>45</v>
-      </c>
-      <c r="N55" t="s">
-        <v>17</v>
-      </c>
-      <c r="O55" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="11"/>
-      <c r="C56" s="9"/>
       <c r="I56" t="s">
         <v>2</v>
       </c>
       <c r="J56" t="s">
+        <v>45</v>
+      </c>
+      <c r="N56" t="s">
+        <v>17</v>
+      </c>
+      <c r="O56" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B57" s="11"/>
+      <c r="C57" s="9"/>
+      <c r="I57" t="s">
+        <v>2</v>
+      </c>
+      <c r="J57" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D57" t="s">
-        <v>45</v>
-      </c>
-      <c r="E57" t="s">
-        <v>44</v>
-      </c>
-      <c r="H57" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>130</v>
+        <v>117</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="D58" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E58" t="s">
-        <v>36</v>
-      </c>
-      <c r="G58" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="H58" t="s">
-        <v>133</v>
-      </c>
-      <c r="I58" t="s">
-        <v>2</v>
-      </c>
-      <c r="J58" t="s">
-        <v>35</v>
-      </c>
-      <c r="N58" t="s">
-        <v>17</v>
-      </c>
-      <c r="O58" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C59" t="s">
-        <v>129</v>
+        <v>132</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>130</v>
       </c>
       <c r="D59" t="s">
         <v>35</v>
@@ -1992,7 +1975,7 @@
         <v>3</v>
       </c>
       <c r="H59" t="s">
-        <v>42</v>
+        <v>133</v>
       </c>
       <c r="I59" t="s">
         <v>2</v>
@@ -2008,12 +1991,44 @@
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="11"/>
-      <c r="C60" s="9"/>
+      <c r="B60" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" t="s">
+        <v>129</v>
+      </c>
+      <c r="D60" t="s">
+        <v>35</v>
+      </c>
+      <c r="E60" t="s">
+        <v>36</v>
+      </c>
+      <c r="G60" t="s">
+        <v>3</v>
+      </c>
+      <c r="H60" t="s">
+        <v>42</v>
+      </c>
+      <c r="I60" t="s">
+        <v>2</v>
+      </c>
+      <c r="J60" t="s">
+        <v>35</v>
+      </c>
+      <c r="N60" t="s">
+        <v>17</v>
+      </c>
+      <c r="O60" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" s="11"/>
       <c r="C61" s="9"/>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62" s="11"/>
+      <c r="C62" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DB - Generally name migration script without date specification
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\INTERPOLAR\Postgres-cds_hub\init\template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="rights_and_functions" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="table_description_convert_def" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
+    <sheet name="table_description_convert_def" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Unknown Author</author>
   </authors>
   <commentList>
-    <comment ref="D23" authorId="0">
+    <comment ref="D23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -45,13 +49,13 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">GRANT TRIGGER
+          <t>GRANT TRIGGER
 GRANT USAGE ON SCHEMA
 GRANT USAGE ON seq</t>
         </r>
       </text>
     </comment>
-    <comment ref="H23" authorId="0">
+    <comment ref="H23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,11 +74,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Rawdaten = varchar oder kein Eintrag dann Datentypen</t>
+          <t>Rawdaten = varchar oder kein Eintrag dann Datentypen</t>
         </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="0">
+    <comment ref="I33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,11 +97,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Bei diesen Views funktioniert die Rechtevergabe im gegensatz zu den diff und view3 Views noch statisch</t>
+          <t>Bei diesen Views funktioniert die Rechtevergabe im gegensatz zu den diff und view3 Views noch statisch</t>
         </r>
       </text>
     </comment>
-    <comment ref="K52" authorId="0">
+    <comment ref="P33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -116,11 +120,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Wie 30 und 31</t>
+          <t>12.7. haben wir in der view geändert - cds2db nicht mehr notwendig</t>
         </r>
       </text>
     </comment>
-    <comment ref="K54" authorId="0">
+    <comment ref="K52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -139,11 +143,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Wie 30 und 31</t>
+          <t>Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="P33" authorId="0">
+    <comment ref="K54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -162,7 +166,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">12.7. haben wir in der view geändert - cds2db nicht mehr notwendig</t>
+          <t>Wie 30 und 31</t>
         </r>
       </text>
     </comment>
@@ -173,420 +177,416 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="135">
   <si>
-    <t xml:space="preserve">Erklärung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spaltenname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschreibung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pfad zur Excel-Datei gefolgt vom Namen des Tabellenblattes in eckigen Klammern mit den Tabellenbeschreibungen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCRIPTNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name des Templates, das ein Script mit diesem Namen erzeugt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OWNER_USER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name des Users, für den Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OWNER_SCHEMA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name des Schemas, für das Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_PREFIX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_POSTFIX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEQ_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIGHTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRANT_TARGET_USER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COPY_FUNC_SCRIPT_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COPY_FUNC_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCHEMA_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POSTFIX_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCHEMA_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POSTFIX_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Definition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEMPLATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COPY_FUNC_SCRIPTNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COPY_FUNC_TEMPLATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_POSTFIX_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_POSTFIX_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./R-cds2db/cds2db/inst/extdata/Table_Description.xlsx[table_description]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100_cre_table_raw_cds2db_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_table.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cds2db_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cds2db_in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_raw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSERT, DELETE, UPDATE, SELECT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120_cre_table_raw_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db_log_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_copy_function.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_raw_cds_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">140_cre_table_typ_cds2db_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TYPED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150_get_last_processing_nr_typed.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_get_last_pnr_typed.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">get_last_processing_nr_typed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">160_cre_table_typ_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">310_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_type_cds_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">180_cre_view_raw_type_diff_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_view_diff.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cds2db_out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_raw_diff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">190_cre_view_typ_dataproc_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_view_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2dataprocessor_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2dataprocessor_out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">190_cre_view_typ_dataproc_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_view_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_last_import</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200_take_over_check_date.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_take_over_check_date_function.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">take_over_last_check_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">210_cre_view_typ_cds2db_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">220_cre_view_raw_cds2db_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_raw_last_import</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230_cre_view_typ_cds2db_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_view_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_last_version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230_cre_view_raw_cds2db_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_raw_last_version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230_cre_view_typ_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230_cre_view_raw_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">250_adding_historical_raw_records.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_adding_historical_records.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_migration.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx[frontend_table_description]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400_cre_table_typ_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2dataprocessor_in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_fe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">440_cre_table_frontend_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2frontend_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2frontend_in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INT_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">420_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">600_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_fe_dp_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">430_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">620_fe_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_fe_fe_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">520_cre_view_fe_out.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2frontend_out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450_cre_table_frontend_in_trig.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_trigger_set_id.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">460_cre_view_fe_dataproc_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_fe_last_import</t>
-  </si>
-  <si>
-    <t xml:space="preserve">470_cre_view_fe_dataproc_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_DEFINITION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name der Definitionsdatei, die konvertiert werden soll (gilt immer für alle Zeilen der Tabelle bis zum Ende oder zu einem anderen Dateinamen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOURCE_COLUMN_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spaltenname in der unveränderten Definitionsdatei (gehört zusammen mit TARGET_COLUMN_NAME in derselben Zeile)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TARGET_COLUMN_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spaltenname in der geänderten Definitionsdatei (gehört zusammen mit SOURCE_COLUMN_NAME in derselben Zeile). Ist der Wert leer, bleibt der Name bestehen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOURCE_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unveränderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem TARGET_TYPE in derselben Zeile)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TARGET_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geänderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem SOURCE_TYPE in derselben Zeile)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESOURCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">varchar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLUMN_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FHIR_EXPRESSION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLUMN_DESCRIPTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REFERENCE_TYPES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FHIR_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLUMN_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SINGLE_LENGTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALUE_LENGTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COUNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALUE_COUNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">decimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">double precision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boolean</t>
+    <t>Erklärung</t>
+  </si>
+  <si>
+    <t>Spaltenname</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>TABLE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Pfad zur Excel-Datei gefolgt vom Namen des Tabellenblattes in eckigen Klammern mit den Tabellenbeschreibungen</t>
+  </si>
+  <si>
+    <t>SCRIPTNAME</t>
+  </si>
+  <si>
+    <t>Name des Templates, das ein Script mit diesem Namen erzeugt.</t>
+  </si>
+  <si>
+    <t>OWNER_USER</t>
+  </si>
+  <si>
+    <t>Name des Users, für den Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
+  </si>
+  <si>
+    <t>OWNER_SCHEMA</t>
+  </si>
+  <si>
+    <t>Name des Schemas, für das Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
+  </si>
+  <si>
+    <t>TABLE_PREFIX</t>
+  </si>
+  <si>
+    <t>TABLE_POSTFIX</t>
+  </si>
+  <si>
+    <t>SEQ_NAME</t>
+  </si>
+  <si>
+    <t>RIGHTS</t>
+  </si>
+  <si>
+    <t>GRANT_TARGET_USER</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_SCRIPT_NAME</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_NAME</t>
+  </si>
+  <si>
+    <t>SCHEMA_2</t>
+  </si>
+  <si>
+    <t>POSTFIX_2</t>
+  </si>
+  <si>
+    <t>SCHEMA_3</t>
+  </si>
+  <si>
+    <t>POSTFIX_3</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>TEMPLATE</t>
+  </si>
+  <si>
+    <t>TAGS</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_SCRIPTNAME</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_TEMPLATE</t>
+  </si>
+  <si>
+    <t>TABLE_POSTFIX_2</t>
+  </si>
+  <si>
+    <t>TABLE_POSTFIX_3</t>
+  </si>
+  <si>
+    <t>./R-cds2db/cds2db/inst/extdata/Table_Description.xlsx[table_description]</t>
+  </si>
+  <si>
+    <t>100_cre_table_raw_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t>template_cre_table.sql</t>
+  </si>
+  <si>
+    <t>cds2db_user</t>
+  </si>
+  <si>
+    <t>cds2db_in</t>
+  </si>
+  <si>
+    <t>RAW</t>
+  </si>
+  <si>
+    <t>_raw</t>
+  </si>
+  <si>
+    <t>INSERT, DELETE, UPDATE, SELECT</t>
+  </si>
+  <si>
+    <t>db_user</t>
+  </si>
+  <si>
+    <t>120_cre_table_raw_db_log.sql</t>
+  </si>
+  <si>
+    <t>db_log_user</t>
+  </si>
+  <si>
+    <t>db_log</t>
+  </si>
+  <si>
+    <t>300_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>template_copy_function.sql</t>
+  </si>
+  <si>
+    <t>copy_raw_cds_in_to_db_log</t>
+  </si>
+  <si>
+    <t>140_cre_table_typ_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t>TYPED</t>
+  </si>
+  <si>
+    <t>150_get_last_processing_nr_typed.sql</t>
+  </si>
+  <si>
+    <t>template_get_last_pnr_typed.sql</t>
+  </si>
+  <si>
+    <t>get_last_processing_nr_typed</t>
+  </si>
+  <si>
+    <t>160_cre_table_typ_log.sql</t>
+  </si>
+  <si>
+    <t>310_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_type_cds_in_to_db_log</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>180_cre_view_raw_type_diff_log.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_diff.sql</t>
+  </si>
+  <si>
+    <t>cds2db_out</t>
+  </si>
+  <si>
+    <t>v_</t>
+  </si>
+  <si>
+    <t>_raw_diff</t>
+  </si>
+  <si>
+    <t>190_cre_view_typ_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_all.sql</t>
+  </si>
+  <si>
+    <t>db2dataprocessor_user</t>
+  </si>
+  <si>
+    <t>db2dataprocessor_out</t>
+  </si>
+  <si>
+    <t>190_cre_view_typ_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_last_import.sql</t>
+  </si>
+  <si>
+    <t>_last_import</t>
+  </si>
+  <si>
+    <t>200_take_over_check_date.sql</t>
+  </si>
+  <si>
+    <t>template_take_over_check_date_function.sql</t>
+  </si>
+  <si>
+    <t>take_over_last_check_date</t>
+  </si>
+  <si>
+    <t>210_cre_view_typ_cds2db_all.sql</t>
+  </si>
+  <si>
+    <t>220_cre_view_raw_cds2db_last_import.sql</t>
+  </si>
+  <si>
+    <t>_raw_last_import</t>
+  </si>
+  <si>
+    <t>230_cre_view_typ_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_last_version.sql</t>
+  </si>
+  <si>
+    <t>_last_version</t>
+  </si>
+  <si>
+    <t>230_cre_view_raw_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t>_raw_last_version</t>
+  </si>
+  <si>
+    <t>230_cre_view_typ_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t>230_cre_view_raw_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t>250_adding_historical_raw_records.sql</t>
+  </si>
+  <si>
+    <t>template_adding_historical_records.sql</t>
+  </si>
+  <si>
+    <t>template_migration.sql</t>
+  </si>
+  <si>
+    <t>./R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx[frontend_table_description]</t>
+  </si>
+  <si>
+    <t>400_cre_table_typ_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t>db2dataprocessor_in</t>
+  </si>
+  <si>
+    <t>_fe</t>
+  </si>
+  <si>
+    <t>440_cre_table_frontend_in.sql</t>
+  </si>
+  <si>
+    <t>db2frontend_user</t>
+  </si>
+  <si>
+    <t>db2frontend_in</t>
+  </si>
+  <si>
+    <t>INT_ID</t>
+  </si>
+  <si>
+    <t>420_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t>600_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_fe_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t>430_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t>620_fe_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_fe_fe_in_to_db_log</t>
+  </si>
+  <si>
+    <t>520_cre_view_fe_out.sql</t>
+  </si>
+  <si>
+    <t>db2frontend_out</t>
+  </si>
+  <si>
+    <t>450_cre_table_frontend_in_trig.sql</t>
+  </si>
+  <si>
+    <t>template_cre_trigger_set_id.sql</t>
+  </si>
+  <si>
+    <t>460_cre_view_fe_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t>_fe_last_import</t>
+  </si>
+  <si>
+    <t>470_cre_view_fe_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t>TABLE_DEFINITION</t>
+  </si>
+  <si>
+    <t>Name der Definitionsdatei, die konvertiert werden soll (gilt immer für alle Zeilen der Tabelle bis zum Ende oder zu einem anderen Dateinamen)</t>
+  </si>
+  <si>
+    <t>SOURCE_COLUMN_NAME</t>
+  </si>
+  <si>
+    <t>Spaltenname in der unveränderten Definitionsdatei (gehört zusammen mit TARGET_COLUMN_NAME in derselben Zeile)</t>
+  </si>
+  <si>
+    <t>TARGET_COLUMN_NAME</t>
+  </si>
+  <si>
+    <t>Spaltenname in der geänderten Definitionsdatei (gehört zusammen mit SOURCE_COLUMN_NAME in derselben Zeile). Ist der Wert leer, bleibt der Name bestehen</t>
+  </si>
+  <si>
+    <t>SOURCE_TYPE</t>
+  </si>
+  <si>
+    <t>unveränderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem TARGET_TYPE in derselben Zeile)</t>
+  </si>
+  <si>
+    <t>TARGET_TYPE</t>
+  </si>
+  <si>
+    <t>geänderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem SOURCE_TYPE in derselben Zeile)</t>
+  </si>
+  <si>
+    <t>RESOURCE</t>
+  </si>
+  <si>
+    <t>TABLE_NAME</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>COLUMN_NAME</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>FHIR_EXPRESSION</t>
+  </si>
+  <si>
+    <t>COLUMN_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>REFERENCE_TYPES</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>FHIR_TYPE</t>
+  </si>
+  <si>
+    <t>COLUMN_TYPE</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>SINGLE_LENGTH</t>
+  </si>
+  <si>
+    <t>VALUE_LENGTH</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>COUNT</t>
+  </si>
+  <si>
+    <t>VALUE_COUNT</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>double precision</t>
+  </si>
+  <si>
+    <t>boolean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,22 +595,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <i val="true"/>
+      <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
@@ -671,19 +656,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.25"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor rgb="FF7F7F7F"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.3999"/>
+        <fgColor theme="9" tint="0.39988402966399123"/>
         <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -691,105 +676,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
-    <cellStyle name="Excel Built-in Bad" xfId="21"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="22"/>
+  <cellStyles count="4">
+    <cellStyle name="Excel Built-in Bad" xfId="2"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="1"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="3"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -848,60 +765,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -933,7 +866,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -957,7 +890,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1017,51 +950,50 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B38" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="B38" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="20.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.71"/>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="73" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="6" width="20.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="40.5703125" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" customWidth="1"/>
+    <col min="13" max="13" width="27" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1069,117 +1001,117 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C19" s="3"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1232,136 +1164,136 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" t="s">
         <v>34</v>
       </c>
-      <c r="H24" s="0" t="s">
+      <c r="H24" t="s">
         <v>35</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="I24" t="s">
         <v>36</v>
       </c>
-      <c r="J24" s="0" t="s">
+      <c r="J24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I25" s="0" t="s">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
         <v>36</v>
       </c>
-      <c r="J25" s="0" t="s">
+      <c r="J25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" t="s">
         <v>34</v>
       </c>
-      <c r="H26" s="0" t="s">
+      <c r="H26" t="s">
         <v>35</v>
       </c>
-      <c r="I26" s="0" t="s">
+      <c r="I26" t="s">
         <v>36</v>
       </c>
-      <c r="J26" s="0" t="s">
+      <c r="J26" t="s">
         <v>39</v>
       </c>
-      <c r="K26" s="0" t="s">
+      <c r="K26" t="s">
         <v>41</v>
       </c>
-      <c r="L26" s="0" t="s">
+      <c r="L26" t="s">
         <v>42</v>
       </c>
-      <c r="M26" s="0" t="s">
+      <c r="M26" t="s">
         <v>43</v>
       </c>
-      <c r="N26" s="0" t="s">
+      <c r="N26" t="s">
         <v>33</v>
       </c>
-      <c r="O26" s="0" t="s">
+      <c r="O26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I27" s="0" t="s">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="0" t="s">
+      <c r="J27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="F28" t="s">
         <v>45</v>
       </c>
-      <c r="I28" s="0" t="s">
+      <c r="I28" t="s">
         <v>36</v>
       </c>
-      <c r="J28" s="0" t="s">
+      <c r="J28" t="s">
         <v>32</v>
       </c>
-      <c r="K28" s="0" t="s">
+      <c r="K28" t="s">
         <v>46</v>
       </c>
-      <c r="L28" s="0" t="s">
+      <c r="L28" t="s">
         <v>47</v>
       </c>
-      <c r="M28" s="0" t="s">
+      <c r="M28" t="s">
         <v>48</v>
       </c>
-      <c r="N28" s="0" t="s">
+      <c r="N28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I29" s="0" t="s">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
         <v>36</v>
       </c>
-      <c r="J29" s="0" t="s">
+      <c r="J29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>49</v>
       </c>
@@ -1396,7 +1328,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="I31" s="6" t="s">
         <v>36</v>
@@ -1405,7 +1337,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="I32" s="6" t="s">
         <v>52</v>
@@ -1414,7 +1346,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>53</v>
       </c>
@@ -1447,7 +1379,7 @@
       </c>
       <c r="P33" s="8"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="I34" s="7" t="s">
         <v>52</v>
@@ -1456,7 +1388,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>58</v>
       </c>
@@ -1482,7 +1414,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>62</v>
       </c>
@@ -1511,7 +1443,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
@@ -1534,7 +1466,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>68</v>
       </c>
@@ -1560,7 +1492,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>69</v>
       </c>
@@ -1592,7 +1524,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>71</v>
       </c>
@@ -1624,7 +1556,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>74</v>
       </c>
@@ -1659,7 +1591,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>76</v>
       </c>
@@ -1691,7 +1623,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>77</v>
       </c>
@@ -1726,7 +1658,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>78</v>
       </c>
@@ -1755,43 +1687,43 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="str">
-        <f aca="true">"migration/migration_to_"&amp;TEXT(TODAY(),"jjjj")&amp;"_"&amp;TEXT(TODAY(),"MM")&amp;"_"&amp;TEXT(TODAY(),"TT")&amp;".sql"</f>
-        <v>migration/migration_to_2025_04_28.sql</v>
+        <f>"migration/migration.sql"</f>
+        <v>migration/migration.sql</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>80</v>
       </c>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" t="s">
         <v>60</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" t="s">
         <v>83</v>
       </c>
-      <c r="H46" s="0" t="s">
+      <c r="H46" t="s">
         <v>84</v>
       </c>
-      <c r="I46" s="0" t="s">
+      <c r="I46" t="s">
         <v>36</v>
       </c>
-      <c r="J46" s="0" t="s">
+      <c r="J46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B47" s="10"/>
       <c r="I47" s="6" t="s">
         <v>36</v>
@@ -1800,49 +1732,49 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I48" s="0" t="s">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
         <v>52</v>
       </c>
-      <c r="J48" s="0" t="s">
+      <c r="J48" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="0" t="s">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>85</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" t="s">
         <v>31</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" t="s">
         <v>86</v>
       </c>
-      <c r="E49" s="0" t="s">
+      <c r="E49" t="s">
         <v>87</v>
       </c>
-      <c r="F49" s="0" t="s">
+      <c r="F49" t="s">
         <v>88</v>
       </c>
-      <c r="H49" s="0" t="s">
+      <c r="H49" t="s">
         <v>84</v>
       </c>
-      <c r="I49" s="0" t="s">
+      <c r="I49" t="s">
         <v>36</v>
       </c>
-      <c r="J49" s="0" t="s">
+      <c r="J49" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I50" s="0" t="s">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
         <v>36</v>
       </c>
-      <c r="J50" s="0" t="s">
+      <c r="J50" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C51" s="11"/>
       <c r="I51" s="6" t="s">
         <v>52</v>
@@ -1851,8 +1783,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="0" t="s">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>89</v>
       </c>
       <c r="C52" s="12" t="s">
@@ -1892,14 +1824,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
       <c r="C53" s="12"/>
       <c r="J53" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>92</v>
       </c>
@@ -1940,7 +1872,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="12"/>
       <c r="I55" s="6" t="s">
@@ -1950,7 +1882,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>95</v>
       </c>
@@ -1979,7 +1911,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
       <c r="C57" s="12"/>
       <c r="I57" s="6" t="s">
@@ -1989,7 +1921,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
         <v>97</v>
       </c>
@@ -2006,7 +1938,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
         <v>99</v>
       </c>
@@ -2038,7 +1970,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
         <v>101</v>
       </c>
@@ -2070,52 +2002,44 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
       <c r="C61" s="12"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
       <c r="C62" s="12"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="68.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.85"/>
+    <col min="1" max="1" width="68.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2123,52 +2047,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>104</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>106</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>108</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>110</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -2185,116 +2109,111 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>115</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>115</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" t="s">
         <v>116</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" t="s">
         <v>119</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" t="s">
         <v>122</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>123</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>124</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" t="s">
         <v>125</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>126</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>127</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" t="s">
         <v>128</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>131</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" t="s">
         <v>132</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="0" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
         <v>134</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" t="s">
         <v>134</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DB - Add config for Dataprocessor_Submodules_Table_Description.xlsx in User_Schema_Rights_Definition.xlsx for creating submodule tables
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -170,12 +170,35 @@
         </r>
       </text>
     </comment>
+    <comment ref="K64" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Autor:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Wie 30 und 31</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="142">
   <si>
     <t>Erklärung</t>
   </si>
@@ -580,6 +603,27 @@
   </si>
   <si>
     <t>boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx[frontend_table_description] </t>
+  </si>
+  <si>
+    <t>330_cre_table_datap_submodules_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t>copy_submodules_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t>331_cre_table_datap_submodules_log.sql</t>
+  </si>
+  <si>
+    <t>332_db_submodules_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>334_cre_view_dataproc_submodules_last_import.sql</t>
+  </si>
+  <si>
+    <t>335_cre_view_dataproc_submodules_all.sql</t>
   </si>
 </sst>
 </file>
@@ -962,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B38" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,7 +1784,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>85</v>
       </c>
@@ -1766,7 +1810,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I50" t="s">
         <v>36</v>
       </c>
@@ -1774,7 +1818,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C51" s="11"/>
       <c r="I51" s="6" t="s">
         <v>52</v>
@@ -1783,7 +1827,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>89</v>
       </c>
@@ -1824,14 +1868,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
       <c r="C53" s="12"/>
       <c r="J53" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>92</v>
       </c>
@@ -1872,7 +1916,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="12"/>
       <c r="I55" s="6" t="s">
@@ -1882,7 +1926,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>95</v>
       </c>
@@ -1911,7 +1955,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
       <c r="C57" s="12"/>
       <c r="I57" s="6" t="s">
@@ -1921,7 +1965,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
         <v>97</v>
       </c>
@@ -1938,7 +1982,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
         <v>99</v>
       </c>
@@ -1970,7 +2014,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
         <v>101</v>
       </c>
@@ -2002,13 +2046,144 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="5"/>
-      <c r="C61" s="12"/>
-    </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>135</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" t="s">
+        <v>60</v>
+      </c>
+      <c r="E61" t="s">
+        <v>83</v>
+      </c>
+      <c r="I61" t="s">
+        <v>36</v>
+      </c>
+      <c r="J61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
-      <c r="C62" s="12"/>
+      <c r="I62" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J62" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I63" t="s">
+        <v>52</v>
+      </c>
+      <c r="J63" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>138</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="L64" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M64" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="N64" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B65" s="6"/>
+      <c r="C65" s="12"/>
+      <c r="J65" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B66" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N66" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B67" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N67" s="6" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
DB - Add config for dataprocessor core tables refs #174
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -193,12 +193,35 @@
         </r>
       </text>
     </comment>
+    <comment ref="K71" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Autor:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Wie 30 und 31</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="149">
   <si>
     <t>Erklärung</t>
   </si>
@@ -624,6 +647,27 @@
   </si>
   <si>
     <t>335_cre_view_dataproc_submodules_all.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./R-dataprocessor/dataprocessor/inst/extdata/Dataprocessor_Table_Description.xlsx[frontend_table_description] </t>
+  </si>
+  <si>
+    <t>340_cre_table_datap_core_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t>341_cre_table_datap_core_log.sql</t>
+  </si>
+  <si>
+    <t>344_cre_view_dataproc_core_last_import.sql</t>
+  </si>
+  <si>
+    <t>345_cre_view_dataproc_core_all.sql</t>
+  </si>
+  <si>
+    <t>342_db_core_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_core_dp_in_to_db_log</t>
   </si>
 </sst>
 </file>
@@ -1006,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q67"/>
+  <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,14 +2166,14 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="C65" s="12"/>
       <c r="J65" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B66" s="6" t="s">
         <v>140</v>
       </c>
@@ -2158,7 +2202,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B67" s="6" t="s">
         <v>141</v>
       </c>
@@ -2182,6 +2226,145 @@
         <v>60</v>
       </c>
       <c r="N67" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>142</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C68" t="s">
+        <v>31</v>
+      </c>
+      <c r="D68" t="s">
+        <v>60</v>
+      </c>
+      <c r="E68" t="s">
+        <v>83</v>
+      </c>
+      <c r="I68" t="s">
+        <v>36</v>
+      </c>
+      <c r="J68" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B69" s="6"/>
+      <c r="I69" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J69" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I70" t="s">
+        <v>52</v>
+      </c>
+      <c r="J70" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>144</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J71" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="L71" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M71" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="N71" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B72" s="6"/>
+      <c r="C72" s="12"/>
+      <c r="J72" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B73" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I73" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J73" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N73" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B74" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N74" s="6" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix User Schema Rights Definition and Table Desciptions
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\INTERPOLAR\Postgres-cds_hub\init\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
-    <sheet name="table_description_convert_def" sheetId="2" r:id="rId2"/>
+    <sheet name="rights_and_functions" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="table_description_convert_def" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,12 +21,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
     <author>Unknown Author</author>
   </authors>
   <commentList>
-    <comment ref="D23" authorId="0" shapeId="0">
+    <comment ref="D23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,13 +45,13 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>GRANT TRIGGER
+          <t xml:space="preserve">GRANT TRIGGER
 GRANT USAGE ON SCHEMA
 GRANT USAGE ON seq</t>
         </r>
       </text>
     </comment>
-    <comment ref="H23" authorId="0" shapeId="0">
+    <comment ref="H23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,11 +70,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Rawdaten = varchar oder kein Eintrag dann Datentypen</t>
+          <t xml:space="preserve">Rawdaten = varchar oder kein Eintrag dann Datentypen</t>
         </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="0" shapeId="0">
+    <comment ref="I33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -97,11 +93,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Bei diesen Views funktioniert die Rechtevergabe im gegensatz zu den diff und view3 Views noch statisch</t>
+          <t xml:space="preserve">Bei diesen Views funktioniert die Rechtevergabe im gegensatz zu den diff und view3 Views noch statisch</t>
         </r>
       </text>
     </comment>
-    <comment ref="P33" authorId="0" shapeId="0">
+    <comment ref="K52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -120,11 +116,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>12.7. haben wir in der view geändert - cds2db nicht mehr notwendig</t>
+          <t xml:space="preserve">Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="K52" authorId="0" shapeId="0">
+    <comment ref="K54" authorId="0">
       <text>
         <r>
           <rPr>
@@ -143,11 +139,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Wie 30 und 31</t>
+          <t xml:space="preserve">Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="K54" authorId="0" shapeId="0">
+    <comment ref="K64" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,11 +162,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Wie 30 und 31</t>
+          <t xml:space="preserve">Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="K64" authorId="0" shapeId="0">
+    <comment ref="K71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -189,11 +185,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Wie 30 und 31</t>
+          <t xml:space="preserve">Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="K71" authorId="0" shapeId="0">
+    <comment ref="P33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -212,7 +208,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Wie 30 und 31</t>
+          <t xml:space="preserve">12.7. haben wir in der view geändert - cds2db nicht mehr notwendig</t>
         </r>
       </text>
     </comment>
@@ -223,458 +219,462 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="149">
   <si>
-    <t>Erklärung</t>
-  </si>
-  <si>
-    <t>Spaltenname</t>
-  </si>
-  <si>
-    <t>Beschreibung</t>
-  </si>
-  <si>
-    <t>TABLE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>Pfad zur Excel-Datei gefolgt vom Namen des Tabellenblattes in eckigen Klammern mit den Tabellenbeschreibungen</t>
-  </si>
-  <si>
-    <t>SCRIPTNAME</t>
-  </si>
-  <si>
-    <t>Name des Templates, das ein Script mit diesem Namen erzeugt.</t>
-  </si>
-  <si>
-    <t>OWNER_USER</t>
-  </si>
-  <si>
-    <t>Name des Users, für den Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
-  </si>
-  <si>
-    <t>OWNER_SCHEMA</t>
-  </si>
-  <si>
-    <t>Name des Schemas, für das Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
-  </si>
-  <si>
-    <t>TABLE_PREFIX</t>
-  </si>
-  <si>
-    <t>TABLE_POSTFIX</t>
-  </si>
-  <si>
-    <t>SEQ_NAME</t>
-  </si>
-  <si>
-    <t>RIGHTS</t>
-  </si>
-  <si>
-    <t>GRANT_TARGET_USER</t>
-  </si>
-  <si>
-    <t>COPY_FUNC_SCRIPT_NAME</t>
-  </si>
-  <si>
-    <t>COPY_FUNC_NAME</t>
-  </si>
-  <si>
-    <t>SCHEMA_2</t>
-  </si>
-  <si>
-    <t>POSTFIX_2</t>
-  </si>
-  <si>
-    <t>SCHEMA_3</t>
-  </si>
-  <si>
-    <t>POSTFIX_3</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>TEMPLATE</t>
-  </si>
-  <si>
-    <t>TAGS</t>
-  </si>
-  <si>
-    <t>COPY_FUNC_SCRIPTNAME</t>
-  </si>
-  <si>
-    <t>COPY_FUNC_TEMPLATE</t>
-  </si>
-  <si>
-    <t>TABLE_POSTFIX_2</t>
-  </si>
-  <si>
-    <t>TABLE_POSTFIX_3</t>
-  </si>
-  <si>
-    <t>./R-cds2db/cds2db/inst/extdata/Table_Description.xlsx[table_description]</t>
-  </si>
-  <si>
-    <t>100_cre_table_raw_cds2db_in.sql</t>
-  </si>
-  <si>
-    <t>template_cre_table.sql</t>
-  </si>
-  <si>
-    <t>cds2db_user</t>
-  </si>
-  <si>
-    <t>cds2db_in</t>
-  </si>
-  <si>
-    <t>RAW</t>
-  </si>
-  <si>
-    <t>_raw</t>
-  </si>
-  <si>
-    <t>INSERT, DELETE, UPDATE, SELECT</t>
-  </si>
-  <si>
-    <t>db_user</t>
-  </si>
-  <si>
-    <t>120_cre_table_raw_db_log.sql</t>
-  </si>
-  <si>
-    <t>db_log_user</t>
-  </si>
-  <si>
-    <t>db_log</t>
-  </si>
-  <si>
-    <t>300_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t>template_copy_function.sql</t>
-  </si>
-  <si>
-    <t>copy_raw_cds_in_to_db_log</t>
-  </si>
-  <si>
-    <t>140_cre_table_typ_cds2db_in.sql</t>
-  </si>
-  <si>
-    <t>TYPED</t>
-  </si>
-  <si>
-    <t>150_get_last_processing_nr_typed.sql</t>
-  </si>
-  <si>
-    <t>template_get_last_pnr_typed.sql</t>
-  </si>
-  <si>
-    <t>get_last_processing_nr_typed</t>
-  </si>
-  <si>
-    <t>160_cre_table_typ_log.sql</t>
-  </si>
-  <si>
-    <t>310_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t>copy_type_cds_in_to_db_log</t>
-  </si>
-  <si>
-    <t>SELECT</t>
-  </si>
-  <si>
-    <t>180_cre_view_raw_type_diff_log.sql</t>
-  </si>
-  <si>
-    <t>template_cre_view_diff.sql</t>
-  </si>
-  <si>
-    <t>cds2db_out</t>
-  </si>
-  <si>
-    <t>v_</t>
-  </si>
-  <si>
-    <t>_raw_diff</t>
-  </si>
-  <si>
-    <t>190_cre_view_typ_dataproc_all.sql</t>
-  </si>
-  <si>
-    <t>template_cre_view_all.sql</t>
-  </si>
-  <si>
-    <t>db2dataprocessor_user</t>
-  </si>
-  <si>
-    <t>db2dataprocessor_out</t>
-  </si>
-  <si>
-    <t>190_cre_view_typ_dataproc_last_import.sql</t>
-  </si>
-  <si>
-    <t>template_cre_view_last_import.sql</t>
-  </si>
-  <si>
-    <t>_last_import</t>
-  </si>
-  <si>
-    <t>200_take_over_check_date.sql</t>
-  </si>
-  <si>
-    <t>template_take_over_check_date_function.sql</t>
-  </si>
-  <si>
-    <t>take_over_last_check_date</t>
-  </si>
-  <si>
-    <t>210_cre_view_typ_cds2db_all.sql</t>
-  </si>
-  <si>
-    <t>220_cre_view_raw_cds2db_last_import.sql</t>
-  </si>
-  <si>
-    <t>_raw_last_import</t>
-  </si>
-  <si>
-    <t>230_cre_view_typ_cds2db_last_version.sql</t>
-  </si>
-  <si>
-    <t>template_cre_view_last_version.sql</t>
-  </si>
-  <si>
-    <t>_last_version</t>
-  </si>
-  <si>
-    <t>230_cre_view_raw_cds2db_last_version.sql</t>
-  </si>
-  <si>
-    <t>_raw_last_version</t>
-  </si>
-  <si>
-    <t>230_cre_view_typ_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t>230_cre_view_raw_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t>250_adding_historical_raw_records.sql</t>
-  </si>
-  <si>
-    <t>template_adding_historical_records.sql</t>
-  </si>
-  <si>
-    <t>template_migration.sql</t>
-  </si>
-  <si>
-    <t>./R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx[frontend_table_description]</t>
-  </si>
-  <si>
-    <t>400_cre_table_typ_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t>db2dataprocessor_in</t>
-  </si>
-  <si>
-    <t>_fe</t>
-  </si>
-  <si>
-    <t>440_cre_table_frontend_in.sql</t>
-  </si>
-  <si>
-    <t>db2frontend_user</t>
-  </si>
-  <si>
-    <t>db2frontend_in</t>
-  </si>
-  <si>
-    <t>INT_ID</t>
-  </si>
-  <si>
-    <t>420_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t>600_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t>copy_fe_dp_in_to_db_log</t>
-  </si>
-  <si>
-    <t>430_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t>620_fe_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t>copy_fe_fe_in_to_db_log</t>
-  </si>
-  <si>
-    <t>520_cre_view_fe_out.sql</t>
-  </si>
-  <si>
-    <t>db2frontend_out</t>
-  </si>
-  <si>
-    <t>450_cre_table_frontend_in_trig.sql</t>
-  </si>
-  <si>
-    <t>template_cre_trigger_set_id.sql</t>
-  </si>
-  <si>
-    <t>460_cre_view_fe_dataproc_last_import.sql</t>
-  </si>
-  <si>
-    <t>_fe_last_import</t>
-  </si>
-  <si>
-    <t>470_cre_view_fe_dataproc_all.sql</t>
-  </si>
-  <si>
-    <t>TABLE_DEFINITION</t>
-  </si>
-  <si>
-    <t>Name der Definitionsdatei, die konvertiert werden soll (gilt immer für alle Zeilen der Tabelle bis zum Ende oder zu einem anderen Dateinamen)</t>
-  </si>
-  <si>
-    <t>SOURCE_COLUMN_NAME</t>
-  </si>
-  <si>
-    <t>Spaltenname in der unveränderten Definitionsdatei (gehört zusammen mit TARGET_COLUMN_NAME in derselben Zeile)</t>
-  </si>
-  <si>
-    <t>TARGET_COLUMN_NAME</t>
-  </si>
-  <si>
-    <t>Spaltenname in der geänderten Definitionsdatei (gehört zusammen mit SOURCE_COLUMN_NAME in derselben Zeile). Ist der Wert leer, bleibt der Name bestehen</t>
-  </si>
-  <si>
-    <t>SOURCE_TYPE</t>
-  </si>
-  <si>
-    <t>unveränderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem TARGET_TYPE in derselben Zeile)</t>
-  </si>
-  <si>
-    <t>TARGET_TYPE</t>
-  </si>
-  <si>
-    <t>geänderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem SOURCE_TYPE in derselben Zeile)</t>
-  </si>
-  <si>
-    <t>RESOURCE</t>
-  </si>
-  <si>
-    <t>TABLE_NAME</t>
-  </si>
-  <si>
-    <t>varchar</t>
-  </si>
-  <si>
-    <t>COLUMN_NAME</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>FHIR_EXPRESSION</t>
-  </si>
-  <si>
-    <t>COLUMN_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>timestamp</t>
-  </si>
-  <si>
-    <t>REFERENCE_TYPES</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>FHIR_TYPE</t>
-  </si>
-  <si>
-    <t>COLUMN_TYPE</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>SINGLE_LENGTH</t>
-  </si>
-  <si>
-    <t>VALUE_LENGTH</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>COUNT</t>
-  </si>
-  <si>
-    <t>VALUE_COUNT</t>
-  </si>
-  <si>
-    <t>decimal</t>
-  </si>
-  <si>
-    <t>double precision</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx[frontend_table_description] </t>
-  </si>
-  <si>
-    <t>330_cre_table_datap_submodules_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t>copy_submodules_dp_in_to_db_log</t>
-  </si>
-  <si>
-    <t>331_cre_table_datap_submodules_log.sql</t>
-  </si>
-  <si>
-    <t>332_db_submodules_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t>334_cre_view_dataproc_submodules_last_import.sql</t>
-  </si>
-  <si>
-    <t>335_cre_view_dataproc_submodules_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./R-dataprocessor/dataprocessor/inst/extdata/Dataprocessor_Table_Description.xlsx[frontend_table_description] </t>
-  </si>
-  <si>
-    <t>340_cre_table_datap_core_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t>341_cre_table_datap_core_log.sql</t>
-  </si>
-  <si>
-    <t>344_cre_view_dataproc_core_last_import.sql</t>
-  </si>
-  <si>
-    <t>345_cre_view_dataproc_core_all.sql</t>
-  </si>
-  <si>
-    <t>342_db_core_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t>copy_core_dp_in_to_db_log</t>
+    <t xml:space="preserve">Erklärung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spaltenname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beschreibung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pfad zur Excel-Datei gefolgt vom Namen des Tabellenblattes in eckigen Klammern mit den Tabellenbeschreibungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCRIPTNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name des Templates, das ein Script mit diesem Namen erzeugt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OWNER_USER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name des Users, für den Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OWNER_SCHEMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name des Schemas, für das Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_PREFIX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_POSTFIX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEQ_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIGHTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT_TARGET_USER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COPY_FUNC_SCRIPT_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COPY_FUNC_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHEMA_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSTFIX_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHEMA_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSTFIX_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMPLATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COPY_FUNC_SCRIPTNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COPY_FUNC_TEMPLATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_POSTFIX_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_POSTFIX_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./R-cds2db/cds2db/inst/extdata/Table_Description.xlsx[table_description]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100_cre_table_raw_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_cre_table.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cds2db_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cds2db_in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSERT, DELETE, UPDATE, SELECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120_cre_table_raw_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db_log_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_copy_function.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy_raw_cds_in_to_db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">140_cre_table_typ_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150_get_last_processing_nr_typed.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_get_last_pnr_typed.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get_last_processing_nr_typed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">160_cre_table_typ_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">310_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy_type_cds_in_to_db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">180_cre_view_raw_type_diff_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_cre_view_diff.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cds2db_out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_raw_diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">190_cre_view_typ_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_cre_view_all.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db2dataprocessor_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db2dataprocessor_out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">190_cre_view_typ_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_cre_view_last_import.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_last_import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200_take_over_check_date.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_take_over_check_date_function.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">take_over_last_check_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">210_cre_view_typ_cds2db_all.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220_cre_view_raw_cds2db_last_import.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_raw_last_import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230_cre_view_typ_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_cre_view_last_version.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_last_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230_cre_view_raw_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_raw_last_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230_cre_view_typ_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230_cre_view_raw_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250_adding_historical_raw_records.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_adding_historical_records.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_migration.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx[frontend_table_description]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400_cre_table_typ_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db2dataprocessor_in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_fe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440_cre_table_frontend_in.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db2frontend_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db2frontend_in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">420_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">600_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy_fe_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">430_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">620_fe_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy_fe_fe_in_to_db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">520_cre_view_fe_out.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db2frontend_out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">450_cre_table_frontend_in_trig.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_cre_trigger_set_id.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">460_cre_view_fe_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_fe_last_import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470_cre_view_fe_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx[table_description]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">330_cre_table_datap_submodules_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">331_cre_table_datap_submodules_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">332_db_submodules_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy_submodules_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">334_cre_view_dataproc_submodules_last_import.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">335_cre_view_dataproc_submodules_all.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./R-dataprocessor/dataprocessor/inst/extdata/Dataprocessor_Table_Description.xlsx[table_description]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">340_cre_table_datap_core_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">341_cre_table_datap_core_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">342_db_core_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy_core_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">344_cre_view_dataproc_core_last_import.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">345_cre_view_dataproc_core_all.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_DEFINITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name der Definitionsdatei, die konvertiert werden soll (gilt immer für alle Zeilen der Tabelle bis zum Ende oder zu einem anderen Dateinamen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOURCE_COLUMN_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spaltenname in der unveränderten Definitionsdatei (gehört zusammen mit TARGET_COLUMN_NAME in derselben Zeile)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TARGET_COLUMN_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spaltenname in der geänderten Definitionsdatei (gehört zusammen mit SOURCE_COLUMN_NAME in derselben Zeile). Ist der Wert leer, bleibt der Name bestehen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOURCE_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unveränderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem TARGET_TYPE in derselben Zeile)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TARGET_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geänderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem SOURCE_TYPE in derselben Zeile)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESOURCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLUMN_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FHIR_EXPRESSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLUMN_DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REFERENCE_TYPES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FHIR_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLUMN_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SINGLE_LENGTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALUE_LENGTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALUE_COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">double precision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,7 +683,22 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
@@ -744,19 +759,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="9" tint="-0.25"/>
         <bgColor rgb="FF7F7F7F"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39988402966399123"/>
+        <fgColor theme="9" tint="0.3998"/>
         <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -764,37 +779,101 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="23">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+  <cellXfs count="12">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Excel Built-in Bad" xfId="2"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="1"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="3"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="9">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
+    <cellStyle name="Excel Built-in Bad" xfId="21"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="22"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -853,76 +932,60 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="44546a"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="e7e6e6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="5b9bd5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="ed7d31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="a5a5a5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="ffc000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4472c4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="70ad47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0563c1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="954f72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -954,7 +1017,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -978,7 +1041,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1038,351 +1101,352 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="73" customWidth="1"/>
-    <col min="3" max="3" width="43.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="6" width="20.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="40.5703125" customWidth="1"/>
-    <col min="12" max="12" width="28.42578125" customWidth="1"/>
-    <col min="13" max="13" width="27" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="95.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="20.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="24.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C19" s="3"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="K23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="L23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M23" s="2" t="s">
+      <c r="M23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N23" s="2" t="s">
+      <c r="N23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="O23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="P23" s="2" t="s">
+      <c r="P23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Q23" s="2" t="s">
+      <c r="Q23" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I25" t="s">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="N26" t="s">
+      <c r="N26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O26" t="s">
+      <c r="O26" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I27" t="s">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L28" t="s">
+      <c r="L28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="N28" t="s">
+      <c r="N28" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I29" t="s">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="6" t="s">
         <v>49</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -1416,8 +1480,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="5"/>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="6"/>
       <c r="I31" s="6" t="s">
         <v>36</v>
       </c>
@@ -1425,8 +1489,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="6"/>
       <c r="I32" s="6" t="s">
         <v>52</v>
       </c>
@@ -1434,8 +1498,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -1467,8 +1531,8 @@
       </c>
       <c r="P33" s="8"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="5"/>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="6"/>
       <c r="I34" s="7" t="s">
         <v>52</v>
       </c>
@@ -1476,8 +1540,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="6" t="s">
         <v>58</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -1502,8 +1566,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C36" s="9" t="s">
@@ -1531,8 +1595,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="6" t="s">
         <v>65</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -1554,8 +1618,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="6" t="s">
         <v>68</v>
       </c>
       <c r="C38" s="6" t="s">
@@ -1580,8 +1644,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="5" t="s">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="6" t="s">
         <v>69</v>
       </c>
       <c r="C39" s="9" t="s">
@@ -1612,8 +1676,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="6" t="s">
         <v>71</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -1644,8 +1708,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="5" t="s">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="6" t="s">
         <v>74</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -1679,8 +1743,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -1711,8 +1775,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="5" t="s">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="6" t="s">
         <v>77</v>
       </c>
       <c r="C43" s="6" t="s">
@@ -1746,8 +1810,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="5" t="s">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="6" t="s">
         <v>78</v>
       </c>
       <c r="C44" s="6" t="s">
@@ -1775,9 +1839,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="5" t="str">
-        <f>"migration/migration.sql"</f>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="6" t="str">
+        <f aca="false">"migration/migration.sql"</f>
         <v>migration/migration.sql</v>
       </c>
       <c r="C45" s="6" t="s">
@@ -1785,33 +1849,33 @@
       </c>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H46" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I46" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J46" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="10"/>
       <c r="I47" s="6" t="s">
         <v>36</v>
@@ -1820,49 +1884,49 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I48" t="s">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I48" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J48" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H49" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I50" t="s">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I50" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="11"/>
       <c r="I51" s="6" t="s">
         <v>52</v>
@@ -1871,11 +1935,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D52" s="6" t="s">
@@ -1912,18 +1976,18 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="5"/>
-      <c r="C53" s="12"/>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="6"/>
+      <c r="C53" s="11"/>
       <c r="J53" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="5" t="s">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="6" t="s">
@@ -1960,9 +2024,9 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="5"/>
-      <c r="C55" s="12"/>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="6"/>
+      <c r="C55" s="11"/>
       <c r="I55" s="6" t="s">
         <v>36</v>
       </c>
@@ -1970,8 +2034,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="5" t="s">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="6" t="s">
         <v>95</v>
       </c>
       <c r="C56" s="9" t="s">
@@ -1999,9 +2063,9 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="5"/>
-      <c r="C57" s="12"/>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="6"/>
+      <c r="C57" s="11"/>
       <c r="I57" s="6" t="s">
         <v>52</v>
       </c>
@@ -2009,11 +2073,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="5" t="s">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C58" s="11" t="s">
         <v>98</v>
       </c>
       <c r="D58" s="6" t="s">
@@ -2026,8 +2090,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="5" t="s">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="6" t="s">
         <v>99</v>
       </c>
       <c r="C59" s="9" t="s">
@@ -2058,8 +2122,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="5" t="s">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C60" s="6" t="s">
@@ -2090,31 +2154,31 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>135</v>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C61" t="s">
+        <v>103</v>
+      </c>
+      <c r="C61" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I61" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J61" t="s">
+      <c r="J61" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="5"/>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="6"/>
       <c r="I62" s="6" t="s">
         <v>36</v>
       </c>
@@ -2122,19 +2186,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I63" t="s">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I63" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J63" t="s">
+      <c r="J63" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>138</v>
-      </c>
-      <c r="C64" s="12" t="s">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C64" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D64" s="6" t="s">
@@ -2154,28 +2218,28 @@
         <v>39</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="L64" s="6" t="s">
         <v>42</v>
       </c>
       <c r="M64" s="6" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="N64" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="6"/>
-      <c r="C65" s="12"/>
+      <c r="C65" s="11"/>
       <c r="J65" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="6" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>63</v>
@@ -2202,9 +2266,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="6" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>59</v>
@@ -2229,30 +2293,30 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>142</v>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C68" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I68" t="s">
+      <c r="I68" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J68" t="s">
+      <c r="J68" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="6"/>
       <c r="I69" s="6" t="s">
         <v>36</v>
@@ -2261,19 +2325,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I70" t="s">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I70" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J70" t="s">
+      <c r="J70" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>144</v>
-      </c>
-      <c r="C71" s="12" t="s">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C71" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D71" s="6" t="s">
@@ -2293,28 +2357,28 @@
         <v>39</v>
       </c>
       <c r="K71" s="6" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="L71" s="6" t="s">
         <v>42</v>
       </c>
       <c r="M71" s="6" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="N71" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="6"/>
-      <c r="C72" s="12"/>
+      <c r="C72" s="11"/>
       <c r="J72" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="6" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>63</v>
@@ -2341,9 +2405,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="6" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>59</v>
@@ -2368,210 +2432,234 @@
         <v>40</v>
       </c>
     </row>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="68.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="68.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.85"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B10" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11" t="s">
-        <v>113</v>
-      </c>
-      <c r="E11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" t="s">
-        <v>115</v>
-      </c>
-      <c r="D12" t="s">
-        <v>116</v>
-      </c>
-      <c r="E12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D14" t="s">
-        <v>122</v>
-      </c>
-      <c r="E14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" t="s">
-        <v>124</v>
-      </c>
-      <c r="D15" t="s">
-        <v>125</v>
-      </c>
-      <c r="E15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="B11" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C11" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E11" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E16" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C12" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E12" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C13" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E17" t="s">
+      <c r="D13" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+      <c r="E13" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E18" t="s">
-        <v>134</v>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DB - rename the sql scripts to harmonize this
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\INTERPOLAR\Postgres-cds_hub\init\template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="rights_and_functions" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="table_description_convert_def" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
+    <sheet name="table_description_convert_def" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Unknown Author</author>
   </authors>
   <commentList>
-    <comment ref="D23" authorId="0">
+    <comment ref="D23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -45,13 +49,13 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">GRANT TRIGGER
+          <t>GRANT TRIGGER
 GRANT USAGE ON SCHEMA
 GRANT USAGE ON seq</t>
         </r>
       </text>
     </comment>
-    <comment ref="H23" authorId="0">
+    <comment ref="H23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,11 +74,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Rawdaten = varchar oder kein Eintrag dann Datentypen</t>
+          <t>Rawdaten = varchar oder kein Eintrag dann Datentypen</t>
         </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="0">
+    <comment ref="I33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,11 +97,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Bei diesen Views funktioniert die Rechtevergabe im gegensatz zu den diff und view3 Views noch statisch</t>
+          <t>Bei diesen Views funktioniert die Rechtevergabe im gegensatz zu den diff und view3 Views noch statisch</t>
         </r>
       </text>
     </comment>
-    <comment ref="K52" authorId="0">
+    <comment ref="P33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -116,11 +120,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Wie 30 und 31</t>
+          <t>12.7. haben wir in der view geändert - cds2db nicht mehr notwendig</t>
         </r>
       </text>
     </comment>
-    <comment ref="K54" authorId="0">
+    <comment ref="K52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -139,11 +143,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Wie 30 und 31</t>
+          <t>Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="K64" authorId="0">
+    <comment ref="K54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -162,11 +166,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Wie 30 und 31</t>
+          <t>Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="K71" authorId="0">
+    <comment ref="K64" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -185,11 +189,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Wie 30 und 31</t>
+          <t>Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="P33" authorId="0">
+    <comment ref="K71" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -208,7 +212,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">12.7. haben wir in der view geändert - cds2db nicht mehr notwendig</t>
+          <t>Wie 30 und 31</t>
         </r>
       </text>
     </comment>
@@ -219,462 +223,458 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="149">
   <si>
-    <t xml:space="preserve">Erklärung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spaltenname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschreibung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pfad zur Excel-Datei gefolgt vom Namen des Tabellenblattes in eckigen Klammern mit den Tabellenbeschreibungen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCRIPTNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name des Templates, das ein Script mit diesem Namen erzeugt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OWNER_USER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name des Users, für den Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OWNER_SCHEMA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name des Schemas, für das Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_PREFIX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_POSTFIX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEQ_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIGHTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRANT_TARGET_USER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COPY_FUNC_SCRIPT_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COPY_FUNC_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCHEMA_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POSTFIX_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCHEMA_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POSTFIX_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Definition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEMPLATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COPY_FUNC_SCRIPTNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COPY_FUNC_TEMPLATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_POSTFIX_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_POSTFIX_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./R-cds2db/cds2db/inst/extdata/Table_Description.xlsx[table_description]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100_cre_table_raw_cds2db_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_table.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cds2db_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cds2db_in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_raw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSERT, DELETE, UPDATE, SELECT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120_cre_table_raw_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db_log_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_copy_function.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_raw_cds_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">140_cre_table_typ_cds2db_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TYPED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150_get_last_processing_nr_typed.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_get_last_pnr_typed.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">get_last_processing_nr_typed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">160_cre_table_typ_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">310_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_type_cds_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">180_cre_view_raw_type_diff_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_view_diff.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cds2db_out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_raw_diff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">190_cre_view_typ_dataproc_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_view_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2dataprocessor_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2dataprocessor_out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">190_cre_view_typ_dataproc_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_view_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_last_import</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200_take_over_check_date.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_take_over_check_date_function.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">take_over_last_check_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">210_cre_view_typ_cds2db_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">220_cre_view_raw_cds2db_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_raw_last_import</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230_cre_view_typ_cds2db_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_view_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_last_version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230_cre_view_raw_cds2db_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_raw_last_version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230_cre_view_typ_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230_cre_view_raw_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">250_adding_historical_raw_records.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_adding_historical_records.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_migration.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx[frontend_table_description]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400_cre_table_typ_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2dataprocessor_in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_fe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">440_cre_table_frontend_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2frontend_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2frontend_in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INT_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">420_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">600_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_fe_dp_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">430_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">620_fe_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_fe_fe_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">520_cre_view_fe_out.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2frontend_out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450_cre_table_frontend_in_trig.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_trigger_set_id.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">460_cre_view_fe_dataproc_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_fe_last_import</t>
-  </si>
-  <si>
-    <t xml:space="preserve">470_cre_view_fe_dataproc_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx[table_description]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">330_cre_table_datap_submodules_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">331_cre_table_datap_submodules_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">332_db_submodules_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_submodules_dp_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">334_cre_view_dataproc_submodules_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">335_cre_view_dataproc_submodules_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./R-dataprocessor/dataprocessor/inst/extdata/Dataprocessor_Table_Description.xlsx[table_description]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">340_cre_table_datap_core_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">341_cre_table_datap_core_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">342_db_core_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_core_dp_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">344_cre_view_dataproc_core_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">345_cre_view_dataproc_core_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_DEFINITION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name der Definitionsdatei, die konvertiert werden soll (gilt immer für alle Zeilen der Tabelle bis zum Ende oder zu einem anderen Dateinamen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOURCE_COLUMN_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spaltenname in der unveränderten Definitionsdatei (gehört zusammen mit TARGET_COLUMN_NAME in derselben Zeile)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TARGET_COLUMN_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spaltenname in der geänderten Definitionsdatei (gehört zusammen mit SOURCE_COLUMN_NAME in derselben Zeile). Ist der Wert leer, bleibt der Name bestehen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOURCE_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unveränderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem TARGET_TYPE in derselben Zeile)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TARGET_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geänderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem SOURCE_TYPE in derselben Zeile)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESOURCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">varchar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLUMN_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FHIR_EXPRESSION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLUMN_DESCRIPTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REFERENCE_TYPES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FHIR_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLUMN_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SINGLE_LENGTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALUE_LENGTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COUNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALUE_COUNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">decimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">double precision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boolean</t>
+    <t>Erklärung</t>
+  </si>
+  <si>
+    <t>Spaltenname</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>TABLE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Pfad zur Excel-Datei gefolgt vom Namen des Tabellenblattes in eckigen Klammern mit den Tabellenbeschreibungen</t>
+  </si>
+  <si>
+    <t>SCRIPTNAME</t>
+  </si>
+  <si>
+    <t>Name des Templates, das ein Script mit diesem Namen erzeugt.</t>
+  </si>
+  <si>
+    <t>OWNER_USER</t>
+  </si>
+  <si>
+    <t>Name des Users, für den Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
+  </si>
+  <si>
+    <t>OWNER_SCHEMA</t>
+  </si>
+  <si>
+    <t>Name des Schemas, für das Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
+  </si>
+  <si>
+    <t>TABLE_PREFIX</t>
+  </si>
+  <si>
+    <t>TABLE_POSTFIX</t>
+  </si>
+  <si>
+    <t>SEQ_NAME</t>
+  </si>
+  <si>
+    <t>RIGHTS</t>
+  </si>
+  <si>
+    <t>GRANT_TARGET_USER</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_SCRIPT_NAME</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_NAME</t>
+  </si>
+  <si>
+    <t>SCHEMA_2</t>
+  </si>
+  <si>
+    <t>POSTFIX_2</t>
+  </si>
+  <si>
+    <t>SCHEMA_3</t>
+  </si>
+  <si>
+    <t>POSTFIX_3</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>TEMPLATE</t>
+  </si>
+  <si>
+    <t>TAGS</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_SCRIPTNAME</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_TEMPLATE</t>
+  </si>
+  <si>
+    <t>TABLE_POSTFIX_2</t>
+  </si>
+  <si>
+    <t>TABLE_POSTFIX_3</t>
+  </si>
+  <si>
+    <t>./R-cds2db/cds2db/inst/extdata/Table_Description.xlsx[table_description]</t>
+  </si>
+  <si>
+    <t>100_cre_table_raw_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t>template_cre_table.sql</t>
+  </si>
+  <si>
+    <t>cds2db_user</t>
+  </si>
+  <si>
+    <t>cds2db_in</t>
+  </si>
+  <si>
+    <t>RAW</t>
+  </si>
+  <si>
+    <t>_raw</t>
+  </si>
+  <si>
+    <t>INSERT, DELETE, UPDATE, SELECT</t>
+  </si>
+  <si>
+    <t>db_user</t>
+  </si>
+  <si>
+    <t>120_cre_table_raw_db_log.sql</t>
+  </si>
+  <si>
+    <t>db_log_user</t>
+  </si>
+  <si>
+    <t>db_log</t>
+  </si>
+  <si>
+    <t>300_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>template_copy_function.sql</t>
+  </si>
+  <si>
+    <t>copy_raw_cds_in_to_db_log</t>
+  </si>
+  <si>
+    <t>140_cre_table_typ_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t>TYPED</t>
+  </si>
+  <si>
+    <t>150_get_last_processing_nr_typed.sql</t>
+  </si>
+  <si>
+    <t>template_get_last_pnr_typed.sql</t>
+  </si>
+  <si>
+    <t>get_last_processing_nr_typed</t>
+  </si>
+  <si>
+    <t>160_cre_table_typ_log.sql</t>
+  </si>
+  <si>
+    <t>310_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_type_cds_in_to_db_log</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>180_cre_view_raw_type_diff_log.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_diff.sql</t>
+  </si>
+  <si>
+    <t>cds2db_out</t>
+  </si>
+  <si>
+    <t>v_</t>
+  </si>
+  <si>
+    <t>_raw_diff</t>
+  </si>
+  <si>
+    <t>190_cre_view_typ_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_all.sql</t>
+  </si>
+  <si>
+    <t>db2dataprocessor_user</t>
+  </si>
+  <si>
+    <t>db2dataprocessor_out</t>
+  </si>
+  <si>
+    <t>190_cre_view_typ_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_last_import.sql</t>
+  </si>
+  <si>
+    <t>_last_import</t>
+  </si>
+  <si>
+    <t>200_take_over_check_date.sql</t>
+  </si>
+  <si>
+    <t>template_take_over_check_date_function.sql</t>
+  </si>
+  <si>
+    <t>take_over_last_check_date</t>
+  </si>
+  <si>
+    <t>210_cre_view_typ_cds2db_all.sql</t>
+  </si>
+  <si>
+    <t>220_cre_view_raw_cds2db_last_import.sql</t>
+  </si>
+  <si>
+    <t>_raw_last_import</t>
+  </si>
+  <si>
+    <t>230_cre_view_typ_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_last_version.sql</t>
+  </si>
+  <si>
+    <t>_last_version</t>
+  </si>
+  <si>
+    <t>230_cre_view_raw_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t>_raw_last_version</t>
+  </si>
+  <si>
+    <t>230_cre_view_typ_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t>230_cre_view_raw_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t>250_adding_historical_raw_records.sql</t>
+  </si>
+  <si>
+    <t>template_adding_historical_records.sql</t>
+  </si>
+  <si>
+    <t>template_migration.sql</t>
+  </si>
+  <si>
+    <t>./R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx[frontend_table_description]</t>
+  </si>
+  <si>
+    <t>400_cre_table_typ_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t>db2dataprocessor_in</t>
+  </si>
+  <si>
+    <t>_fe</t>
+  </si>
+  <si>
+    <t>440_cre_table_frontend_in.sql</t>
+  </si>
+  <si>
+    <t>db2frontend_user</t>
+  </si>
+  <si>
+    <t>db2frontend_in</t>
+  </si>
+  <si>
+    <t>INT_ID</t>
+  </si>
+  <si>
+    <t>420_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t>600_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_fe_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t>430_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t>620_fe_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_fe_fe_in_to_db_log</t>
+  </si>
+  <si>
+    <t>520_cre_view_fe_out.sql</t>
+  </si>
+  <si>
+    <t>db2frontend_out</t>
+  </si>
+  <si>
+    <t>450_cre_table_frontend_in_trig.sql</t>
+  </si>
+  <si>
+    <t>template_cre_trigger_set_id.sql</t>
+  </si>
+  <si>
+    <t>460_cre_view_fe_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t>_fe_last_import</t>
+  </si>
+  <si>
+    <t>470_cre_view_fe_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t>./R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx[table_description]</t>
+  </si>
+  <si>
+    <t>332_db_submodules_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_submodules_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t>334_cre_view_dataproc_submodules_last_import.sql</t>
+  </si>
+  <si>
+    <t>335_cre_view_dataproc_submodules_all.sql</t>
+  </si>
+  <si>
+    <t>./R-dataprocessor/dataprocessor/inst/extdata/Dataprocessor_Table_Description.xlsx[table_description]</t>
+  </si>
+  <si>
+    <t>342_db_core_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_core_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t>344_cre_view_dataproc_core_last_import.sql</t>
+  </si>
+  <si>
+    <t>345_cre_view_dataproc_core_all.sql</t>
+  </si>
+  <si>
+    <t>TABLE_DEFINITION</t>
+  </si>
+  <si>
+    <t>Name der Definitionsdatei, die konvertiert werden soll (gilt immer für alle Zeilen der Tabelle bis zum Ende oder zu einem anderen Dateinamen)</t>
+  </si>
+  <si>
+    <t>SOURCE_COLUMN_NAME</t>
+  </si>
+  <si>
+    <t>Spaltenname in der unveränderten Definitionsdatei (gehört zusammen mit TARGET_COLUMN_NAME in derselben Zeile)</t>
+  </si>
+  <si>
+    <t>TARGET_COLUMN_NAME</t>
+  </si>
+  <si>
+    <t>Spaltenname in der geänderten Definitionsdatei (gehört zusammen mit SOURCE_COLUMN_NAME in derselben Zeile). Ist der Wert leer, bleibt der Name bestehen</t>
+  </si>
+  <si>
+    <t>SOURCE_TYPE</t>
+  </si>
+  <si>
+    <t>unveränderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem TARGET_TYPE in derselben Zeile)</t>
+  </si>
+  <si>
+    <t>TARGET_TYPE</t>
+  </si>
+  <si>
+    <t>geänderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem SOURCE_TYPE in derselben Zeile)</t>
+  </si>
+  <si>
+    <t>RESOURCE</t>
+  </si>
+  <si>
+    <t>TABLE_NAME</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>COLUMN_NAME</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>FHIR_EXPRESSION</t>
+  </si>
+  <si>
+    <t>COLUMN_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>REFERENCE_TYPES</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>FHIR_TYPE</t>
+  </si>
+  <si>
+    <t>COLUMN_TYPE</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>SINGLE_LENGTH</t>
+  </si>
+  <si>
+    <t>VALUE_LENGTH</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>COUNT</t>
+  </si>
+  <si>
+    <t>VALUE_COUNT</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>double precision</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>330_cre_table_dataproc_submodules_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t>331_cre_table_dataproc_submodules_log.sql</t>
+  </si>
+  <si>
+    <t>340_cre_table_dataproc_core_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t>341_cre_table_dataproc_core_log.sql</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,22 +683,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <i val="true"/>
+      <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
@@ -759,19 +744,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.25"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor rgb="FF7F7F7F"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.3998"/>
+        <fgColor theme="9" tint="0.39979247413556324"/>
         <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -779,101 +764,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
-    <cellStyle name="Excel Built-in Bad" xfId="21"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="22"/>
+  <cellStyles count="4">
+    <cellStyle name="Excel Built-in Bad" xfId="2"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="1"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="3"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -932,60 +852,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -1017,7 +953,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -1041,7 +977,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1101,51 +1037,50 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:Q1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="95.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="20.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="24.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="40.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="28.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.71"/>
+    <col min="1" max="1" width="95.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="73" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="20.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="40.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="27" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1153,11 +1088,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1165,7 +1100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1173,7 +1108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1181,7 +1116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1189,81 +1124,81 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
@@ -1316,7 +1251,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1345,7 +1280,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I25" s="1" t="s">
         <v>36</v>
       </c>
@@ -1353,7 +1288,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>38</v>
       </c>
@@ -1394,7 +1329,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I27" s="1" t="s">
         <v>36</v>
       </c>
@@ -1402,7 +1337,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
@@ -1437,7 +1372,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I29" s="1" t="s">
         <v>36</v>
       </c>
@@ -1445,7 +1380,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>49</v>
       </c>
@@ -1480,7 +1415,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="I31" s="6" t="s">
         <v>36</v>
@@ -1489,7 +1424,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="I32" s="6" t="s">
         <v>52</v>
@@ -1498,7 +1433,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>53</v>
       </c>
@@ -1531,7 +1466,7 @@
       </c>
       <c r="P33" s="8"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="I34" s="7" t="s">
         <v>52</v>
@@ -1540,7 +1475,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>58</v>
       </c>
@@ -1566,7 +1501,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>62</v>
       </c>
@@ -1595,7 +1530,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>65</v>
       </c>
@@ -1618,7 +1553,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
         <v>68</v>
       </c>
@@ -1644,7 +1579,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>69</v>
       </c>
@@ -1676,7 +1611,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>71</v>
       </c>
@@ -1708,7 +1643,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>74</v>
       </c>
@@ -1743,7 +1678,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>76</v>
       </c>
@@ -1775,7 +1710,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>77</v>
       </c>
@@ -1810,7 +1745,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>78</v>
       </c>
@@ -1839,9 +1774,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="str">
-        <f aca="false">"migration/migration.sql"</f>
+        <f>"migration/migration.sql"</f>
         <v>migration/migration.sql</v>
       </c>
       <c r="C45" s="6" t="s">
@@ -1849,7 +1784,7 @@
       </c>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>81</v>
       </c>
@@ -1875,7 +1810,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B47" s="10"/>
       <c r="I47" s="6" t="s">
         <v>36</v>
@@ -1884,7 +1819,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I48" s="1" t="s">
         <v>52</v>
       </c>
@@ -1892,7 +1827,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>85</v>
       </c>
@@ -1918,7 +1853,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I50" s="1" t="s">
         <v>36</v>
       </c>
@@ -1926,7 +1861,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C51" s="11"/>
       <c r="I51" s="6" t="s">
         <v>52</v>
@@ -1935,7 +1870,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>89</v>
       </c>
@@ -1976,14 +1911,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="C53" s="11"/>
       <c r="J53" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
         <v>92</v>
       </c>
@@ -2024,7 +1959,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="C55" s="11"/>
       <c r="I55" s="6" t="s">
@@ -2034,7 +1969,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>95</v>
       </c>
@@ -2063,7 +1998,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="C57" s="11"/>
       <c r="I57" s="6" t="s">
@@ -2073,7 +2008,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
         <v>97</v>
       </c>
@@ -2090,7 +2025,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
         <v>99</v>
       </c>
@@ -2122,7 +2057,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B60" s="6" t="s">
         <v>101</v>
       </c>
@@ -2154,12 +2089,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>31</v>
@@ -2177,7 +2112,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
       <c r="I62" s="6" t="s">
         <v>36</v>
@@ -2186,7 +2121,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I63" s="1" t="s">
         <v>52</v>
       </c>
@@ -2194,9 +2129,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>31</v>
@@ -2218,28 +2153,28 @@
         <v>39</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L64" s="6" t="s">
         <v>42</v>
       </c>
       <c r="M64" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N64" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="C65" s="11"/>
       <c r="J65" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B66" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>63</v>
@@ -2266,9 +2201,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B67" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>59</v>
@@ -2293,12 +2228,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>31</v>
@@ -2316,7 +2251,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="I69" s="6" t="s">
         <v>36</v>
@@ -2325,7 +2260,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I70" s="1" t="s">
         <v>52</v>
       </c>
@@ -2333,9 +2268,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>111</v>
+        <v>148</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>31</v>
@@ -2357,28 +2292,28 @@
         <v>39</v>
       </c>
       <c r="K71" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="L71" s="6" t="s">
         <v>42</v>
       </c>
       <c r="M71" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="N71" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="C72" s="11"/>
       <c r="J72" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B73" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>63</v>
@@ -2405,9 +2340,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B74" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>59</v>
@@ -2432,55 +2367,36 @@
         <v>40</v>
       </c>
     </row>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="68.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.85"/>
+    <col min="1" max="1" width="68.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2488,178 +2404,173 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E15" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove count and lenght column
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\INTERPOLAR\Postgres-cds_hub\init\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
-    <sheet name="table_description_convert_def" sheetId="2" r:id="rId2"/>
+    <sheet name="rights_and_functions" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="table_description_convert_def" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,12 +21,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Unknown Author</author>
+    <author>Unbekannter Autor</author>
   </authors>
   <commentList>
-    <comment ref="D23" authorId="0" shapeId="0">
+    <comment ref="D23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,13 +45,13 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>GRANT TRIGGER
+          <t xml:space="preserve">GRANT TRIGGER
 GRANT USAGE ON SCHEMA
 GRANT USAGE ON seq</t>
         </r>
       </text>
     </comment>
-    <comment ref="H23" authorId="0" shapeId="0">
+    <comment ref="H23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,11 +70,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Rawdaten = varchar oder kein Eintrag dann Datentypen</t>
+          <t xml:space="preserve">Rawdaten = varchar oder kein Eintrag dann Datentypen</t>
         </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="0" shapeId="0">
+    <comment ref="I33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -97,11 +93,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Bei diesen Views funktioniert die Rechtevergabe im gegensatz zu den diff und view3 Views noch statisch</t>
+          <t xml:space="preserve">Bei diesen Views funktioniert die Rechtevergabe im gegensatz zu den diff und view3 Views noch statisch</t>
         </r>
       </text>
     </comment>
-    <comment ref="P33" authorId="0" shapeId="0">
+    <comment ref="K52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -120,11 +116,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>12.7. haben wir in der view geändert - cds2db nicht mehr notwendig</t>
+          <t xml:space="preserve">Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="K52" authorId="0" shapeId="0">
+    <comment ref="K54" authorId="0">
       <text>
         <r>
           <rPr>
@@ -143,11 +139,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Wie 30 und 31</t>
+          <t xml:space="preserve">Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="K54" authorId="0" shapeId="0">
+    <comment ref="K64" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,11 +162,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Wie 30 und 31</t>
+          <t xml:space="preserve">Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="K64" authorId="0" shapeId="0">
+    <comment ref="K71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -189,11 +185,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Wie 30 und 31</t>
+          <t xml:space="preserve">Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="K71" authorId="0" shapeId="0">
+    <comment ref="P33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -212,7 +208,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Wie 30 und 31</t>
+          <t xml:space="preserve">12.7. haben wir in der view geändert - cds2db nicht mehr notwendig</t>
         </r>
       </text>
     </comment>
@@ -221,460 +217,452 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="149">
-  <si>
-    <t>Erklärung</t>
-  </si>
-  <si>
-    <t>Spaltenname</t>
-  </si>
-  <si>
-    <t>Beschreibung</t>
-  </si>
-  <si>
-    <t>TABLE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>Pfad zur Excel-Datei gefolgt vom Namen des Tabellenblattes in eckigen Klammern mit den Tabellenbeschreibungen</t>
-  </si>
-  <si>
-    <t>SCRIPTNAME</t>
-  </si>
-  <si>
-    <t>Name des Templates, das ein Script mit diesem Namen erzeugt.</t>
-  </si>
-  <si>
-    <t>OWNER_USER</t>
-  </si>
-  <si>
-    <t>Name des Users, für den Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
-  </si>
-  <si>
-    <t>OWNER_SCHEMA</t>
-  </si>
-  <si>
-    <t>Name des Schemas, für das Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
-  </si>
-  <si>
-    <t>TABLE_PREFIX</t>
-  </si>
-  <si>
-    <t>TABLE_POSTFIX</t>
-  </si>
-  <si>
-    <t>SEQ_NAME</t>
-  </si>
-  <si>
-    <t>RIGHTS</t>
-  </si>
-  <si>
-    <t>GRANT_TARGET_USER</t>
-  </si>
-  <si>
-    <t>COPY_FUNC_SCRIPT_NAME</t>
-  </si>
-  <si>
-    <t>COPY_FUNC_NAME</t>
-  </si>
-  <si>
-    <t>SCHEMA_2</t>
-  </si>
-  <si>
-    <t>POSTFIX_2</t>
-  </si>
-  <si>
-    <t>SCHEMA_3</t>
-  </si>
-  <si>
-    <t>POSTFIX_3</t>
-  </si>
-  <si>
-    <t>Definition</t>
-  </si>
-  <si>
-    <t>TEMPLATE</t>
-  </si>
-  <si>
-    <t>TAGS</t>
-  </si>
-  <si>
-    <t>COPY_FUNC_SCRIPTNAME</t>
-  </si>
-  <si>
-    <t>COPY_FUNC_TEMPLATE</t>
-  </si>
-  <si>
-    <t>TABLE_POSTFIX_2</t>
-  </si>
-  <si>
-    <t>TABLE_POSTFIX_3</t>
-  </si>
-  <si>
-    <t>./R-cds2db/cds2db/inst/extdata/Table_Description.xlsx[table_description]</t>
-  </si>
-  <si>
-    <t>100_cre_table_raw_cds2db_in.sql</t>
-  </si>
-  <si>
-    <t>template_cre_table.sql</t>
-  </si>
-  <si>
-    <t>cds2db_user</t>
-  </si>
-  <si>
-    <t>cds2db_in</t>
-  </si>
-  <si>
-    <t>RAW</t>
-  </si>
-  <si>
-    <t>_raw</t>
-  </si>
-  <si>
-    <t>INSERT, DELETE, UPDATE, SELECT</t>
-  </si>
-  <si>
-    <t>db_user</t>
-  </si>
-  <si>
-    <t>120_cre_table_raw_db_log.sql</t>
-  </si>
-  <si>
-    <t>db_log_user</t>
-  </si>
-  <si>
-    <t>db_log</t>
-  </si>
-  <si>
-    <t>300_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t>template_copy_function.sql</t>
-  </si>
-  <si>
-    <t>copy_raw_cds_in_to_db_log</t>
-  </si>
-  <si>
-    <t>140_cre_table_typ_cds2db_in.sql</t>
-  </si>
-  <si>
-    <t>TYPED</t>
-  </si>
-  <si>
-    <t>150_get_last_processing_nr_typed.sql</t>
-  </si>
-  <si>
-    <t>template_get_last_pnr_typed.sql</t>
-  </si>
-  <si>
-    <t>get_last_processing_nr_typed</t>
-  </si>
-  <si>
-    <t>160_cre_table_typ_log.sql</t>
-  </si>
-  <si>
-    <t>310_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t>copy_type_cds_in_to_db_log</t>
-  </si>
-  <si>
-    <t>SELECT</t>
-  </si>
-  <si>
-    <t>180_cre_view_raw_type_diff_log.sql</t>
-  </si>
-  <si>
-    <t>template_cre_view_diff.sql</t>
-  </si>
-  <si>
-    <t>cds2db_out</t>
-  </si>
-  <si>
-    <t>v_</t>
-  </si>
-  <si>
-    <t>_raw_diff</t>
-  </si>
-  <si>
-    <t>190_cre_view_typ_dataproc_all.sql</t>
-  </si>
-  <si>
-    <t>template_cre_view_all.sql</t>
-  </si>
-  <si>
-    <t>db2dataprocessor_user</t>
-  </si>
-  <si>
-    <t>db2dataprocessor_out</t>
-  </si>
-  <si>
-    <t>190_cre_view_typ_dataproc_last_import.sql</t>
-  </si>
-  <si>
-    <t>template_cre_view_last_import.sql</t>
-  </si>
-  <si>
-    <t>_last_import</t>
-  </si>
-  <si>
-    <t>200_take_over_check_date.sql</t>
-  </si>
-  <si>
-    <t>template_take_over_check_date_function.sql</t>
-  </si>
-  <si>
-    <t>take_over_last_check_date</t>
-  </si>
-  <si>
-    <t>210_cre_view_typ_cds2db_all.sql</t>
-  </si>
-  <si>
-    <t>220_cre_view_raw_cds2db_last_import.sql</t>
-  </si>
-  <si>
-    <t>_raw_last_import</t>
-  </si>
-  <si>
-    <t>230_cre_view_typ_cds2db_last_version.sql</t>
-  </si>
-  <si>
-    <t>template_cre_view_last_version.sql</t>
-  </si>
-  <si>
-    <t>_last_version</t>
-  </si>
-  <si>
-    <t>230_cre_view_raw_cds2db_last_version.sql</t>
-  </si>
-  <si>
-    <t>_raw_last_version</t>
-  </si>
-  <si>
-    <t>230_cre_view_typ_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t>230_cre_view_raw_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t>250_adding_historical_raw_records.sql</t>
-  </si>
-  <si>
-    <t>template_adding_historical_records.sql</t>
-  </si>
-  <si>
-    <t>template_migration.sql</t>
-  </si>
-  <si>
-    <t>./R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx[frontend_table_description]</t>
-  </si>
-  <si>
-    <t>400_cre_table_typ_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t>db2dataprocessor_in</t>
-  </si>
-  <si>
-    <t>_fe</t>
-  </si>
-  <si>
-    <t>440_cre_table_frontend_in.sql</t>
-  </si>
-  <si>
-    <t>db2frontend_user</t>
-  </si>
-  <si>
-    <t>db2frontend_in</t>
-  </si>
-  <si>
-    <t>INT_ID</t>
-  </si>
-  <si>
-    <t>420_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t>600_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t>copy_fe_dp_in_to_db_log</t>
-  </si>
-  <si>
-    <t>430_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t>620_fe_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t>copy_fe_fe_in_to_db_log</t>
-  </si>
-  <si>
-    <t>520_cre_view_fe_out.sql</t>
-  </si>
-  <si>
-    <t>db2frontend_out</t>
-  </si>
-  <si>
-    <t>450_cre_table_frontend_in_trig.sql</t>
-  </si>
-  <si>
-    <t>template_cre_trigger_set_id.sql</t>
-  </si>
-  <si>
-    <t>460_cre_view_fe_dataproc_last_import.sql</t>
-  </si>
-  <si>
-    <t>_fe_last_import</t>
-  </si>
-  <si>
-    <t>470_cre_view_fe_dataproc_all.sql</t>
-  </si>
-  <si>
-    <t>./R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx[table_description]</t>
-  </si>
-  <si>
-    <t>332_db_submodules_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t>copy_submodules_dp_in_to_db_log</t>
-  </si>
-  <si>
-    <t>334_cre_view_dataproc_submodules_last_import.sql</t>
-  </si>
-  <si>
-    <t>335_cre_view_dataproc_submodules_all.sql</t>
-  </si>
-  <si>
-    <t>./R-dataprocessor/dataprocessor/inst/extdata/Dataprocessor_Table_Description.xlsx[table_description]</t>
-  </si>
-  <si>
-    <t>342_db_core_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t>copy_core_dp_in_to_db_log</t>
-  </si>
-  <si>
-    <t>344_cre_view_dataproc_core_last_import.sql</t>
-  </si>
-  <si>
-    <t>345_cre_view_dataproc_core_all.sql</t>
-  </si>
-  <si>
-    <t>TABLE_DEFINITION</t>
-  </si>
-  <si>
-    <t>Name der Definitionsdatei, die konvertiert werden soll (gilt immer für alle Zeilen der Tabelle bis zum Ende oder zu einem anderen Dateinamen)</t>
-  </si>
-  <si>
-    <t>SOURCE_COLUMN_NAME</t>
-  </si>
-  <si>
-    <t>Spaltenname in der unveränderten Definitionsdatei (gehört zusammen mit TARGET_COLUMN_NAME in derselben Zeile)</t>
-  </si>
-  <si>
-    <t>TARGET_COLUMN_NAME</t>
-  </si>
-  <si>
-    <t>Spaltenname in der geänderten Definitionsdatei (gehört zusammen mit SOURCE_COLUMN_NAME in derselben Zeile). Ist der Wert leer, bleibt der Name bestehen</t>
-  </si>
-  <si>
-    <t>SOURCE_TYPE</t>
-  </si>
-  <si>
-    <t>unveränderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem TARGET_TYPE in derselben Zeile)</t>
-  </si>
-  <si>
-    <t>TARGET_TYPE</t>
-  </si>
-  <si>
-    <t>geänderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem SOURCE_TYPE in derselben Zeile)</t>
-  </si>
-  <si>
-    <t>RESOURCE</t>
-  </si>
-  <si>
-    <t>TABLE_NAME</t>
-  </si>
-  <si>
-    <t>varchar</t>
-  </si>
-  <si>
-    <t>COLUMN_NAME</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>FHIR_EXPRESSION</t>
-  </si>
-  <si>
-    <t>COLUMN_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>timestamp</t>
-  </si>
-  <si>
-    <t>REFERENCE_TYPES</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>FHIR_TYPE</t>
-  </si>
-  <si>
-    <t>COLUMN_TYPE</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>SINGLE_LENGTH</t>
-  </si>
-  <si>
-    <t>VALUE_LENGTH</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>COUNT</t>
-  </si>
-  <si>
-    <t>VALUE_COUNT</t>
-  </si>
-  <si>
-    <t>decimal</t>
-  </si>
-  <si>
-    <t>double precision</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>330_cre_table_dataproc_submodules_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t>331_cre_table_dataproc_submodules_log.sql</t>
-  </si>
-  <si>
-    <t>340_cre_table_dataproc_core_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t>341_cre_table_dataproc_core_log.sql</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="145">
+  <si>
+    <t xml:space="preserve">Erklärung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spaltenname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beschreibung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pfad zur Excel-Datei gefolgt vom Namen des Tabellenblattes in eckigen Klammern mit den Tabellenbeschreibungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCRIPTNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name des Templates, das ein Script mit diesem Namen erzeugt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OWNER_USER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name des Users, für den Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OWNER_SCHEMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name des Schemas, für das Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_PREFIX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_POSTFIX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEQ_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIGHTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRANT_TARGET_USER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COPY_FUNC_SCRIPT_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COPY_FUNC_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHEMA_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSTFIX_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHEMA_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSTFIX_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMPLATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COPY_FUNC_SCRIPTNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COPY_FUNC_TEMPLATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_POSTFIX_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_POSTFIX_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./R-cds2db/cds2db/inst/extdata/Table_Description.xlsx[table_description]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100_cre_table_raw_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_cre_table.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cds2db_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cds2db_in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_raw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSERT, DELETE, UPDATE, SELECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120_cre_table_raw_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db_log_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_copy_function.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy_raw_cds_in_to_db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">140_cre_table_typ_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150_get_last_processing_nr_typed.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_get_last_pnr_typed.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get_last_processing_nr_typed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">160_cre_table_typ_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">310_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy_type_cds_in_to_db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">180_cre_view_raw_type_diff_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_cre_view_diff.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cds2db_out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_raw_diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">190_cre_view_typ_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_cre_view_all.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db2dataprocessor_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db2dataprocessor_out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">190_cre_view_typ_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_cre_view_last_import.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_last_import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200_take_over_check_date.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_take_over_check_date_function.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">take_over_last_check_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">210_cre_view_typ_cds2db_all.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220_cre_view_raw_cds2db_last_import.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_raw_last_import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230_cre_view_typ_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_cre_view_last_version.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_last_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230_cre_view_raw_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_raw_last_version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230_cre_view_typ_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">230_cre_view_raw_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250_adding_historical_raw_records.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_adding_historical_records.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_migration.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx[frontend_table_description]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400_cre_table_typ_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db2dataprocessor_in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_fe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">440_cre_table_frontend_in.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db2frontend_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db2frontend_in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">420_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">600_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy_fe_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">430_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">620_fe_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy_fe_fe_in_to_db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">520_cre_view_fe_out.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db2frontend_out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">450_cre_table_frontend_in_trig.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_cre_trigger_set_id.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">460_cre_view_fe_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_fe_last_import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470_cre_view_fe_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx[table_description]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">330_cre_table_dataproc_submodules_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">331_cre_table_dataproc_submodules_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">332_db_submodules_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy_submodules_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">334_cre_view_dataproc_submodules_last_import.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">335_cre_view_dataproc_submodules_all.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">./R-dataprocessor/dataprocessor/inst/extdata/Dataprocessor_Table_Description.xlsx[table_description]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">340_cre_table_dataproc_core_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">341_cre_table_dataproc_core_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">342_db_core_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy_core_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">344_cre_view_dataproc_core_last_import.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">345_cre_view_dataproc_core_all.sql</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_DEFINITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name der Definitionsdatei, die konvertiert werden soll (gilt immer für alle Zeilen der Tabelle bis zum Ende oder zu einem anderen Dateinamen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOURCE_COLUMN_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spaltenname in der unveränderten Definitionsdatei (gehört zusammen mit TARGET_COLUMN_NAME in derselben Zeile)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TARGET_COLUMN_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spaltenname in der geänderten Definitionsdatei (gehört zusammen mit SOURCE_COLUMN_NAME in derselben Zeile). Ist der Wert leer, bleibt der Name bestehen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOURCE_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unveränderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem TARGET_TYPE in derselben Zeile)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TARGET_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geänderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem SOURCE_TYPE in derselben Zeile)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESOURCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLUMN_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FHIR_EXPRESSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLUMN_DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timestamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REFERENCE_TYPES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FHIR_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLUMN_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">double precision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,7 +671,22 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
@@ -744,19 +747,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="9" tint="-0.25"/>
         <bgColor rgb="FF7F7F7F"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39979247413556324"/>
+        <fgColor theme="9" tint="0.3997"/>
         <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -764,36 +767,101 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="23">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Excel Built-in Bad" xfId="2"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="1"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="3"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="9">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
+    <cellStyle name="Excel Built-in Bad" xfId="21"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="22"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -852,76 +920,60 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="44546a"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="e7e6e6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="5b9bd5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="ed7d31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="a5a5a5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="ffc000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4472c4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="70ad47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0563c1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="954f72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -953,7 +1005,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -977,7 +1029,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1037,50 +1089,51 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B72" activeCellId="0" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="95.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="73" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="20.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="40.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="28.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="27" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" style="1" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="95.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="24.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="28.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="16.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.72"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1088,11 +1141,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1100,7 +1153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1108,7 +1161,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1116,7 +1169,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1124,81 +1177,81 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="4"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
@@ -1251,7 +1304,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1280,7 +1333,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I25" s="1" t="s">
         <v>36</v>
       </c>
@@ -1288,7 +1341,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
         <v>38</v>
       </c>
@@ -1329,7 +1382,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I27" s="1" t="s">
         <v>36</v>
       </c>
@@ -1337,7 +1390,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
@@ -1372,7 +1425,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I29" s="1" t="s">
         <v>36</v>
       </c>
@@ -1380,7 +1433,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="6" t="s">
         <v>49</v>
       </c>
@@ -1415,7 +1468,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="6"/>
       <c r="I31" s="6" t="s">
         <v>36</v>
@@ -1424,7 +1477,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="6"/>
       <c r="I32" s="6" t="s">
         <v>52</v>
@@ -1433,7 +1486,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="6" t="s">
         <v>53</v>
       </c>
@@ -1466,7 +1519,7 @@
       </c>
       <c r="P33" s="8"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="6"/>
       <c r="I34" s="7" t="s">
         <v>52</v>
@@ -1475,7 +1528,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="6" t="s">
         <v>58</v>
       </c>
@@ -1501,7 +1554,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="6" t="s">
         <v>62</v>
       </c>
@@ -1530,7 +1583,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="6" t="s">
         <v>65</v>
       </c>
@@ -1553,7 +1606,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="6" t="s">
         <v>68</v>
       </c>
@@ -1579,7 +1632,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="6" t="s">
         <v>69</v>
       </c>
@@ -1611,7 +1664,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="6" t="s">
         <v>71</v>
       </c>
@@ -1643,7 +1696,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="6" t="s">
         <v>74</v>
       </c>
@@ -1678,7 +1731,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="6" t="s">
         <v>76</v>
       </c>
@@ -1710,7 +1763,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="6" t="s">
         <v>77</v>
       </c>
@@ -1745,7 +1798,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="6" t="s">
         <v>78</v>
       </c>
@@ -1774,9 +1827,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="6" t="str">
-        <f>"migration/migration.sql"</f>
+        <f aca="false">"migration/migration.sql"</f>
         <v>migration/migration.sql</v>
       </c>
       <c r="C45" s="6" t="s">
@@ -1784,7 +1837,7 @@
       </c>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>81</v>
       </c>
@@ -1810,7 +1863,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="10"/>
       <c r="I47" s="6" t="s">
         <v>36</v>
@@ -1819,7 +1872,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="1" t="s">
         <v>52</v>
       </c>
@@ -1827,7 +1880,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="1" t="s">
         <v>85</v>
       </c>
@@ -1853,7 +1906,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I50" s="1" t="s">
         <v>36</v>
       </c>
@@ -1861,7 +1914,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="11"/>
       <c r="I51" s="6" t="s">
         <v>52</v>
@@ -1870,7 +1923,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="1" t="s">
         <v>89</v>
       </c>
@@ -1911,14 +1964,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="6"/>
       <c r="C53" s="11"/>
       <c r="J53" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="6" t="s">
         <v>92</v>
       </c>
@@ -1959,7 +2012,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="6"/>
       <c r="C55" s="11"/>
       <c r="I55" s="6" t="s">
@@ -1969,7 +2022,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="6" t="s">
         <v>95</v>
       </c>
@@ -1998,7 +2051,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="6"/>
       <c r="C57" s="11"/>
       <c r="I57" s="6" t="s">
@@ -2008,7 +2061,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="6" t="s">
         <v>97</v>
       </c>
@@ -2025,7 +2078,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="6" t="s">
         <v>99</v>
       </c>
@@ -2057,7 +2110,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="6" t="s">
         <v>101</v>
       </c>
@@ -2089,12 +2142,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>31</v>
@@ -2112,7 +2165,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="6"/>
       <c r="I62" s="6" t="s">
         <v>36</v>
@@ -2121,7 +2174,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I63" s="1" t="s">
         <v>52</v>
       </c>
@@ -2129,9 +2182,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="1" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>31</v>
@@ -2153,28 +2206,28 @@
         <v>39</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="L64" s="6" t="s">
         <v>42</v>
       </c>
       <c r="M64" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="N64" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="6"/>
       <c r="C65" s="11"/>
       <c r="J65" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>63</v>
@@ -2201,9 +2254,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>59</v>
@@ -2228,12 +2281,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>31</v>
@@ -2251,7 +2304,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="6"/>
       <c r="I69" s="6" t="s">
         <v>36</v>
@@ -2260,7 +2313,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I70" s="1" t="s">
         <v>52</v>
       </c>
@@ -2268,9 +2321,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="1" t="s">
-        <v>148</v>
+        <v>111</v>
       </c>
       <c r="C71" s="11" t="s">
         <v>31</v>
@@ -2292,28 +2345,28 @@
         <v>39</v>
       </c>
       <c r="K71" s="6" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="L71" s="6" t="s">
         <v>42</v>
       </c>
       <c r="M71" s="6" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="N71" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="6"/>
       <c r="C72" s="11"/>
       <c r="J72" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="6" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>63</v>
@@ -2340,9 +2393,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="6" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>59</v>
@@ -2368,35 +2421,43 @@
       </c>
     </row>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="68.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="68.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.86"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2404,156 +2465,144 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>137</v>
-      </c>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C17" s="1" t="s">
         <v>141</v>
       </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="1" t="s">
         <v>142</v>
       </c>
@@ -2561,7 +2610,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="1" t="s">
         <v>144</v>
       </c>
@@ -2570,7 +2619,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DB - Extend the table definition (templates) of the frontend tables with necessary indexes for the views of the last version. refs #1041
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\INTERPOLAR\Postgres-cds_hub\init\template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="rights_and_functions" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="table_description_convert_def" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
+    <sheet name="table_description_convert_def" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Unbekannter Autor</author>
   </authors>
   <commentList>
-    <comment ref="D23" authorId="0">
+    <comment ref="D23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -45,13 +49,13 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">GRANT TRIGGER
+          <t>GRANT TRIGGER
 GRANT USAGE ON SCHEMA
 GRANT USAGE ON seq</t>
         </r>
       </text>
     </comment>
-    <comment ref="H23" authorId="0">
+    <comment ref="H23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,11 +74,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Rawdaten = varchar oder kein Eintrag dann Datentypen</t>
+          <t>Rawdaten = varchar oder kein Eintrag dann Datentypen</t>
         </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="0">
+    <comment ref="I33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,11 +97,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Bei diesen Views funktioniert die Rechtevergabe im gegensatz zu den diff und view3 Views noch statisch</t>
+          <t>Bei diesen Views funktioniert die Rechtevergabe im gegensatz zu den diff und view3 Views noch statisch</t>
         </r>
       </text>
     </comment>
-    <comment ref="K52" authorId="0">
+    <comment ref="P33" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -116,11 +120,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Wie 30 und 31</t>
+          <t>12.7. haben wir in der view geändert - cds2db nicht mehr notwendig</t>
         </r>
       </text>
     </comment>
-    <comment ref="K54" authorId="0">
+    <comment ref="K52" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -139,11 +143,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Wie 30 und 31</t>
+          <t>Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="K64" authorId="0">
+    <comment ref="K54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -162,11 +166,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Wie 30 und 31</t>
+          <t>Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="K71" authorId="0">
+    <comment ref="K64" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -185,11 +189,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Wie 30 und 31</t>
+          <t>Wie 30 und 31</t>
         </r>
       </text>
     </comment>
-    <comment ref="P33" authorId="0">
+    <comment ref="K71" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -208,7 +212,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">12.7. haben wir in der view geändert - cds2db nicht mehr notwendig</t>
+          <t>Wie 30 und 31</t>
         </r>
       </text>
     </comment>
@@ -217,452 +221,451 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="145">
-  <si>
-    <t xml:space="preserve">Erklärung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spaltenname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beschreibung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pfad zur Excel-Datei gefolgt vom Namen des Tabellenblattes in eckigen Klammern mit den Tabellenbeschreibungen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCRIPTNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name des Templates, das ein Script mit diesem Namen erzeugt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OWNER_USER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name des Users, für den Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OWNER_SCHEMA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name des Schemas, für das Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_PREFIX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_POSTFIX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEQ_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIGHTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRANT_TARGET_USER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COPY_FUNC_SCRIPT_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COPY_FUNC_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCHEMA_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POSTFIX_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCHEMA_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POSTFIX_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Definition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEMPLATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COPY_FUNC_SCRIPTNAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COPY_FUNC_TEMPLATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_POSTFIX_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_POSTFIX_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./R-cds2db/cds2db/inst/extdata/Table_Description.xlsx[table_description]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100_cre_table_raw_cds2db_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_table.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cds2db_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cds2db_in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_raw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSERT, DELETE, UPDATE, SELECT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120_cre_table_raw_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db_log_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_copy_function.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_raw_cds_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">140_cre_table_typ_cds2db_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TYPED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150_get_last_processing_nr_typed.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_get_last_pnr_typed.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">get_last_processing_nr_typed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">160_cre_table_typ_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">310_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_type_cds_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">180_cre_view_raw_type_diff_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_view_diff.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cds2db_out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_raw_diff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">190_cre_view_typ_dataproc_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_view_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2dataprocessor_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2dataprocessor_out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">190_cre_view_typ_dataproc_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_view_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_last_import</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200_take_over_check_date.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_take_over_check_date_function.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">take_over_last_check_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">210_cre_view_typ_cds2db_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">220_cre_view_raw_cds2db_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_raw_last_import</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230_cre_view_typ_cds2db_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_view_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_last_version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230_cre_view_raw_cds2db_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_raw_last_version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230_cre_view_typ_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">230_cre_view_raw_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">250_adding_historical_raw_records.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_adding_historical_records.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_migration.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx[frontend_table_description]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400_cre_table_typ_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2dataprocessor_in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_fe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">440_cre_table_frontend_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2frontend_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2frontend_in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INT_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">420_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">600_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_fe_dp_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">430_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">620_fe_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_fe_fe_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">520_cre_view_fe_out.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">db2frontend_out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450_cre_table_frontend_in_trig.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">template_cre_trigger_set_id.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">460_cre_view_fe_dataproc_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_fe_last_import</t>
-  </si>
-  <si>
-    <t xml:space="preserve">470_cre_view_fe_dataproc_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx[table_description]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">330_cre_table_dataproc_submodules_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">331_cre_table_dataproc_submodules_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">332_db_submodules_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_submodules_dp_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">334_cre_view_dataproc_submodules_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">335_cre_view_dataproc_submodules_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">./R-dataprocessor/dataprocessor/inst/extdata/Dataprocessor_Table_Description.xlsx[table_description]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">340_cre_table_dataproc_core_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">341_cre_table_dataproc_core_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">342_db_core_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">copy_core_dp_in_to_db_log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">344_cre_view_dataproc_core_last_import.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">345_cre_view_dataproc_core_all.sql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_DEFINITION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name der Definitionsdatei, die konvertiert werden soll (gilt immer für alle Zeilen der Tabelle bis zum Ende oder zu einem anderen Dateinamen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOURCE_COLUMN_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spaltenname in der unveränderten Definitionsdatei (gehört zusammen mit TARGET_COLUMN_NAME in derselben Zeile)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TARGET_COLUMN_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spaltenname in der geänderten Definitionsdatei (gehört zusammen mit SOURCE_COLUMN_NAME in derselben Zeile). Ist der Wert leer, bleibt der Name bestehen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOURCE_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unveränderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem TARGET_TYPE in derselben Zeile)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TARGET_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geänderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem SOURCE_TYPE in derselben Zeile)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESOURCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TABLE_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">varchar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLUMN_NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FHIR_EXPRESSION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLUMN_DESCRIPTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REFERENCE_TYPES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FHIR_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COLUMN_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">decimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">double precision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boolean</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="146">
+  <si>
+    <t>Erklärung</t>
+  </si>
+  <si>
+    <t>Spaltenname</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>TABLE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Pfad zur Excel-Datei gefolgt vom Namen des Tabellenblattes in eckigen Klammern mit den Tabellenbeschreibungen</t>
+  </si>
+  <si>
+    <t>SCRIPTNAME</t>
+  </si>
+  <si>
+    <t>Name des Templates, das ein Script mit diesem Namen erzeugt.</t>
+  </si>
+  <si>
+    <t>OWNER_USER</t>
+  </si>
+  <si>
+    <t>Name des Users, für den Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
+  </si>
+  <si>
+    <t>OWNER_SCHEMA</t>
+  </si>
+  <si>
+    <t>Name des Schemas, für das Tabellen und Rechte angelegt werden (nur wenn relevant, insbesondere bei Scripten mit Create Table Statements)</t>
+  </si>
+  <si>
+    <t>TABLE_PREFIX</t>
+  </si>
+  <si>
+    <t>TABLE_POSTFIX</t>
+  </si>
+  <si>
+    <t>SEQ_NAME</t>
+  </si>
+  <si>
+    <t>RIGHTS</t>
+  </si>
+  <si>
+    <t>GRANT_TARGET_USER</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_SCRIPT_NAME</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_NAME</t>
+  </si>
+  <si>
+    <t>SCHEMA_2</t>
+  </si>
+  <si>
+    <t>POSTFIX_2</t>
+  </si>
+  <si>
+    <t>SCHEMA_3</t>
+  </si>
+  <si>
+    <t>POSTFIX_3</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>TEMPLATE</t>
+  </si>
+  <si>
+    <t>TAGS</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_SCRIPTNAME</t>
+  </si>
+  <si>
+    <t>COPY_FUNC_TEMPLATE</t>
+  </si>
+  <si>
+    <t>TABLE_POSTFIX_2</t>
+  </si>
+  <si>
+    <t>TABLE_POSTFIX_3</t>
+  </si>
+  <si>
+    <t>./R-cds2db/cds2db/inst/extdata/Table_Description.xlsx[table_description]</t>
+  </si>
+  <si>
+    <t>100_cre_table_raw_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t>template_cre_table.sql</t>
+  </si>
+  <si>
+    <t>cds2db_user</t>
+  </si>
+  <si>
+    <t>cds2db_in</t>
+  </si>
+  <si>
+    <t>RAW</t>
+  </si>
+  <si>
+    <t>_raw</t>
+  </si>
+  <si>
+    <t>INSERT, DELETE, UPDATE, SELECT</t>
+  </si>
+  <si>
+    <t>db_user</t>
+  </si>
+  <si>
+    <t>120_cre_table_raw_db_log.sql</t>
+  </si>
+  <si>
+    <t>db_log_user</t>
+  </si>
+  <si>
+    <t>db_log</t>
+  </si>
+  <si>
+    <t>300_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>template_copy_function.sql</t>
+  </si>
+  <si>
+    <t>copy_raw_cds_in_to_db_log</t>
+  </si>
+  <si>
+    <t>140_cre_table_typ_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t>TYPED</t>
+  </si>
+  <si>
+    <t>150_get_last_processing_nr_typed.sql</t>
+  </si>
+  <si>
+    <t>template_get_last_pnr_typed.sql</t>
+  </si>
+  <si>
+    <t>get_last_processing_nr_typed</t>
+  </si>
+  <si>
+    <t>160_cre_table_typ_log.sql</t>
+  </si>
+  <si>
+    <t>310_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_type_cds_in_to_db_log</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>180_cre_view_raw_type_diff_log.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_diff.sql</t>
+  </si>
+  <si>
+    <t>cds2db_out</t>
+  </si>
+  <si>
+    <t>v_</t>
+  </si>
+  <si>
+    <t>_raw_diff</t>
+  </si>
+  <si>
+    <t>190_cre_view_typ_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_all.sql</t>
+  </si>
+  <si>
+    <t>db2dataprocessor_user</t>
+  </si>
+  <si>
+    <t>db2dataprocessor_out</t>
+  </si>
+  <si>
+    <t>190_cre_view_typ_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_last_import.sql</t>
+  </si>
+  <si>
+    <t>_last_import</t>
+  </si>
+  <si>
+    <t>200_take_over_check_date.sql</t>
+  </si>
+  <si>
+    <t>template_take_over_check_date_function.sql</t>
+  </si>
+  <si>
+    <t>take_over_last_check_date</t>
+  </si>
+  <si>
+    <t>210_cre_view_typ_cds2db_all.sql</t>
+  </si>
+  <si>
+    <t>220_cre_view_raw_cds2db_last_import.sql</t>
+  </si>
+  <si>
+    <t>_raw_last_import</t>
+  </si>
+  <si>
+    <t>230_cre_view_typ_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t>template_cre_view_last_version.sql</t>
+  </si>
+  <si>
+    <t>_last_version</t>
+  </si>
+  <si>
+    <t>230_cre_view_raw_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t>_raw_last_version</t>
+  </si>
+  <si>
+    <t>230_cre_view_typ_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t>230_cre_view_raw_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t>250_adding_historical_raw_records.sql</t>
+  </si>
+  <si>
+    <t>template_adding_historical_records.sql</t>
+  </si>
+  <si>
+    <t>template_migration.sql</t>
+  </si>
+  <si>
+    <t>./R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx[frontend_table_description]</t>
+  </si>
+  <si>
+    <t>400_cre_table_typ_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t>db2dataprocessor_in</t>
+  </si>
+  <si>
+    <t>_fe</t>
+  </si>
+  <si>
+    <t>440_cre_table_frontend_in.sql</t>
+  </si>
+  <si>
+    <t>db2frontend_user</t>
+  </si>
+  <si>
+    <t>db2frontend_in</t>
+  </si>
+  <si>
+    <t>INT_ID</t>
+  </si>
+  <si>
+    <t>420_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t>600_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_fe_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t>430_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t>620_fe_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_fe_fe_in_to_db_log</t>
+  </si>
+  <si>
+    <t>520_cre_view_fe_out.sql</t>
+  </si>
+  <si>
+    <t>db2frontend_out</t>
+  </si>
+  <si>
+    <t>450_cre_table_frontend_in_trig.sql</t>
+  </si>
+  <si>
+    <t>template_cre_trigger_set_id.sql</t>
+  </si>
+  <si>
+    <t>460_cre_view_fe_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t>_fe_last_import</t>
+  </si>
+  <si>
+    <t>470_cre_view_fe_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t>./R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx[table_description]</t>
+  </si>
+  <si>
+    <t>330_cre_table_dataproc_submodules_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t>331_cre_table_dataproc_submodules_log.sql</t>
+  </si>
+  <si>
+    <t>332_db_submodules_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_submodules_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t>334_cre_view_dataproc_submodules_last_import.sql</t>
+  </si>
+  <si>
+    <t>335_cre_view_dataproc_submodules_all.sql</t>
+  </si>
+  <si>
+    <t>./R-dataprocessor/dataprocessor/inst/extdata/Dataprocessor_Table_Description.xlsx[table_description]</t>
+  </si>
+  <si>
+    <t>340_cre_table_dataproc_core_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t>341_cre_table_dataproc_core_log.sql</t>
+  </si>
+  <si>
+    <t>342_db_core_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>copy_core_dp_in_to_db_log</t>
+  </si>
+  <si>
+    <t>344_cre_view_dataproc_core_last_import.sql</t>
+  </si>
+  <si>
+    <t>345_cre_view_dataproc_core_all.sql</t>
+  </si>
+  <si>
+    <t>TABLE_DEFINITION</t>
+  </si>
+  <si>
+    <t>Name der Definitionsdatei, die konvertiert werden soll (gilt immer für alle Zeilen der Tabelle bis zum Ende oder zu einem anderen Dateinamen)</t>
+  </si>
+  <si>
+    <t>SOURCE_COLUMN_NAME</t>
+  </si>
+  <si>
+    <t>Spaltenname in der unveränderten Definitionsdatei (gehört zusammen mit TARGET_COLUMN_NAME in derselben Zeile)</t>
+  </si>
+  <si>
+    <t>TARGET_COLUMN_NAME</t>
+  </si>
+  <si>
+    <t>Spaltenname in der geänderten Definitionsdatei (gehört zusammen mit SOURCE_COLUMN_NAME in derselben Zeile). Ist der Wert leer, bleibt der Name bestehen</t>
+  </si>
+  <si>
+    <t>SOURCE_TYPE</t>
+  </si>
+  <si>
+    <t>unveränderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem TARGET_TYPE in derselben Zeile)</t>
+  </si>
+  <si>
+    <t>TARGET_TYPE</t>
+  </si>
+  <si>
+    <t>geänderter Typ aus der 'type' Spalte in der Definitionsdatei (gehört zusammen mit dem SOURCE_TYPE in derselben Zeile)</t>
+  </si>
+  <si>
+    <t>RESOURCE</t>
+  </si>
+  <si>
+    <t>TABLE_NAME</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>COLUMN_NAME</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>FHIR_EXPRESSION</t>
+  </si>
+  <si>
+    <t>COLUMN_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>REFERENCE_TYPES</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>FHIR_TYPE</t>
+  </si>
+  <si>
+    <t>COLUMN_TYPE</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>double precision</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>INT_ID FE_RC_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,20 +676,10 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <i val="true"/>
+      <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
@@ -712,11 +705,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -747,19 +735,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.25"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor rgb="FF7F7F7F"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.3997"/>
+        <fgColor theme="9" tint="0.39967040009765925"/>
         <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -767,101 +755,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
-    <cellStyle name="Excel Built-in Bad" xfId="21"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="22"/>
+  <cellStyles count="4">
+    <cellStyle name="Excel Built-in Bad" xfId="2"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="1"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="3"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -920,60 +843,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -1005,7 +944,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -1029,7 +968,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1089,51 +1028,50 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B72" activeCellId="0" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="95.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="24.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="40.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="28.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="16.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.72"/>
+    <col min="1" max="1" width="95.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="73" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="20.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="40.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="27" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1141,11 +1079,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1153,7 +1091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1161,7 +1099,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1169,7 +1107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1177,81 +1115,81 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
@@ -1304,7 +1242,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1333,7 +1271,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I25" s="1" t="s">
         <v>36</v>
       </c>
@@ -1341,7 +1279,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>38</v>
       </c>
@@ -1382,7 +1320,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I27" s="1" t="s">
         <v>36</v>
       </c>
@@ -1390,7 +1328,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>44</v>
       </c>
@@ -1425,7 +1363,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I29" s="1" t="s">
         <v>36</v>
       </c>
@@ -1433,7 +1371,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>49</v>
       </c>
@@ -1468,7 +1406,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
       <c r="I31" s="6" t="s">
         <v>36</v>
@@ -1477,7 +1415,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="I32" s="6" t="s">
         <v>52</v>
@@ -1486,7 +1424,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>53</v>
       </c>
@@ -1519,7 +1457,7 @@
       </c>
       <c r="P33" s="8"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="I34" s="7" t="s">
         <v>52</v>
@@ -1528,7 +1466,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>58</v>
       </c>
@@ -1554,7 +1492,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>62</v>
       </c>
@@ -1583,7 +1521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>65</v>
       </c>
@@ -1606,7 +1544,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
         <v>68</v>
       </c>
@@ -1632,7 +1570,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>69</v>
       </c>
@@ -1664,7 +1602,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>71</v>
       </c>
@@ -1696,7 +1634,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>74</v>
       </c>
@@ -1731,7 +1669,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>76</v>
       </c>
@@ -1763,7 +1701,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>77</v>
       </c>
@@ -1798,7 +1736,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>78</v>
       </c>
@@ -1827,9 +1765,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="str">
-        <f aca="false">"migration/migration.sql"</f>
+        <f>"migration/migration.sql"</f>
         <v>migration/migration.sql</v>
       </c>
       <c r="C45" s="6" t="s">
@@ -1837,7 +1775,7 @@
       </c>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>81</v>
       </c>
@@ -1863,7 +1801,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B47" s="10"/>
       <c r="I47" s="6" t="s">
         <v>36</v>
@@ -1872,7 +1810,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I48" s="1" t="s">
         <v>52</v>
       </c>
@@ -1880,7 +1818,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>85</v>
       </c>
@@ -1906,7 +1844,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I50" s="1" t="s">
         <v>36</v>
       </c>
@@ -1914,7 +1852,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C51" s="11"/>
       <c r="I51" s="6" t="s">
         <v>52</v>
@@ -1923,7 +1861,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>89</v>
       </c>
@@ -1937,7 +1875,7 @@
         <v>40</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>88</v>
+        <v>145</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>84</v>
@@ -1964,14 +1902,14 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
       <c r="C53" s="11"/>
       <c r="J53" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
         <v>92</v>
       </c>
@@ -1985,7 +1923,7 @@
         <v>40</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>88</v>
+        <v>145</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>84</v>
@@ -2012,7 +1950,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
       <c r="C55" s="11"/>
       <c r="I55" s="6" t="s">
@@ -2022,7 +1960,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>95</v>
       </c>
@@ -2051,7 +1989,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="C57" s="11"/>
       <c r="I57" s="6" t="s">
@@ -2061,7 +1999,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
         <v>97</v>
       </c>
@@ -2078,7 +2016,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
         <v>99</v>
       </c>
@@ -2110,7 +2048,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B60" s="6" t="s">
         <v>101</v>
       </c>
@@ -2142,7 +2080,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>102</v>
       </c>
@@ -2165,7 +2103,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
       <c r="I62" s="6" t="s">
         <v>36</v>
@@ -2174,7 +2112,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I63" s="1" t="s">
         <v>52</v>
       </c>
@@ -2182,7 +2120,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>104</v>
       </c>
@@ -2218,14 +2156,14 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="C65" s="11"/>
       <c r="J65" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B66" s="6" t="s">
         <v>107</v>
       </c>
@@ -2254,7 +2192,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B67" s="6" t="s">
         <v>108</v>
       </c>
@@ -2281,7 +2219,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>109</v>
       </c>
@@ -2304,7 +2242,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B69" s="6"/>
       <c r="I69" s="6" t="s">
         <v>36</v>
@@ -2313,7 +2251,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I70" s="1" t="s">
         <v>52</v>
       </c>
@@ -2321,7 +2259,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
         <v>111</v>
       </c>
@@ -2357,14 +2295,14 @@
         <v>83</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="C72" s="11"/>
       <c r="J72" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B73" s="6" t="s">
         <v>114</v>
       </c>
@@ -2393,7 +2331,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B74" s="6" t="s">
         <v>115</v>
       </c>
@@ -2421,43 +2359,35 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="68.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.86"/>
+    <col min="1" max="1" width="68.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2465,7 +2395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>116</v>
       </c>
@@ -2473,7 +2403,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>118</v>
       </c>
@@ -2481,7 +2411,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>120</v>
       </c>
@@ -2489,7 +2419,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>122</v>
       </c>
@@ -2497,7 +2427,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>124</v>
       </c>
@@ -2505,12 +2435,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
@@ -2527,7 +2457,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2541,7 +2471,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>129</v>
       </c>
@@ -2555,7 +2485,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>131</v>
       </c>
@@ -2569,7 +2499,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>135</v>
       </c>
@@ -2580,7 +2510,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>137</v>
       </c>
@@ -2594,7 +2524,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>140</v>
       </c>
@@ -2602,7 +2532,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
         <v>142</v>
       </c>
@@ -2610,7 +2540,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
         <v>144</v>
       </c>
@@ -2619,12 +2549,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DB - View in each output schema to view the database parameters - template which can be configured for each schema - view naming is fixed. refs#1131
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="0" shapeId="0">
+    <comment ref="I36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P33" authorId="0" shapeId="0">
+    <comment ref="P36" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K52" authorId="0" shapeId="0">
+    <comment ref="K55" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K54" authorId="0" shapeId="0">
+    <comment ref="K57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -170,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K64" authorId="0" shapeId="0">
+    <comment ref="K67" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K71" authorId="0" shapeId="0">
+    <comment ref="K74" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="151">
   <si>
     <t>Erklärung</t>
   </si>
@@ -659,6 +659,21 @@
   </si>
   <si>
     <t>INT_ID FE_RC_ID</t>
+  </si>
+  <si>
+    <t>template_cre_view_parameter.sql</t>
+  </si>
+  <si>
+    <t>031_cre_view_parameter_cds2db_out.sql</t>
+  </si>
+  <si>
+    <t>032_cre_view_parameter_dataproc_out.sql</t>
+  </si>
+  <si>
+    <t>033_cre_view_parameter_dataproc_out.sql</t>
+  </si>
+  <si>
+    <t>fix</t>
   </si>
 </sst>
 </file>
@@ -1040,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1194,9 @@
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
@@ -1247,315 +1264,312 @@
         <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J24" s="1" t="s">
+      <c r="E24" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>37</v>
+      <c r="B25" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>38</v>
+        <v>149</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="D27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I27" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="I28" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N28" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="I29" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="I33" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J30" s="6" t="s">
+      <c r="J33" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K30" s="6" t="s">
+      <c r="K33" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="L30" s="6" t="s">
+      <c r="L33" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M30" s="6" t="s">
+      <c r="M33" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="N30" s="6" t="s">
+      <c r="N33" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="I31" s="6" t="s">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="6"/>
+      <c r="I34" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J31" s="6" t="s">
+      <c r="J34" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="I32" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O33" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P33" s="8"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="6"/>
-      <c r="I34" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>56</v>
-      </c>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B35" s="6"/>
       <c r="I35" s="6" t="s">
         <v>52</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N35" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>56</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I36" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="J36" s="6" t="s">
-        <v>60</v>
+      <c r="J36" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="N36" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H37" s="6" t="s">
+      <c r="O36" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K37" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="M37" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="N37" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P36" s="8"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="6"/>
+      <c r="I37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>56</v>
@@ -1563,83 +1577,71 @@
       <c r="I38" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J38" s="7" t="s">
-        <v>32</v>
+      <c r="J38" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="N38" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>63</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>56</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J39" s="7" t="s">
-        <v>32</v>
+      <c r="J39" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="N39" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O39" s="6" t="s">
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H40" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I40" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J40" s="7" t="s">
-        <v>32</v>
+      <c r="K40" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M40" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="N40" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>32</v>
@@ -1647,15 +1649,9 @@
       <c r="E41" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="G41" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H41" s="6" t="s">
-        <v>75</v>
-      </c>
       <c r="I41" s="6" t="s">
         <v>52</v>
       </c>
@@ -1665,83 +1661,77 @@
       <c r="N41" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O41" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>56</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I42" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J42" s="6" t="s">
-        <v>60</v>
+      <c r="J42" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="N42" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O42" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>56</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I43" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J43" s="6" t="s">
-        <v>60</v>
+      <c r="J43" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="N43" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O43" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>32</v>
@@ -1749,90 +1739,149 @@
       <c r="E44" s="6" t="s">
         <v>55</v>
       </c>
+      <c r="F44" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="G44" s="6" t="s">
         <v>56</v>
       </c>
       <c r="H44" s="6" t="s">
         <v>75</v>
       </c>
+      <c r="I44" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="J44" s="7" t="s">
         <v>32</v>
       </c>
       <c r="N44" s="6" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="O44" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="6" t="str">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N45" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N46" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O46" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N47" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="str">
         <f>"migration/migration.sql"</f>
         <v>migration/migration.sql</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C48" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="J45" s="7"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="J48" s="7"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="10"/>
-      <c r="I47" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I48" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>84</v>
@@ -1841,205 +1890,189 @@
         <v>36</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I50" s="1" t="s">
+      <c r="B50" s="10"/>
+      <c r="I50" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="J50" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C51" s="11"/>
-      <c r="I51" s="6" t="s">
+      <c r="I51" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J51" s="6" t="s">
+      <c r="J51" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D52" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H52" s="6" t="s">
+      <c r="D52" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I52" s="6" t="s">
+      <c r="I52" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J52" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K52" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L52" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="M52" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="N52" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="O52" s="6" t="s">
-        <v>84</v>
+      <c r="J52" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="6"/>
-      <c r="C53" s="11"/>
-      <c r="J53" s="6" t="s">
+      <c r="I53" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J53" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>84</v>
-      </c>
+      <c r="C54" s="11"/>
       <c r="I54" s="6" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="J54" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K54" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="L54" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="M54" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="N54" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="O54" s="6" t="s">
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H55" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="6"/>
-      <c r="C55" s="11"/>
       <c r="I55" s="6" t="s">
         <v>36</v>
       </c>
       <c r="J55" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L55" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M55" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="N55" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B56" s="6"/>
+      <c r="C56" s="11"/>
+      <c r="J56" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I56" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J56" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="N56" s="6" t="s">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B57" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E57" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O56" s="6" t="s">
+      <c r="F57" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H57" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="6"/>
-      <c r="C57" s="11"/>
       <c r="I57" s="6" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="J57" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="L57" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M57" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="N57" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="O57" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B58" s="6"/>
+      <c r="C58" s="11"/>
+      <c r="I58" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J58" s="6" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>63</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="G59" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H59" s="6" t="s">
-        <v>100</v>
-      </c>
       <c r="I59" s="6" t="s">
         <v>52</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="N59" s="6" t="s">
         <v>40</v>
@@ -2049,312 +2082,371 @@
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>84</v>
-      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="11"/>
       <c r="I60" s="6" t="s">
         <v>52</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N60" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B61" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H61" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B62" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H62" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J62" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N62" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O60" s="6" t="s">
+      <c r="O62" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B63" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J63" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N63" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O63" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B64" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C64" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D61" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E61" s="6" t="s">
+      <c r="D64" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E64" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I61" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J61" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="6"/>
-      <c r="I62" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J62" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I63" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C64" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H64" s="6"/>
       <c r="I64" s="6" t="s">
         <v>36</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K64" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="L64" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="M64" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="N64" s="6" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
-      <c r="C65" s="11"/>
+      <c r="I65" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="J65" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B66" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H66" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I66" s="6" t="s">
+      <c r="I66" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J66" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N66" s="6" t="s">
+      <c r="J66" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E67" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B67" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G67" s="6" t="s">
-        <v>56</v>
+      <c r="F67" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="H67" s="6"/>
       <c r="I67" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L67" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M67" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="N67" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B68" s="6"/>
+      <c r="C68" s="11"/>
+      <c r="J68" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B69" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I69" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J67" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N67" s="6" t="s">
+      <c r="J69" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N69" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B70" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J70" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N70" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B71" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C71" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D68" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E68" s="6" t="s">
+      <c r="D71" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E71" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I68" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J68" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B69" s="6"/>
-      <c r="I69" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J69" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I70" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B71" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C71" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H71" s="6"/>
       <c r="I71" s="6" t="s">
         <v>36</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K71" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="L71" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="M71" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="N71" s="6" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
-      <c r="C72" s="11"/>
+      <c r="I72" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="J72" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B73" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G73" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H73" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I73" s="6" t="s">
+      <c r="I73" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J73" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N73" s="6" t="s">
+      <c r="J73" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E74" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B74" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G74" s="6" t="s">
-        <v>56</v>
+      <c r="F74" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="H74" s="6"/>
       <c r="I74" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K74" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="L74" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M74" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="N74" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B75" s="6"/>
+      <c r="C75" s="11"/>
+      <c r="J75" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B76" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I76" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="J74" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N74" s="6" t="s">
+      <c r="J76" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N76" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B77" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J77" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N77" s="6" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DB - Generated SQL view scripts and integration into migration script refs #1131
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/init/template/User_Schema_Rights_Definition.xlsx
@@ -670,10 +670,10 @@
     <t>032_cre_view_parameter_dataproc_out.sql</t>
   </si>
   <si>
-    <t>033_cre_view_parameter_dataproc_out.sql</t>
-  </si>
-  <si>
     <t>fix</t>
+  </si>
+  <si>
+    <t>033_cre_view_parameter_frontend_out.sql</t>
   </si>
 </sst>
 </file>
@@ -1057,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6" t="s">
@@ -1302,7 +1302,7 @@
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6" t="s">
@@ -1314,7 +1314,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>146</v>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="6" t="s">

</xml_diff>